<commit_message>
Añadi funcion para generar reportes mensuales
</commit_message>
<xml_diff>
--- a/assets/plantillaIngresos.xlsx
+++ b/assets/plantillaIngresos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\OneDrive\Escritorio\python\programaEscuela\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659C7C16-666A-4F66-A3E6-4570B3F47C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCE6CA-A097-40B8-B57B-1F86C2CA85FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,6 +518,163 @@
     <xf numFmtId="44" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -583,163 +740,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2170,8 +2170,8 @@
   </sheetPr>
   <dimension ref="A1:CF43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="69" zoomScaleNormal="69" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40:AZ40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="69" zoomScaleNormal="69" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2905,45 +2905,45 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
-      <c r="AG1" s="105"/>
-      <c r="AH1" s="105"/>
-      <c r="AI1" s="105"/>
-      <c r="AJ1" s="105"/>
-      <c r="AK1" s="105"/>
-      <c r="AL1" s="105"/>
-      <c r="AM1" s="105"/>
-      <c r="AN1" s="105"/>
-      <c r="AO1" s="106" t="s">
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="61"/>
+      <c r="AO1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="AP1" s="107"/>
-      <c r="AQ1" s="107"/>
-      <c r="AR1" s="107"/>
-      <c r="AS1" s="107"/>
-      <c r="AT1" s="107"/>
-      <c r="AU1" s="107"/>
-      <c r="AV1" s="107"/>
-      <c r="AW1" s="107"/>
-      <c r="AX1" s="107"/>
-      <c r="AY1" s="108"/>
-      <c r="AZ1" s="108"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="63"/>
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="63"/>
+      <c r="AX1" s="63"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
     </row>
     <row r="2" spans="1:61" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -3000,60 +3000,60 @@
       <c r="AZ2" s="56"/>
     </row>
     <row r="3" spans="1:61" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="109"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="109"/>
-      <c r="AB3" s="109"/>
-      <c r="AC3" s="109"/>
-      <c r="AD3" s="109"/>
-      <c r="AE3" s="109"/>
-      <c r="AF3" s="109"/>
-      <c r="AG3" s="109"/>
-      <c r="AH3" s="109"/>
-      <c r="AI3" s="109"/>
-      <c r="AJ3" s="109"/>
-      <c r="AK3" s="109"/>
-      <c r="AL3" s="109"/>
-      <c r="AM3" s="109"/>
-      <c r="AN3" s="109"/>
-      <c r="AO3" s="109"/>
-      <c r="AP3" s="109"/>
-      <c r="AQ3" s="109"/>
-      <c r="AR3" s="109"/>
-      <c r="AS3" s="109"/>
-      <c r="AT3" s="109"/>
-      <c r="AU3" s="109"/>
-      <c r="AV3" s="109"/>
-      <c r="AW3" s="109"/>
-      <c r="AX3" s="109"/>
-      <c r="AY3" s="109"/>
-      <c r="AZ3" s="109"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="65"/>
+      <c r="AL3" s="65"/>
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65"/>
+      <c r="AX3" s="65"/>
+      <c r="AY3" s="65"/>
+      <c r="AZ3" s="65"/>
     </row>
     <row r="4" spans="1:61" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -3097,16 +3097,16 @@
       <c r="AM4" s="6"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="7"/>
-      <c r="AP4" s="106"/>
-      <c r="AQ4" s="107"/>
-      <c r="AR4" s="107"/>
-      <c r="AS4" s="107"/>
-      <c r="AT4" s="107"/>
-      <c r="AU4" s="107"/>
-      <c r="AV4" s="107"/>
-      <c r="AW4" s="107"/>
-      <c r="AX4" s="107"/>
-      <c r="AY4" s="107"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="63"/>
+      <c r="AR4" s="63"/>
+      <c r="AS4" s="63"/>
+      <c r="AT4" s="63"/>
+      <c r="AU4" s="63"/>
+      <c r="AV4" s="63"/>
+      <c r="AW4" s="63"/>
+      <c r="AX4" s="63"/>
+      <c r="AY4" s="63"/>
       <c r="AZ4" s="8"/>
     </row>
     <row r="5" spans="1:61" s="13" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3129,43 +3129,43 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="110"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="110"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="66"/>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="110"/>
-      <c r="AD5" s="110"/>
-      <c r="AE5" s="110"/>
-      <c r="AF5" s="110"/>
-      <c r="AG5" s="110"/>
-      <c r="AH5" s="110"/>
-      <c r="AI5" s="110"/>
-      <c r="AJ5" s="110"/>
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="66"/>
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="66"/>
+      <c r="AH5" s="66"/>
+      <c r="AI5" s="66"/>
+      <c r="AJ5" s="66"/>
       <c r="AK5" s="12"/>
-      <c r="AL5" s="111" t="s">
+      <c r="AL5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="AM5" s="111"/>
-      <c r="AN5" s="111"/>
-      <c r="AO5" s="111"/>
-      <c r="AP5" s="111"/>
-      <c r="AQ5" s="111"/>
-      <c r="AR5" s="111"/>
+      <c r="AM5" s="67"/>
+      <c r="AN5" s="67"/>
+      <c r="AO5" s="67"/>
+      <c r="AP5" s="67"/>
+      <c r="AQ5" s="67"/>
+      <c r="AR5" s="67"/>
       <c r="AS5" s="12"/>
-      <c r="AT5" s="111" t="s">
+      <c r="AT5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="AU5" s="111"/>
-      <c r="AV5" s="111"/>
-      <c r="AW5" s="111"/>
-      <c r="AX5" s="111"/>
-      <c r="AY5" s="111"/>
-      <c r="AZ5" s="111"/>
+      <c r="AU5" s="67"/>
+      <c r="AV5" s="67"/>
+      <c r="AW5" s="67"/>
+      <c r="AX5" s="67"/>
+      <c r="AY5" s="67"/>
+      <c r="AZ5" s="67"/>
     </row>
     <row r="6" spans="1:61" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -3187,39 +3187,39 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="112"/>
-      <c r="U6" s="112"/>
-      <c r="V6" s="112"/>
-      <c r="W6" s="112"/>
-      <c r="X6" s="112"/>
-      <c r="Y6" s="112"/>
-      <c r="Z6" s="112"/>
-      <c r="AA6" s="112"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="68"/>
+      <c r="Z6" s="68"/>
+      <c r="AA6" s="68"/>
       <c r="AB6" s="14"/>
-      <c r="AC6" s="112"/>
-      <c r="AD6" s="112"/>
-      <c r="AE6" s="112"/>
-      <c r="AF6" s="112"/>
-      <c r="AG6" s="112"/>
-      <c r="AH6" s="112"/>
-      <c r="AI6" s="112"/>
-      <c r="AJ6" s="112"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="68"/>
+      <c r="AF6" s="68"/>
+      <c r="AG6" s="68"/>
+      <c r="AH6" s="68"/>
+      <c r="AI6" s="68"/>
+      <c r="AJ6" s="68"/>
       <c r="AK6" s="14"/>
-      <c r="AL6" s="103"/>
-      <c r="AM6" s="113"/>
-      <c r="AN6" s="115"/>
-      <c r="AO6" s="113"/>
-      <c r="AP6" s="116"/>
-      <c r="AQ6" s="103"/>
-      <c r="AR6" s="113"/>
+      <c r="AL6" s="59"/>
+      <c r="AM6" s="69"/>
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="69"/>
+      <c r="AP6" s="72"/>
+      <c r="AQ6" s="59"/>
+      <c r="AR6" s="69"/>
       <c r="AS6" s="12"/>
-      <c r="AT6" s="103"/>
-      <c r="AU6" s="103"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="AX6" s="103"/>
-      <c r="AY6" s="103"/>
-      <c r="AZ6" s="103"/>
+      <c r="AT6" s="59"/>
+      <c r="AU6" s="59"/>
+      <c r="AV6" s="59"/>
+      <c r="AW6" s="59"/>
+      <c r="AX6" s="59"/>
+      <c r="AY6" s="59"/>
+      <c r="AZ6" s="59"/>
     </row>
     <row r="7" spans="1:61" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3241,39 +3241,39 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="112"/>
-      <c r="X7" s="112"/>
-      <c r="Y7" s="112"/>
-      <c r="Z7" s="112"/>
-      <c r="AA7" s="112"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="68"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="112"/>
-      <c r="AD7" s="112"/>
-      <c r="AE7" s="112"/>
-      <c r="AF7" s="112"/>
-      <c r="AG7" s="112"/>
-      <c r="AH7" s="112"/>
-      <c r="AI7" s="112"/>
-      <c r="AJ7" s="112"/>
+      <c r="AC7" s="68"/>
+      <c r="AD7" s="68"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="68"/>
+      <c r="AG7" s="68"/>
+      <c r="AH7" s="68"/>
+      <c r="AI7" s="68"/>
+      <c r="AJ7" s="68"/>
       <c r="AK7" s="14"/>
-      <c r="AL7" s="114"/>
-      <c r="AM7" s="114"/>
-      <c r="AN7" s="117"/>
-      <c r="AO7" s="114"/>
-      <c r="AP7" s="118"/>
-      <c r="AQ7" s="114"/>
-      <c r="AR7" s="114"/>
+      <c r="AL7" s="70"/>
+      <c r="AM7" s="70"/>
+      <c r="AN7" s="73"/>
+      <c r="AO7" s="70"/>
+      <c r="AP7" s="74"/>
+      <c r="AQ7" s="70"/>
+      <c r="AR7" s="70"/>
       <c r="AS7" s="12"/>
-      <c r="AT7" s="104"/>
-      <c r="AU7" s="104"/>
-      <c r="AV7" s="104"/>
-      <c r="AW7" s="104"/>
-      <c r="AX7" s="104"/>
-      <c r="AY7" s="104"/>
-      <c r="AZ7" s="104"/>
+      <c r="AT7" s="60"/>
+      <c r="AU7" s="60"/>
+      <c r="AV7" s="60"/>
+      <c r="AW7" s="60"/>
+      <c r="AX7" s="60"/>
+      <c r="AY7" s="60"/>
+      <c r="AZ7" s="60"/>
     </row>
     <row r="8" spans="1:61" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -3334,116 +3334,116 @@
       <c r="AZ8" s="52"/>
     </row>
     <row r="9" spans="1:61" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="86"/>
-      <c r="Z9" s="86"/>
-      <c r="AA9" s="86"/>
-      <c r="AB9" s="86"/>
-      <c r="AC9" s="86"/>
-      <c r="AD9" s="86"/>
-      <c r="AE9" s="86"/>
-      <c r="AF9" s="86"/>
-      <c r="AG9" s="86"/>
-      <c r="AH9" s="86"/>
-      <c r="AI9" s="86"/>
-      <c r="AJ9" s="86"/>
-      <c r="AK9" s="86"/>
-      <c r="AL9" s="86"/>
-      <c r="AM9" s="86"/>
-      <c r="AN9" s="86"/>
-      <c r="AO9" s="86"/>
-      <c r="AP9" s="86"/>
-      <c r="AQ9" s="86"/>
-      <c r="AR9" s="87"/>
-      <c r="AS9" s="86" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
+      <c r="T9" s="78"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="78"/>
+      <c r="W9" s="78"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="78"/>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78"/>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78"/>
+      <c r="AD9" s="78"/>
+      <c r="AE9" s="78"/>
+      <c r="AF9" s="78"/>
+      <c r="AG9" s="78"/>
+      <c r="AH9" s="78"/>
+      <c r="AI9" s="78"/>
+      <c r="AJ9" s="78"/>
+      <c r="AK9" s="78"/>
+      <c r="AL9" s="78"/>
+      <c r="AM9" s="78"/>
+      <c r="AN9" s="78"/>
+      <c r="AO9" s="78"/>
+      <c r="AP9" s="78"/>
+      <c r="AQ9" s="78"/>
+      <c r="AR9" s="79"/>
+      <c r="AS9" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AT9" s="86"/>
-      <c r="AU9" s="86"/>
-      <c r="AV9" s="86"/>
-      <c r="AW9" s="86"/>
-      <c r="AX9" s="86"/>
-      <c r="AY9" s="86"/>
-      <c r="AZ9" s="86"/>
+      <c r="AT9" s="78"/>
+      <c r="AU9" s="78"/>
+      <c r="AV9" s="78"/>
+      <c r="AW9" s="78"/>
+      <c r="AX9" s="78"/>
+      <c r="AY9" s="78"/>
+      <c r="AZ9" s="78"/>
     </row>
     <row r="10" spans="1:61" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="88"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="89"/>
-      <c r="S10" s="89"/>
-      <c r="T10" s="89"/>
-      <c r="U10" s="89"/>
-      <c r="V10" s="89"/>
-      <c r="W10" s="89"/>
-      <c r="X10" s="89"/>
-      <c r="Y10" s="89"/>
-      <c r="Z10" s="89"/>
-      <c r="AA10" s="89"/>
-      <c r="AB10" s="89"/>
-      <c r="AC10" s="89"/>
-      <c r="AD10" s="89"/>
-      <c r="AE10" s="89"/>
-      <c r="AF10" s="89"/>
-      <c r="AG10" s="89"/>
-      <c r="AH10" s="89"/>
-      <c r="AI10" s="89"/>
-      <c r="AJ10" s="89"/>
-      <c r="AK10" s="89"/>
-      <c r="AL10" s="89"/>
-      <c r="AM10" s="89"/>
-      <c r="AN10" s="89"/>
-      <c r="AO10" s="89"/>
-      <c r="AP10" s="89"/>
-      <c r="AQ10" s="89"/>
-      <c r="AR10" s="90"/>
-      <c r="AS10" s="91"/>
-      <c r="AT10" s="92"/>
-      <c r="AU10" s="92"/>
-      <c r="AV10" s="92"/>
-      <c r="AW10" s="92"/>
-      <c r="AX10" s="92"/>
-      <c r="AY10" s="92"/>
-      <c r="AZ10" s="92"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="81"/>
+      <c r="AD10" s="81"/>
+      <c r="AE10" s="81"/>
+      <c r="AF10" s="81"/>
+      <c r="AG10" s="81"/>
+      <c r="AH10" s="81"/>
+      <c r="AI10" s="81"/>
+      <c r="AJ10" s="81"/>
+      <c r="AK10" s="81"/>
+      <c r="AL10" s="81"/>
+      <c r="AM10" s="81"/>
+      <c r="AN10" s="81"/>
+      <c r="AO10" s="81"/>
+      <c r="AP10" s="81"/>
+      <c r="AQ10" s="81"/>
+      <c r="AR10" s="82"/>
+      <c r="AS10" s="83"/>
+      <c r="AT10" s="84"/>
+      <c r="AU10" s="84"/>
+      <c r="AV10" s="84"/>
+      <c r="AW10" s="84"/>
+      <c r="AX10" s="84"/>
+      <c r="AY10" s="84"/>
+      <c r="AZ10" s="84"/>
     </row>
     <row r="11" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -3500,118 +3500,118 @@
       <c r="AZ11" s="52"/>
     </row>
     <row r="12" spans="1:61" s="20" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="97" t="s">
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="98"/>
-      <c r="P12" s="98"/>
-      <c r="Q12" s="98"/>
-      <c r="R12" s="98"/>
-      <c r="S12" s="98"/>
-      <c r="T12" s="98"/>
-      <c r="U12" s="98"/>
-      <c r="V12" s="98"/>
-      <c r="W12" s="98"/>
-      <c r="X12" s="98"/>
-      <c r="Y12" s="98"/>
-      <c r="Z12" s="98"/>
-      <c r="AA12" s="98"/>
-      <c r="AB12" s="98"/>
-      <c r="AC12" s="98"/>
-      <c r="AD12" s="98"/>
-      <c r="AE12" s="98"/>
-      <c r="AF12" s="98"/>
-      <c r="AG12" s="98"/>
-      <c r="AH12" s="98"/>
-      <c r="AI12" s="98"/>
-      <c r="AJ12" s="98"/>
-      <c r="AK12" s="99"/>
-      <c r="AL12" s="99"/>
-      <c r="AM12" s="99"/>
-      <c r="AN12" s="99"/>
-      <c r="AO12" s="99"/>
-      <c r="AP12" s="99"/>
-      <c r="AQ12" s="99"/>
-      <c r="AR12" s="99"/>
-      <c r="AS12" s="97" t="s">
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
+      <c r="T12" s="90"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="90"/>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="90"/>
+      <c r="AA12" s="90"/>
+      <c r="AB12" s="90"/>
+      <c r="AC12" s="90"/>
+      <c r="AD12" s="90"/>
+      <c r="AE12" s="90"/>
+      <c r="AF12" s="90"/>
+      <c r="AG12" s="90"/>
+      <c r="AH12" s="90"/>
+      <c r="AI12" s="90"/>
+      <c r="AJ12" s="90"/>
+      <c r="AK12" s="91"/>
+      <c r="AL12" s="91"/>
+      <c r="AM12" s="91"/>
+      <c r="AN12" s="91"/>
+      <c r="AO12" s="91"/>
+      <c r="AP12" s="91"/>
+      <c r="AQ12" s="91"/>
+      <c r="AR12" s="91"/>
+      <c r="AS12" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="AT12" s="99"/>
-      <c r="AU12" s="99"/>
-      <c r="AV12" s="99"/>
-      <c r="AW12" s="99"/>
-      <c r="AX12" s="99"/>
-      <c r="AY12" s="99"/>
-      <c r="AZ12" s="99"/>
+      <c r="AT12" s="91"/>
+      <c r="AU12" s="91"/>
+      <c r="AV12" s="91"/>
+      <c r="AW12" s="91"/>
+      <c r="AX12" s="91"/>
+      <c r="AY12" s="91"/>
+      <c r="AZ12" s="91"/>
     </row>
     <row r="13" spans="1:61" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
-      <c r="Z13" s="86"/>
-      <c r="AA13" s="86"/>
-      <c r="AB13" s="86"/>
-      <c r="AC13" s="86"/>
-      <c r="AD13" s="86"/>
-      <c r="AE13" s="86"/>
-      <c r="AF13" s="86"/>
-      <c r="AG13" s="86"/>
-      <c r="AH13" s="86"/>
-      <c r="AI13" s="86"/>
-      <c r="AJ13" s="86"/>
-      <c r="AK13" s="101"/>
-      <c r="AL13" s="101"/>
-      <c r="AM13" s="101"/>
-      <c r="AN13" s="101"/>
-      <c r="AO13" s="101"/>
-      <c r="AP13" s="101"/>
-      <c r="AQ13" s="101"/>
-      <c r="AR13" s="101"/>
-      <c r="AS13" s="102"/>
-      <c r="AT13" s="101"/>
-      <c r="AU13" s="101"/>
-      <c r="AV13" s="101"/>
-      <c r="AW13" s="101"/>
-      <c r="AX13" s="101"/>
-      <c r="AY13" s="101"/>
-      <c r="AZ13" s="101"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="78"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="78"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="78"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="78"/>
+      <c r="AE13" s="78"/>
+      <c r="AF13" s="78"/>
+      <c r="AG13" s="78"/>
+      <c r="AH13" s="78"/>
+      <c r="AI13" s="78"/>
+      <c r="AJ13" s="78"/>
+      <c r="AK13" s="93"/>
+      <c r="AL13" s="93"/>
+      <c r="AM13" s="93"/>
+      <c r="AN13" s="93"/>
+      <c r="AO13" s="93"/>
+      <c r="AP13" s="93"/>
+      <c r="AQ13" s="93"/>
+      <c r="AR13" s="93"/>
+      <c r="AS13" s="94"/>
+      <c r="AT13" s="93"/>
+      <c r="AU13" s="93"/>
+      <c r="AV13" s="93"/>
+      <c r="AW13" s="93"/>
+      <c r="AX13" s="93"/>
+      <c r="AY13" s="93"/>
+      <c r="AZ13" s="93"/>
     </row>
     <row r="14" spans="1:61" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
@@ -3670,19 +3670,16 @@
     </row>
     <row r="15" spans="1:61" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
       <c r="E15" s="25"/>
       <c r="F15" s="26"/>
       <c r="G15" s="27" t="str">
         <f>IF(ISBLANK(B15),"",VLOOKUP(B15,'[1]CLAVES INGRESOS'!$A$1:$B$65536,2,0))</f>
         <v/>
       </c>
-      <c r="H15" s="27">
-        <f ca="1">H15:H30</f>
-        <v>0</v>
-      </c>
+      <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
@@ -3720,12 +3717,12 @@
       <c r="AQ15" s="30"/>
       <c r="AR15" s="31"/>
       <c r="AS15" s="32"/>
-      <c r="AT15" s="78"/>
-      <c r="AU15" s="79"/>
-      <c r="AV15" s="79"/>
-      <c r="AW15" s="79"/>
-      <c r="AX15" s="79"/>
-      <c r="AY15" s="79"/>
+      <c r="AT15" s="76"/>
+      <c r="AU15" s="77"/>
+      <c r="AV15" s="77"/>
+      <c r="AW15" s="77"/>
+      <c r="AX15" s="77"/>
+      <c r="AY15" s="77"/>
       <c r="AZ15" s="33"/>
       <c r="BA15" s="34" t="str">
         <f>IF(ISBLANK(B15),"",VLOOKUP(B15,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3756,9 +3753,9 @@
     </row>
     <row r="16" spans="1:61" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
       <c r="G16" s="27" t="str">
@@ -3803,12 +3800,12 @@
       <c r="AQ16" s="27"/>
       <c r="AR16" s="58"/>
       <c r="AS16" s="39"/>
-      <c r="AT16" s="78"/>
-      <c r="AU16" s="79"/>
-      <c r="AV16" s="79"/>
-      <c r="AW16" s="79"/>
-      <c r="AX16" s="79"/>
-      <c r="AY16" s="79"/>
+      <c r="AT16" s="76"/>
+      <c r="AU16" s="77"/>
+      <c r="AV16" s="77"/>
+      <c r="AW16" s="77"/>
+      <c r="AX16" s="77"/>
+      <c r="AY16" s="77"/>
       <c r="AZ16" s="33"/>
       <c r="BA16" s="34" t="str">
         <f>IF(ISBLANK(B16),"",VLOOKUP(B16,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3839,9 +3836,9 @@
     </row>
     <row r="17" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
       <c r="G17" s="27" t="str">
@@ -3886,12 +3883,12 @@
       <c r="AQ17" s="27"/>
       <c r="AR17" s="58"/>
       <c r="AS17" s="32"/>
-      <c r="AT17" s="78"/>
-      <c r="AU17" s="79"/>
-      <c r="AV17" s="79"/>
-      <c r="AW17" s="79"/>
-      <c r="AX17" s="79"/>
-      <c r="AY17" s="79"/>
+      <c r="AT17" s="76"/>
+      <c r="AU17" s="77"/>
+      <c r="AV17" s="77"/>
+      <c r="AW17" s="77"/>
+      <c r="AX17" s="77"/>
+      <c r="AY17" s="77"/>
       <c r="AZ17" s="33"/>
       <c r="BA17" s="34" t="str">
         <f>IF(ISBLANK(B17),"",VLOOKUP(B17,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3922,9 +3919,9 @@
     </row>
     <row r="18" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
       <c r="G18" s="27" t="str">
@@ -3969,12 +3966,12 @@
       <c r="AQ18" s="27"/>
       <c r="AR18" s="58"/>
       <c r="AS18" s="39"/>
-      <c r="AT18" s="78"/>
-      <c r="AU18" s="79"/>
-      <c r="AV18" s="79"/>
-      <c r="AW18" s="79"/>
-      <c r="AX18" s="79"/>
-      <c r="AY18" s="79"/>
+      <c r="AT18" s="76"/>
+      <c r="AU18" s="77"/>
+      <c r="AV18" s="77"/>
+      <c r="AW18" s="77"/>
+      <c r="AX18" s="77"/>
+      <c r="AY18" s="77"/>
       <c r="AZ18" s="33"/>
       <c r="BA18" s="34" t="str">
         <f>IF(ISBLANK(B18),"",VLOOKUP(B18,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4008,9 +4005,9 @@
     </row>
     <row r="19" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
       <c r="G19" s="27" t="str">
@@ -4055,12 +4052,12 @@
       <c r="AQ19" s="27"/>
       <c r="AR19" s="58"/>
       <c r="AS19" s="32"/>
-      <c r="AT19" s="78"/>
-      <c r="AU19" s="79"/>
-      <c r="AV19" s="79"/>
-      <c r="AW19" s="79"/>
-      <c r="AX19" s="79"/>
-      <c r="AY19" s="79"/>
+      <c r="AT19" s="76"/>
+      <c r="AU19" s="77"/>
+      <c r="AV19" s="77"/>
+      <c r="AW19" s="77"/>
+      <c r="AX19" s="77"/>
+      <c r="AY19" s="77"/>
       <c r="AZ19" s="33"/>
       <c r="BA19" s="34" t="str">
         <f>IF(ISBLANK(B19),"",VLOOKUP(B19,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4091,9 +4088,9 @@
     </row>
     <row r="20" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
       <c r="G20" s="27" t="str">
@@ -4138,12 +4135,12 @@
       <c r="AQ20" s="27"/>
       <c r="AR20" s="58"/>
       <c r="AS20" s="39"/>
-      <c r="AT20" s="78"/>
-      <c r="AU20" s="79"/>
-      <c r="AV20" s="79"/>
-      <c r="AW20" s="79"/>
-      <c r="AX20" s="79"/>
-      <c r="AY20" s="79"/>
+      <c r="AT20" s="76"/>
+      <c r="AU20" s="77"/>
+      <c r="AV20" s="77"/>
+      <c r="AW20" s="77"/>
+      <c r="AX20" s="77"/>
+      <c r="AY20" s="77"/>
       <c r="AZ20" s="33"/>
       <c r="BA20" s="34" t="str">
         <f>IF(ISBLANK(B20),"",VLOOKUP(B20,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4165,9 +4162,9 @@
     </row>
     <row r="21" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
       <c r="G21" s="27" t="str">
@@ -4212,12 +4209,12 @@
       <c r="AQ21" s="27"/>
       <c r="AR21" s="58"/>
       <c r="AS21" s="32"/>
-      <c r="AT21" s="78"/>
-      <c r="AU21" s="79"/>
-      <c r="AV21" s="79"/>
-      <c r="AW21" s="79"/>
-      <c r="AX21" s="79"/>
-      <c r="AY21" s="79"/>
+      <c r="AT21" s="76"/>
+      <c r="AU21" s="77"/>
+      <c r="AV21" s="77"/>
+      <c r="AW21" s="77"/>
+      <c r="AX21" s="77"/>
+      <c r="AY21" s="77"/>
       <c r="AZ21" s="33"/>
       <c r="BA21" s="34" t="str">
         <f>IF(ISBLANK(B21),"",VLOOKUP(B21,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4236,9 +4233,9 @@
     </row>
     <row r="22" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="25"/>
       <c r="F22" s="26"/>
       <c r="G22" s="27" t="str">
@@ -4285,12 +4282,12 @@
       <c r="AQ22" s="27"/>
       <c r="AR22" s="58"/>
       <c r="AS22" s="39"/>
-      <c r="AT22" s="78"/>
-      <c r="AU22" s="79"/>
-      <c r="AV22" s="79"/>
-      <c r="AW22" s="79"/>
-      <c r="AX22" s="79"/>
-      <c r="AY22" s="79"/>
+      <c r="AT22" s="76"/>
+      <c r="AU22" s="77"/>
+      <c r="AV22" s="77"/>
+      <c r="AW22" s="77"/>
+      <c r="AX22" s="77"/>
+      <c r="AY22" s="77"/>
       <c r="AZ22" s="33"/>
       <c r="BA22" s="34" t="str">
         <f>IF(ISBLANK(B22),"",VLOOKUP(B22,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4307,9 +4304,9 @@
     </row>
     <row r="23" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="27" t="str">
@@ -4356,12 +4353,12 @@
       <c r="AQ23" s="27"/>
       <c r="AR23" s="40"/>
       <c r="AS23" s="32"/>
-      <c r="AT23" s="78"/>
-      <c r="AU23" s="79"/>
-      <c r="AV23" s="79"/>
-      <c r="AW23" s="79"/>
-      <c r="AX23" s="79"/>
-      <c r="AY23" s="79"/>
+      <c r="AT23" s="76"/>
+      <c r="AU23" s="77"/>
+      <c r="AV23" s="77"/>
+      <c r="AW23" s="77"/>
+      <c r="AX23" s="77"/>
+      <c r="AY23" s="77"/>
       <c r="AZ23" s="33"/>
       <c r="BA23" s="34" t="str">
         <f>IF(ISBLANK(B23),"",VLOOKUP(B23,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4379,9 +4376,9 @@
     </row>
     <row r="24" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
       <c r="G24" s="27" t="str">
@@ -4428,12 +4425,12 @@
       <c r="AQ24" s="30"/>
       <c r="AR24" s="40"/>
       <c r="AS24" s="39"/>
-      <c r="AT24" s="78"/>
-      <c r="AU24" s="79"/>
-      <c r="AV24" s="79"/>
-      <c r="AW24" s="79"/>
-      <c r="AX24" s="79"/>
-      <c r="AY24" s="79"/>
+      <c r="AT24" s="76"/>
+      <c r="AU24" s="77"/>
+      <c r="AV24" s="77"/>
+      <c r="AW24" s="77"/>
+      <c r="AX24" s="77"/>
+      <c r="AY24" s="77"/>
       <c r="AZ24" s="33"/>
       <c r="BA24" s="34" t="str">
         <f>IF(ISBLANK(B24),"",VLOOKUP(B24,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4450,9 +4447,9 @@
     </row>
     <row r="25" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
       <c r="G25" s="27" t="str">
@@ -4499,12 +4496,12 @@
       <c r="AQ25" s="30"/>
       <c r="AR25" s="40"/>
       <c r="AS25" s="39"/>
-      <c r="AT25" s="78"/>
-      <c r="AU25" s="79"/>
-      <c r="AV25" s="79"/>
-      <c r="AW25" s="79"/>
-      <c r="AX25" s="79"/>
-      <c r="AY25" s="79"/>
+      <c r="AT25" s="76"/>
+      <c r="AU25" s="77"/>
+      <c r="AV25" s="77"/>
+      <c r="AW25" s="77"/>
+      <c r="AX25" s="77"/>
+      <c r="AY25" s="77"/>
       <c r="AZ25" s="33"/>
       <c r="BA25" s="34" t="str">
         <f>IF(ISBLANK(B25),"",VLOOKUP(B25,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4521,9 +4518,9 @@
     </row>
     <row r="26" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
       <c r="G26" s="27" t="str">
@@ -4570,12 +4567,12 @@
       <c r="AQ26" s="30"/>
       <c r="AR26" s="40"/>
       <c r="AS26" s="39"/>
-      <c r="AT26" s="78"/>
-      <c r="AU26" s="79"/>
-      <c r="AV26" s="79"/>
-      <c r="AW26" s="79"/>
-      <c r="AX26" s="79"/>
-      <c r="AY26" s="79"/>
+      <c r="AT26" s="76"/>
+      <c r="AU26" s="77"/>
+      <c r="AV26" s="77"/>
+      <c r="AW26" s="77"/>
+      <c r="AX26" s="77"/>
+      <c r="AY26" s="77"/>
       <c r="AZ26" s="33"/>
       <c r="BA26" s="34" t="str">
         <f>IF(ISBLANK(B26),"",VLOOKUP(B26,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4592,9 +4589,9 @@
     </row>
     <row r="27" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
       <c r="E27" s="25"/>
       <c r="F27" s="26"/>
       <c r="G27" s="27" t="str">
@@ -4639,12 +4636,12 @@
       <c r="AQ27" s="27"/>
       <c r="AR27" s="58"/>
       <c r="AS27" s="39"/>
-      <c r="AT27" s="78"/>
-      <c r="AU27" s="79"/>
-      <c r="AV27" s="79"/>
-      <c r="AW27" s="79"/>
-      <c r="AX27" s="79"/>
-      <c r="AY27" s="79"/>
+      <c r="AT27" s="76"/>
+      <c r="AU27" s="77"/>
+      <c r="AV27" s="77"/>
+      <c r="AW27" s="77"/>
+      <c r="AX27" s="77"/>
+      <c r="AY27" s="77"/>
       <c r="AZ27" s="33"/>
       <c r="BA27" s="34" t="str">
         <f>IF(ISBLANK(B27),"",VLOOKUP(B27,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4661,9 +4658,9 @@
     </row>
     <row r="28" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="25"/>
       <c r="F28" s="26"/>
       <c r="G28" s="27" t="str">
@@ -4710,12 +4707,12 @@
       <c r="AQ28" s="30"/>
       <c r="AR28" s="40"/>
       <c r="AS28" s="39"/>
-      <c r="AT28" s="78"/>
-      <c r="AU28" s="79"/>
-      <c r="AV28" s="79"/>
-      <c r="AW28" s="79"/>
-      <c r="AX28" s="79"/>
-      <c r="AY28" s="79"/>
+      <c r="AT28" s="76"/>
+      <c r="AU28" s="77"/>
+      <c r="AV28" s="77"/>
+      <c r="AW28" s="77"/>
+      <c r="AX28" s="77"/>
+      <c r="AY28" s="77"/>
       <c r="AZ28" s="33"/>
       <c r="BA28" s="34" t="str">
         <f>IF(ISBLANK(B28),"",VLOOKUP(B28,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4732,9 +4729,9 @@
     </row>
     <row r="29" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="25"/>
       <c r="F29" s="26"/>
       <c r="G29" s="27" t="str">
@@ -4781,12 +4778,12 @@
       <c r="AQ29" s="30"/>
       <c r="AR29" s="40"/>
       <c r="AS29" s="39"/>
-      <c r="AT29" s="78"/>
-      <c r="AU29" s="79"/>
-      <c r="AV29" s="79"/>
-      <c r="AW29" s="79"/>
-      <c r="AX29" s="79"/>
-      <c r="AY29" s="79"/>
+      <c r="AT29" s="76"/>
+      <c r="AU29" s="77"/>
+      <c r="AV29" s="77"/>
+      <c r="AW29" s="77"/>
+      <c r="AX29" s="77"/>
+      <c r="AY29" s="77"/>
       <c r="AZ29" s="33"/>
       <c r="BA29" s="34" t="str">
         <f>IF(ISBLANK(B29),"",VLOOKUP(B29,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4803,9 +4800,9 @@
     </row>
     <row r="30" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="str">
@@ -4852,12 +4849,12 @@
       <c r="AQ30" s="30"/>
       <c r="AR30" s="40"/>
       <c r="AS30" s="39"/>
-      <c r="AT30" s="78"/>
-      <c r="AU30" s="79"/>
-      <c r="AV30" s="79"/>
-      <c r="AW30" s="79"/>
-      <c r="AX30" s="79"/>
-      <c r="AY30" s="79"/>
+      <c r="AT30" s="76"/>
+      <c r="AU30" s="77"/>
+      <c r="AV30" s="77"/>
+      <c r="AW30" s="77"/>
+      <c r="AX30" s="77"/>
+      <c r="AY30" s="77"/>
       <c r="AZ30" s="33"/>
       <c r="BA30" s="34" t="str">
         <f>IF(ISBLANK(B30),"",VLOOKUP(B30,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4874,9 +4871,9 @@
     </row>
     <row r="31" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="str">
@@ -4923,12 +4920,12 @@
       <c r="AQ31" s="30"/>
       <c r="AR31" s="40"/>
       <c r="AS31" s="39"/>
-      <c r="AT31" s="78"/>
-      <c r="AU31" s="79"/>
-      <c r="AV31" s="79"/>
-      <c r="AW31" s="79"/>
-      <c r="AX31" s="79"/>
-      <c r="AY31" s="79"/>
+      <c r="AT31" s="76"/>
+      <c r="AU31" s="77"/>
+      <c r="AV31" s="77"/>
+      <c r="AW31" s="77"/>
+      <c r="AX31" s="77"/>
+      <c r="AY31" s="77"/>
       <c r="AZ31" s="33"/>
       <c r="BA31" s="34" t="str">
         <f>IF(ISBLANK(B31),"",VLOOKUP(B31,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4948,9 +4945,9 @@
     </row>
     <row r="32" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="21"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
       <c r="G32" s="27" t="str">
@@ -4997,12 +4994,12 @@
       <c r="AQ32" s="30"/>
       <c r="AR32" s="40"/>
       <c r="AS32" s="39"/>
-      <c r="AT32" s="78"/>
-      <c r="AU32" s="79"/>
-      <c r="AV32" s="79"/>
-      <c r="AW32" s="79"/>
-      <c r="AX32" s="79"/>
-      <c r="AY32" s="79"/>
+      <c r="AT32" s="76"/>
+      <c r="AU32" s="77"/>
+      <c r="AV32" s="77"/>
+      <c r="AW32" s="77"/>
+      <c r="AX32" s="77"/>
+      <c r="AY32" s="77"/>
       <c r="AZ32" s="33"/>
       <c r="BA32" s="34" t="str">
         <f>IF(ISBLANK(B32),"",VLOOKUP(B32,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5019,9 +5016,9 @@
     </row>
     <row r="33" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="27" t="str">
@@ -5068,12 +5065,12 @@
       <c r="AQ33" s="30"/>
       <c r="AR33" s="40"/>
       <c r="AS33" s="39"/>
-      <c r="AT33" s="78"/>
-      <c r="AU33" s="79"/>
-      <c r="AV33" s="79"/>
-      <c r="AW33" s="79"/>
-      <c r="AX33" s="79"/>
-      <c r="AY33" s="79"/>
+      <c r="AT33" s="76"/>
+      <c r="AU33" s="77"/>
+      <c r="AV33" s="77"/>
+      <c r="AW33" s="77"/>
+      <c r="AX33" s="77"/>
+      <c r="AY33" s="77"/>
       <c r="AZ33" s="33"/>
       <c r="BA33" s="34" t="str">
         <f>IF(ISBLANK(B33),"",VLOOKUP(B33,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5090,9 +5087,9 @@
     </row>
     <row r="34" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
       <c r="G34" s="27" t="str">
@@ -5139,12 +5136,12 @@
       <c r="AQ34" s="30"/>
       <c r="AR34" s="40"/>
       <c r="AS34" s="39"/>
-      <c r="AT34" s="78"/>
-      <c r="AU34" s="79"/>
-      <c r="AV34" s="79"/>
-      <c r="AW34" s="79"/>
-      <c r="AX34" s="79"/>
-      <c r="AY34" s="79"/>
+      <c r="AT34" s="76"/>
+      <c r="AU34" s="77"/>
+      <c r="AV34" s="77"/>
+      <c r="AW34" s="77"/>
+      <c r="AX34" s="77"/>
+      <c r="AY34" s="77"/>
       <c r="AZ34" s="33"/>
       <c r="BA34" s="34" t="str">
         <f>IF(ISBLANK(B34),"",VLOOKUP(B34,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5161,9 +5158,9 @@
     </row>
     <row r="35" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
       <c r="G35" s="27" t="str">
@@ -5210,12 +5207,12 @@
       <c r="AQ35" s="30"/>
       <c r="AR35" s="40"/>
       <c r="AS35" s="39"/>
-      <c r="AT35" s="78"/>
-      <c r="AU35" s="79"/>
-      <c r="AV35" s="79"/>
-      <c r="AW35" s="79"/>
-      <c r="AX35" s="79"/>
-      <c r="AY35" s="79"/>
+      <c r="AT35" s="76"/>
+      <c r="AU35" s="77"/>
+      <c r="AV35" s="77"/>
+      <c r="AW35" s="77"/>
+      <c r="AX35" s="77"/>
+      <c r="AY35" s="77"/>
       <c r="AZ35" s="33"/>
       <c r="BA35" s="34" t="str">
         <f>IF(ISBLANK(B35),"",VLOOKUP(B35,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5232,58 +5229,58 @@
     </row>
     <row r="36" spans="1:58" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="81"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="81"/>
-      <c r="N36" s="81"/>
-      <c r="O36" s="81"/>
-      <c r="P36" s="81"/>
-      <c r="Q36" s="81"/>
-      <c r="R36" s="81"/>
-      <c r="S36" s="81"/>
-      <c r="T36" s="81"/>
-      <c r="U36" s="81"/>
-      <c r="V36" s="81"/>
-      <c r="W36" s="81"/>
-      <c r="X36" s="81"/>
-      <c r="Y36" s="81"/>
-      <c r="Z36" s="81"/>
-      <c r="AA36" s="81"/>
-      <c r="AB36" s="81"/>
-      <c r="AC36" s="81"/>
-      <c r="AD36" s="81"/>
-      <c r="AE36" s="81"/>
-      <c r="AF36" s="81"/>
-      <c r="AG36" s="81"/>
-      <c r="AH36" s="81"/>
-      <c r="AI36" s="81"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="96"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
+      <c r="Q36" s="96"/>
+      <c r="R36" s="96"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="96"/>
+      <c r="U36" s="96"/>
+      <c r="V36" s="96"/>
+      <c r="W36" s="96"/>
+      <c r="X36" s="96"/>
+      <c r="Y36" s="96"/>
+      <c r="Z36" s="96"/>
+      <c r="AA36" s="96"/>
+      <c r="AB36" s="96"/>
+      <c r="AC36" s="96"/>
+      <c r="AD36" s="96"/>
+      <c r="AE36" s="96"/>
+      <c r="AF36" s="96"/>
+      <c r="AG36" s="96"/>
+      <c r="AH36" s="96"/>
+      <c r="AI36" s="96"/>
       <c r="AJ36" s="26"/>
       <c r="AK36" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AL36" s="82"/>
-      <c r="AM36" s="83"/>
-      <c r="AN36" s="83"/>
-      <c r="AO36" s="83"/>
-      <c r="AP36" s="83"/>
-      <c r="AQ36" s="83"/>
+      <c r="AL36" s="97"/>
+      <c r="AM36" s="98"/>
+      <c r="AN36" s="98"/>
+      <c r="AO36" s="98"/>
+      <c r="AP36" s="98"/>
+      <c r="AQ36" s="98"/>
       <c r="AR36" s="25"/>
       <c r="AS36" s="39"/>
-      <c r="AT36" s="84"/>
-      <c r="AU36" s="85"/>
-      <c r="AV36" s="85"/>
-      <c r="AW36" s="85"/>
-      <c r="AX36" s="85"/>
-      <c r="AY36" s="85"/>
+      <c r="AT36" s="99"/>
+      <c r="AU36" s="100"/>
+      <c r="AV36" s="100"/>
+      <c r="AW36" s="100"/>
+      <c r="AX36" s="100"/>
+      <c r="AY36" s="100"/>
       <c r="AZ36" s="33"/>
       <c r="BA36" s="34" t="str">
         <f>IF(ISBLANK(B36),"",VLOOKUP(B36,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5402,17 +5399,17 @@
         <v>10</v>
       </c>
       <c r="AR38" s="1"/>
-      <c r="AS38" s="65">
+      <c r="AS38" s="107">
         <f>SUM(AT15:AY35)</f>
         <v>0</v>
       </c>
-      <c r="AT38" s="66"/>
-      <c r="AU38" s="66"/>
-      <c r="AV38" s="66"/>
-      <c r="AW38" s="66"/>
-      <c r="AX38" s="66"/>
-      <c r="AY38" s="66"/>
-      <c r="AZ38" s="66"/>
+      <c r="AT38" s="108"/>
+      <c r="AU38" s="108"/>
+      <c r="AV38" s="108"/>
+      <c r="AW38" s="108"/>
+      <c r="AX38" s="108"/>
+      <c r="AY38" s="108"/>
+      <c r="AZ38" s="108"/>
       <c r="BA38" s="24"/>
     </row>
     <row r="39" spans="1:58" s="20" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5471,58 +5468,58 @@
       <c r="BA39" s="24"/>
     </row>
     <row r="40" spans="1:58" s="20" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69"/>
-      <c r="Q40" s="69"/>
-      <c r="R40" s="69"/>
-      <c r="S40" s="69"/>
-      <c r="T40" s="69"/>
-      <c r="U40" s="69"/>
-      <c r="V40" s="69"/>
-      <c r="W40" s="69"/>
-      <c r="X40" s="69"/>
-      <c r="Y40" s="69"/>
-      <c r="Z40" s="69"/>
-      <c r="AA40" s="69"/>
-      <c r="AB40" s="69"/>
-      <c r="AC40" s="69"/>
-      <c r="AD40" s="69"/>
-      <c r="AE40" s="69"/>
-      <c r="AF40" s="69"/>
-      <c r="AG40" s="69"/>
-      <c r="AH40" s="69"/>
-      <c r="AI40" s="69"/>
-      <c r="AJ40" s="69"/>
-      <c r="AK40" s="69"/>
-      <c r="AL40" s="69"/>
-      <c r="AM40" s="69"/>
-      <c r="AN40" s="69"/>
-      <c r="AO40" s="69"/>
-      <c r="AP40" s="69"/>
-      <c r="AQ40" s="69"/>
-      <c r="AR40" s="69"/>
-      <c r="AS40" s="69"/>
-      <c r="AT40" s="69"/>
-      <c r="AU40" s="69"/>
-      <c r="AV40" s="69"/>
-      <c r="AW40" s="69"/>
-      <c r="AX40" s="69"/>
-      <c r="AY40" s="69"/>
-      <c r="AZ40" s="69"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
+      <c r="J40" s="110"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="111"/>
+      <c r="N40" s="111"/>
+      <c r="O40" s="111"/>
+      <c r="P40" s="111"/>
+      <c r="Q40" s="111"/>
+      <c r="R40" s="111"/>
+      <c r="S40" s="111"/>
+      <c r="T40" s="111"/>
+      <c r="U40" s="111"/>
+      <c r="V40" s="111"/>
+      <c r="W40" s="111"/>
+      <c r="X40" s="111"/>
+      <c r="Y40" s="111"/>
+      <c r="Z40" s="111"/>
+      <c r="AA40" s="111"/>
+      <c r="AB40" s="111"/>
+      <c r="AC40" s="111"/>
+      <c r="AD40" s="111"/>
+      <c r="AE40" s="111"/>
+      <c r="AF40" s="111"/>
+      <c r="AG40" s="111"/>
+      <c r="AH40" s="111"/>
+      <c r="AI40" s="111"/>
+      <c r="AJ40" s="111"/>
+      <c r="AK40" s="111"/>
+      <c r="AL40" s="111"/>
+      <c r="AM40" s="111"/>
+      <c r="AN40" s="111"/>
+      <c r="AO40" s="111"/>
+      <c r="AP40" s="111"/>
+      <c r="AQ40" s="111"/>
+      <c r="AR40" s="111"/>
+      <c r="AS40" s="111"/>
+      <c r="AT40" s="111"/>
+      <c r="AU40" s="111"/>
+      <c r="AV40" s="111"/>
+      <c r="AW40" s="111"/>
+      <c r="AX40" s="111"/>
+      <c r="AY40" s="111"/>
+      <c r="AZ40" s="111"/>
       <c r="BA40" s="24"/>
     </row>
     <row r="41" spans="1:58" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
@@ -5552,22 +5549,22 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="70"/>
-      <c r="AB41" s="70"/>
-      <c r="AC41" s="70"/>
-      <c r="AD41" s="70"/>
-      <c r="AE41" s="70"/>
-      <c r="AF41" s="70"/>
-      <c r="AG41" s="70"/>
-      <c r="AH41" s="70"/>
-      <c r="AI41" s="70"/>
-      <c r="AJ41" s="70"/>
-      <c r="AK41" s="70"/>
-      <c r="AL41" s="70"/>
-      <c r="AM41" s="70"/>
-      <c r="AN41" s="70"/>
-      <c r="AO41" s="70"/>
-      <c r="AP41" s="70"/>
+      <c r="AA41" s="112"/>
+      <c r="AB41" s="112"/>
+      <c r="AC41" s="112"/>
+      <c r="AD41" s="112"/>
+      <c r="AE41" s="112"/>
+      <c r="AF41" s="112"/>
+      <c r="AG41" s="112"/>
+      <c r="AH41" s="112"/>
+      <c r="AI41" s="112"/>
+      <c r="AJ41" s="112"/>
+      <c r="AK41" s="112"/>
+      <c r="AL41" s="112"/>
+      <c r="AM41" s="112"/>
+      <c r="AN41" s="112"/>
+      <c r="AO41" s="112"/>
+      <c r="AP41" s="112"/>
       <c r="AQ41" s="1"/>
       <c r="AR41" s="48"/>
       <c r="AS41" s="1"/>
@@ -5582,133 +5579,196 @@
       <c r="BB41" s="51"/>
     </row>
     <row r="42" spans="1:58" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="71" t="s">
+      <c r="A42" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="71"/>
-      <c r="M42" s="71"/>
-      <c r="N42" s="71"/>
-      <c r="O42" s="71"/>
-      <c r="P42" s="71"/>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="73" t="s">
+      <c r="B42" s="113"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+      <c r="G42" s="113"/>
+      <c r="H42" s="113"/>
+      <c r="I42" s="113"/>
+      <c r="J42" s="113"/>
+      <c r="K42" s="113"/>
+      <c r="L42" s="113"/>
+      <c r="M42" s="113"/>
+      <c r="N42" s="113"/>
+      <c r="O42" s="113"/>
+      <c r="P42" s="113"/>
+      <c r="Q42" s="114"/>
+      <c r="R42" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
-      <c r="W42" s="71"/>
-      <c r="X42" s="71"/>
-      <c r="Y42" s="71"/>
-      <c r="Z42" s="71"/>
-      <c r="AA42" s="71"/>
-      <c r="AB42" s="71"/>
-      <c r="AC42" s="71"/>
-      <c r="AD42" s="71"/>
-      <c r="AE42" s="71"/>
-      <c r="AF42" s="71"/>
-      <c r="AG42" s="71"/>
-      <c r="AH42" s="71"/>
-      <c r="AI42" s="71"/>
-      <c r="AJ42" s="71"/>
-      <c r="AK42" s="71"/>
-      <c r="AL42" s="72"/>
-      <c r="AM42" s="74" t="s">
+      <c r="S42" s="113"/>
+      <c r="T42" s="113"/>
+      <c r="U42" s="113"/>
+      <c r="V42" s="113"/>
+      <c r="W42" s="113"/>
+      <c r="X42" s="113"/>
+      <c r="Y42" s="113"/>
+      <c r="Z42" s="113"/>
+      <c r="AA42" s="113"/>
+      <c r="AB42" s="113"/>
+      <c r="AC42" s="113"/>
+      <c r="AD42" s="113"/>
+      <c r="AE42" s="113"/>
+      <c r="AF42" s="113"/>
+      <c r="AG42" s="113"/>
+      <c r="AH42" s="113"/>
+      <c r="AI42" s="113"/>
+      <c r="AJ42" s="113"/>
+      <c r="AK42" s="113"/>
+      <c r="AL42" s="114"/>
+      <c r="AM42" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="AN42" s="75"/>
-      <c r="AO42" s="75"/>
-      <c r="AP42" s="75"/>
-      <c r="AQ42" s="75"/>
-      <c r="AR42" s="75"/>
-      <c r="AS42" s="75"/>
-      <c r="AT42" s="75"/>
-      <c r="AU42" s="75"/>
-      <c r="AV42" s="75"/>
-      <c r="AW42" s="75"/>
-      <c r="AX42" s="75"/>
-      <c r="AY42" s="75"/>
-      <c r="AZ42" s="75"/>
-      <c r="BA42" s="75"/>
-      <c r="BB42" s="75"/>
-      <c r="BC42" s="76"/>
+      <c r="AN42" s="117"/>
+      <c r="AO42" s="117"/>
+      <c r="AP42" s="117"/>
+      <c r="AQ42" s="117"/>
+      <c r="AR42" s="117"/>
+      <c r="AS42" s="117"/>
+      <c r="AT42" s="117"/>
+      <c r="AU42" s="117"/>
+      <c r="AV42" s="117"/>
+      <c r="AW42" s="117"/>
+      <c r="AX42" s="117"/>
+      <c r="AY42" s="117"/>
+      <c r="AZ42" s="117"/>
+      <c r="BA42" s="117"/>
+      <c r="BB42" s="117"/>
+      <c r="BC42" s="118"/>
     </row>
     <row r="43" spans="1:58" s="20" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="60"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="60"/>
-      <c r="N43" s="60"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="60"/>
-      <c r="Q43" s="61"/>
-      <c r="R43" s="62" t="s">
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="102"/>
+      <c r="J43" s="102"/>
+      <c r="K43" s="102"/>
+      <c r="L43" s="102"/>
+      <c r="M43" s="102"/>
+      <c r="N43" s="102"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="102"/>
+      <c r="Q43" s="103"/>
+      <c r="R43" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="S43" s="60"/>
-      <c r="T43" s="60"/>
-      <c r="U43" s="60"/>
-      <c r="V43" s="60"/>
-      <c r="W43" s="60"/>
-      <c r="X43" s="60"/>
-      <c r="Y43" s="60"/>
-      <c r="Z43" s="60"/>
-      <c r="AA43" s="60"/>
-      <c r="AB43" s="60"/>
-      <c r="AC43" s="60"/>
-      <c r="AD43" s="60"/>
-      <c r="AE43" s="60"/>
-      <c r="AF43" s="60"/>
-      <c r="AG43" s="60"/>
-      <c r="AH43" s="60"/>
-      <c r="AI43" s="63"/>
-      <c r="AJ43" s="63"/>
-      <c r="AK43" s="63"/>
-      <c r="AL43" s="64"/>
-      <c r="AM43" s="59" t="s">
+      <c r="S43" s="102"/>
+      <c r="T43" s="102"/>
+      <c r="U43" s="102"/>
+      <c r="V43" s="102"/>
+      <c r="W43" s="102"/>
+      <c r="X43" s="102"/>
+      <c r="Y43" s="102"/>
+      <c r="Z43" s="102"/>
+      <c r="AA43" s="102"/>
+      <c r="AB43" s="102"/>
+      <c r="AC43" s="102"/>
+      <c r="AD43" s="102"/>
+      <c r="AE43" s="102"/>
+      <c r="AF43" s="102"/>
+      <c r="AG43" s="102"/>
+      <c r="AH43" s="102"/>
+      <c r="AI43" s="105"/>
+      <c r="AJ43" s="105"/>
+      <c r="AK43" s="105"/>
+      <c r="AL43" s="106"/>
+      <c r="AM43" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="AN43" s="60"/>
-      <c r="AO43" s="60"/>
-      <c r="AP43" s="60"/>
-      <c r="AQ43" s="60"/>
-      <c r="AR43" s="60"/>
-      <c r="AS43" s="60"/>
-      <c r="AT43" s="60"/>
-      <c r="AU43" s="60"/>
-      <c r="AV43" s="60"/>
-      <c r="AW43" s="60"/>
-      <c r="AX43" s="60"/>
-      <c r="AY43" s="60"/>
-      <c r="AZ43" s="60"/>
-      <c r="BA43" s="60"/>
-      <c r="BB43" s="60"/>
-      <c r="BC43" s="61"/>
+      <c r="AN43" s="102"/>
+      <c r="AO43" s="102"/>
+      <c r="AP43" s="102"/>
+      <c r="AQ43" s="102"/>
+      <c r="AR43" s="102"/>
+      <c r="AS43" s="102"/>
+      <c r="AT43" s="102"/>
+      <c r="AU43" s="102"/>
+      <c r="AV43" s="102"/>
+      <c r="AW43" s="102"/>
+      <c r="AX43" s="102"/>
+      <c r="AY43" s="102"/>
+      <c r="AZ43" s="102"/>
+      <c r="BA43" s="102"/>
+      <c r="BB43" s="102"/>
+      <c r="BC43" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A43:Q43"/>
+    <mergeCell ref="R43:AL43"/>
+    <mergeCell ref="AM43:BC43"/>
+    <mergeCell ref="AS38:AZ38"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="J40:AZ40"/>
+    <mergeCell ref="AA41:AP41"/>
+    <mergeCell ref="A42:Q42"/>
+    <mergeCell ref="R42:AL42"/>
+    <mergeCell ref="AM42:BC42"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="AT34:AY34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="AT35:AY35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G36:AI36"/>
+    <mergeCell ref="AL36:AQ36"/>
+    <mergeCell ref="AT36:AY36"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="AT31:AY31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="AT32:AY32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="AT33:AY33"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="AT28:AY28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="AT29:AY29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="AT30:AY30"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="AT25:AY25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="AT26:AY26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="AT27:AY27"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="AT18:AY18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="AT19:AY19"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="AT24:AY24"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="AT20:AY20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="AT21:AY21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="AT22:AY22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="AT23:AY23"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="AT17:AY17"/>
+    <mergeCell ref="A9:AR9"/>
+    <mergeCell ref="AS9:AZ9"/>
+    <mergeCell ref="A10:AR10"/>
+    <mergeCell ref="AS10:AZ10"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:AR13"/>
+    <mergeCell ref="AS12:AZ13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="AT15:AY15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="AT16:AY16"/>
     <mergeCell ref="AT6:AZ7"/>
     <mergeCell ref="P1:AN1"/>
     <mergeCell ref="AO1:AX1"/>
@@ -5724,69 +5784,6 @@
     <mergeCell ref="AL6:AM7"/>
     <mergeCell ref="AN6:AP7"/>
     <mergeCell ref="AQ6:AR7"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="AT17:AY17"/>
-    <mergeCell ref="A9:AR9"/>
-    <mergeCell ref="AS9:AZ9"/>
-    <mergeCell ref="A10:AR10"/>
-    <mergeCell ref="AS10:AZ10"/>
-    <mergeCell ref="A12:E13"/>
-    <mergeCell ref="F12:AR13"/>
-    <mergeCell ref="AS12:AZ13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="AT15:AY15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="AT16:AY16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="AT18:AY18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="AT19:AY19"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="AT24:AY24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="AT20:AY20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="AT21:AY21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="AT22:AY22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="AT23:AY23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="AT25:AY25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="AT26:AY26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="AT27:AY27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="AT28:AY28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="AT29:AY29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="AT30:AY30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="AT31:AY31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="AT32:AY32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="AT33:AY33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="AT34:AY34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="AT35:AY35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="G36:AI36"/>
-    <mergeCell ref="AL36:AQ36"/>
-    <mergeCell ref="AT36:AY36"/>
-    <mergeCell ref="A43:Q43"/>
-    <mergeCell ref="R43:AL43"/>
-    <mergeCell ref="AM43:BC43"/>
-    <mergeCell ref="AS38:AZ38"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="J40:AZ40"/>
-    <mergeCell ref="AA41:AP41"/>
-    <mergeCell ref="A42:Q42"/>
-    <mergeCell ref="R42:AL42"/>
-    <mergeCell ref="AM42:BC42"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ41:AX42 KM41:KT42 UI41:UP42 AEE41:AEL42 AOA41:AOH42 AXW41:AYD42 BHS41:BHZ42 BRO41:BRV42 CBK41:CBR42 CLG41:CLN42 CVC41:CVJ42 DEY41:DFF42 DOU41:DPB42 DYQ41:DYX42 EIM41:EIT42 ESI41:ESP42 FCE41:FCL42 FMA41:FMH42 FVW41:FWD42 GFS41:GFZ42 GPO41:GPV42 GZK41:GZR42 HJG41:HJN42 HTC41:HTJ42 ICY41:IDF42 IMU41:INB42 IWQ41:IWX42 JGM41:JGT42 JQI41:JQP42 KAE41:KAL42 KKA41:KKH42 KTW41:KUD42 LDS41:LDZ42 LNO41:LNV42 LXK41:LXR42 MHG41:MHN42 MRC41:MRJ42 NAY41:NBF42 NKU41:NLB42 NUQ41:NUX42 OEM41:OET42 OOI41:OOP42 OYE41:OYL42 PIA41:PIH42 PRW41:PSD42 QBS41:QBZ42 QLO41:QLV42 QVK41:QVR42 RFG41:RFN42 RPC41:RPJ42 RYY41:RZF42 SIU41:SJB42 SSQ41:SSX42 TCM41:TCT42 TMI41:TMP42 TWE41:TWL42 UGA41:UGH42 UPW41:UQD42 UZS41:UZZ42 VJO41:VJV42 VTK41:VTR42 WDG41:WDN42 WNC41:WNJ42 WWY41:WXF42 AQ65577:AX65578 KM65577:KT65578 UI65577:UP65578 AEE65577:AEL65578 AOA65577:AOH65578 AXW65577:AYD65578 BHS65577:BHZ65578 BRO65577:BRV65578 CBK65577:CBR65578 CLG65577:CLN65578 CVC65577:CVJ65578 DEY65577:DFF65578 DOU65577:DPB65578 DYQ65577:DYX65578 EIM65577:EIT65578 ESI65577:ESP65578 FCE65577:FCL65578 FMA65577:FMH65578 FVW65577:FWD65578 GFS65577:GFZ65578 GPO65577:GPV65578 GZK65577:GZR65578 HJG65577:HJN65578 HTC65577:HTJ65578 ICY65577:IDF65578 IMU65577:INB65578 IWQ65577:IWX65578 JGM65577:JGT65578 JQI65577:JQP65578 KAE65577:KAL65578 KKA65577:KKH65578 KTW65577:KUD65578 LDS65577:LDZ65578 LNO65577:LNV65578 LXK65577:LXR65578 MHG65577:MHN65578 MRC65577:MRJ65578 NAY65577:NBF65578 NKU65577:NLB65578 NUQ65577:NUX65578 OEM65577:OET65578 OOI65577:OOP65578 OYE65577:OYL65578 PIA65577:PIH65578 PRW65577:PSD65578 QBS65577:QBZ65578 QLO65577:QLV65578 QVK65577:QVR65578 RFG65577:RFN65578 RPC65577:RPJ65578 RYY65577:RZF65578 SIU65577:SJB65578 SSQ65577:SSX65578 TCM65577:TCT65578 TMI65577:TMP65578 TWE65577:TWL65578 UGA65577:UGH65578 UPW65577:UQD65578 UZS65577:UZZ65578 VJO65577:VJV65578 VTK65577:VTR65578 WDG65577:WDN65578 WNC65577:WNJ65578 WWY65577:WXF65578 AQ131113:AX131114 KM131113:KT131114 UI131113:UP131114 AEE131113:AEL131114 AOA131113:AOH131114 AXW131113:AYD131114 BHS131113:BHZ131114 BRO131113:BRV131114 CBK131113:CBR131114 CLG131113:CLN131114 CVC131113:CVJ131114 DEY131113:DFF131114 DOU131113:DPB131114 DYQ131113:DYX131114 EIM131113:EIT131114 ESI131113:ESP131114 FCE131113:FCL131114 FMA131113:FMH131114 FVW131113:FWD131114 GFS131113:GFZ131114 GPO131113:GPV131114 GZK131113:GZR131114 HJG131113:HJN131114 HTC131113:HTJ131114 ICY131113:IDF131114 IMU131113:INB131114 IWQ131113:IWX131114 JGM131113:JGT131114 JQI131113:JQP131114 KAE131113:KAL131114 KKA131113:KKH131114 KTW131113:KUD131114 LDS131113:LDZ131114 LNO131113:LNV131114 LXK131113:LXR131114 MHG131113:MHN131114 MRC131113:MRJ131114 NAY131113:NBF131114 NKU131113:NLB131114 NUQ131113:NUX131114 OEM131113:OET131114 OOI131113:OOP131114 OYE131113:OYL131114 PIA131113:PIH131114 PRW131113:PSD131114 QBS131113:QBZ131114 QLO131113:QLV131114 QVK131113:QVR131114 RFG131113:RFN131114 RPC131113:RPJ131114 RYY131113:RZF131114 SIU131113:SJB131114 SSQ131113:SSX131114 TCM131113:TCT131114 TMI131113:TMP131114 TWE131113:TWL131114 UGA131113:UGH131114 UPW131113:UQD131114 UZS131113:UZZ131114 VJO131113:VJV131114 VTK131113:VTR131114 WDG131113:WDN131114 WNC131113:WNJ131114 WWY131113:WXF131114 AQ196649:AX196650 KM196649:KT196650 UI196649:UP196650 AEE196649:AEL196650 AOA196649:AOH196650 AXW196649:AYD196650 BHS196649:BHZ196650 BRO196649:BRV196650 CBK196649:CBR196650 CLG196649:CLN196650 CVC196649:CVJ196650 DEY196649:DFF196650 DOU196649:DPB196650 DYQ196649:DYX196650 EIM196649:EIT196650 ESI196649:ESP196650 FCE196649:FCL196650 FMA196649:FMH196650 FVW196649:FWD196650 GFS196649:GFZ196650 GPO196649:GPV196650 GZK196649:GZR196650 HJG196649:HJN196650 HTC196649:HTJ196650 ICY196649:IDF196650 IMU196649:INB196650 IWQ196649:IWX196650 JGM196649:JGT196650 JQI196649:JQP196650 KAE196649:KAL196650 KKA196649:KKH196650 KTW196649:KUD196650 LDS196649:LDZ196650 LNO196649:LNV196650 LXK196649:LXR196650 MHG196649:MHN196650 MRC196649:MRJ196650 NAY196649:NBF196650 NKU196649:NLB196650 NUQ196649:NUX196650 OEM196649:OET196650 OOI196649:OOP196650 OYE196649:OYL196650 PIA196649:PIH196650 PRW196649:PSD196650 QBS196649:QBZ196650 QLO196649:QLV196650 QVK196649:QVR196650 RFG196649:RFN196650 RPC196649:RPJ196650 RYY196649:RZF196650 SIU196649:SJB196650 SSQ196649:SSX196650 TCM196649:TCT196650 TMI196649:TMP196650 TWE196649:TWL196650 UGA196649:UGH196650 UPW196649:UQD196650 UZS196649:UZZ196650 VJO196649:VJV196650 VTK196649:VTR196650 WDG196649:WDN196650 WNC196649:WNJ196650 WWY196649:WXF196650 AQ262185:AX262186 KM262185:KT262186 UI262185:UP262186 AEE262185:AEL262186 AOA262185:AOH262186 AXW262185:AYD262186 BHS262185:BHZ262186 BRO262185:BRV262186 CBK262185:CBR262186 CLG262185:CLN262186 CVC262185:CVJ262186 DEY262185:DFF262186 DOU262185:DPB262186 DYQ262185:DYX262186 EIM262185:EIT262186 ESI262185:ESP262186 FCE262185:FCL262186 FMA262185:FMH262186 FVW262185:FWD262186 GFS262185:GFZ262186 GPO262185:GPV262186 GZK262185:GZR262186 HJG262185:HJN262186 HTC262185:HTJ262186 ICY262185:IDF262186 IMU262185:INB262186 IWQ262185:IWX262186 JGM262185:JGT262186 JQI262185:JQP262186 KAE262185:KAL262186 KKA262185:KKH262186 KTW262185:KUD262186 LDS262185:LDZ262186 LNO262185:LNV262186 LXK262185:LXR262186 MHG262185:MHN262186 MRC262185:MRJ262186 NAY262185:NBF262186 NKU262185:NLB262186 NUQ262185:NUX262186 OEM262185:OET262186 OOI262185:OOP262186 OYE262185:OYL262186 PIA262185:PIH262186 PRW262185:PSD262186 QBS262185:QBZ262186 QLO262185:QLV262186 QVK262185:QVR262186 RFG262185:RFN262186 RPC262185:RPJ262186 RYY262185:RZF262186 SIU262185:SJB262186 SSQ262185:SSX262186 TCM262185:TCT262186 TMI262185:TMP262186 TWE262185:TWL262186 UGA262185:UGH262186 UPW262185:UQD262186 UZS262185:UZZ262186 VJO262185:VJV262186 VTK262185:VTR262186 WDG262185:WDN262186 WNC262185:WNJ262186 WWY262185:WXF262186 AQ327721:AX327722 KM327721:KT327722 UI327721:UP327722 AEE327721:AEL327722 AOA327721:AOH327722 AXW327721:AYD327722 BHS327721:BHZ327722 BRO327721:BRV327722 CBK327721:CBR327722 CLG327721:CLN327722 CVC327721:CVJ327722 DEY327721:DFF327722 DOU327721:DPB327722 DYQ327721:DYX327722 EIM327721:EIT327722 ESI327721:ESP327722 FCE327721:FCL327722 FMA327721:FMH327722 FVW327721:FWD327722 GFS327721:GFZ327722 GPO327721:GPV327722 GZK327721:GZR327722 HJG327721:HJN327722 HTC327721:HTJ327722 ICY327721:IDF327722 IMU327721:INB327722 IWQ327721:IWX327722 JGM327721:JGT327722 JQI327721:JQP327722 KAE327721:KAL327722 KKA327721:KKH327722 KTW327721:KUD327722 LDS327721:LDZ327722 LNO327721:LNV327722 LXK327721:LXR327722 MHG327721:MHN327722 MRC327721:MRJ327722 NAY327721:NBF327722 NKU327721:NLB327722 NUQ327721:NUX327722 OEM327721:OET327722 OOI327721:OOP327722 OYE327721:OYL327722 PIA327721:PIH327722 PRW327721:PSD327722 QBS327721:QBZ327722 QLO327721:QLV327722 QVK327721:QVR327722 RFG327721:RFN327722 RPC327721:RPJ327722 RYY327721:RZF327722 SIU327721:SJB327722 SSQ327721:SSX327722 TCM327721:TCT327722 TMI327721:TMP327722 TWE327721:TWL327722 UGA327721:UGH327722 UPW327721:UQD327722 UZS327721:UZZ327722 VJO327721:VJV327722 VTK327721:VTR327722 WDG327721:WDN327722 WNC327721:WNJ327722 WWY327721:WXF327722 AQ393257:AX393258 KM393257:KT393258 UI393257:UP393258 AEE393257:AEL393258 AOA393257:AOH393258 AXW393257:AYD393258 BHS393257:BHZ393258 BRO393257:BRV393258 CBK393257:CBR393258 CLG393257:CLN393258 CVC393257:CVJ393258 DEY393257:DFF393258 DOU393257:DPB393258 DYQ393257:DYX393258 EIM393257:EIT393258 ESI393257:ESP393258 FCE393257:FCL393258 FMA393257:FMH393258 FVW393257:FWD393258 GFS393257:GFZ393258 GPO393257:GPV393258 GZK393257:GZR393258 HJG393257:HJN393258 HTC393257:HTJ393258 ICY393257:IDF393258 IMU393257:INB393258 IWQ393257:IWX393258 JGM393257:JGT393258 JQI393257:JQP393258 KAE393257:KAL393258 KKA393257:KKH393258 KTW393257:KUD393258 LDS393257:LDZ393258 LNO393257:LNV393258 LXK393257:LXR393258 MHG393257:MHN393258 MRC393257:MRJ393258 NAY393257:NBF393258 NKU393257:NLB393258 NUQ393257:NUX393258 OEM393257:OET393258 OOI393257:OOP393258 OYE393257:OYL393258 PIA393257:PIH393258 PRW393257:PSD393258 QBS393257:QBZ393258 QLO393257:QLV393258 QVK393257:QVR393258 RFG393257:RFN393258 RPC393257:RPJ393258 RYY393257:RZF393258 SIU393257:SJB393258 SSQ393257:SSX393258 TCM393257:TCT393258 TMI393257:TMP393258 TWE393257:TWL393258 UGA393257:UGH393258 UPW393257:UQD393258 UZS393257:UZZ393258 VJO393257:VJV393258 VTK393257:VTR393258 WDG393257:WDN393258 WNC393257:WNJ393258 WWY393257:WXF393258 AQ458793:AX458794 KM458793:KT458794 UI458793:UP458794 AEE458793:AEL458794 AOA458793:AOH458794 AXW458793:AYD458794 BHS458793:BHZ458794 BRO458793:BRV458794 CBK458793:CBR458794 CLG458793:CLN458794 CVC458793:CVJ458794 DEY458793:DFF458794 DOU458793:DPB458794 DYQ458793:DYX458794 EIM458793:EIT458794 ESI458793:ESP458794 FCE458793:FCL458794 FMA458793:FMH458794 FVW458793:FWD458794 GFS458793:GFZ458794 GPO458793:GPV458794 GZK458793:GZR458794 HJG458793:HJN458794 HTC458793:HTJ458794 ICY458793:IDF458794 IMU458793:INB458794 IWQ458793:IWX458794 JGM458793:JGT458794 JQI458793:JQP458794 KAE458793:KAL458794 KKA458793:KKH458794 KTW458793:KUD458794 LDS458793:LDZ458794 LNO458793:LNV458794 LXK458793:LXR458794 MHG458793:MHN458794 MRC458793:MRJ458794 NAY458793:NBF458794 NKU458793:NLB458794 NUQ458793:NUX458794 OEM458793:OET458794 OOI458793:OOP458794 OYE458793:OYL458794 PIA458793:PIH458794 PRW458793:PSD458794 QBS458793:QBZ458794 QLO458793:QLV458794 QVK458793:QVR458794 RFG458793:RFN458794 RPC458793:RPJ458794 RYY458793:RZF458794 SIU458793:SJB458794 SSQ458793:SSX458794 TCM458793:TCT458794 TMI458793:TMP458794 TWE458793:TWL458794 UGA458793:UGH458794 UPW458793:UQD458794 UZS458793:UZZ458794 VJO458793:VJV458794 VTK458793:VTR458794 WDG458793:WDN458794 WNC458793:WNJ458794 WWY458793:WXF458794 AQ524329:AX524330 KM524329:KT524330 UI524329:UP524330 AEE524329:AEL524330 AOA524329:AOH524330 AXW524329:AYD524330 BHS524329:BHZ524330 BRO524329:BRV524330 CBK524329:CBR524330 CLG524329:CLN524330 CVC524329:CVJ524330 DEY524329:DFF524330 DOU524329:DPB524330 DYQ524329:DYX524330 EIM524329:EIT524330 ESI524329:ESP524330 FCE524329:FCL524330 FMA524329:FMH524330 FVW524329:FWD524330 GFS524329:GFZ524330 GPO524329:GPV524330 GZK524329:GZR524330 HJG524329:HJN524330 HTC524329:HTJ524330 ICY524329:IDF524330 IMU524329:INB524330 IWQ524329:IWX524330 JGM524329:JGT524330 JQI524329:JQP524330 KAE524329:KAL524330 KKA524329:KKH524330 KTW524329:KUD524330 LDS524329:LDZ524330 LNO524329:LNV524330 LXK524329:LXR524330 MHG524329:MHN524330 MRC524329:MRJ524330 NAY524329:NBF524330 NKU524329:NLB524330 NUQ524329:NUX524330 OEM524329:OET524330 OOI524329:OOP524330 OYE524329:OYL524330 PIA524329:PIH524330 PRW524329:PSD524330 QBS524329:QBZ524330 QLO524329:QLV524330 QVK524329:QVR524330 RFG524329:RFN524330 RPC524329:RPJ524330 RYY524329:RZF524330 SIU524329:SJB524330 SSQ524329:SSX524330 TCM524329:TCT524330 TMI524329:TMP524330 TWE524329:TWL524330 UGA524329:UGH524330 UPW524329:UQD524330 UZS524329:UZZ524330 VJO524329:VJV524330 VTK524329:VTR524330 WDG524329:WDN524330 WNC524329:WNJ524330 WWY524329:WXF524330 AQ589865:AX589866 KM589865:KT589866 UI589865:UP589866 AEE589865:AEL589866 AOA589865:AOH589866 AXW589865:AYD589866 BHS589865:BHZ589866 BRO589865:BRV589866 CBK589865:CBR589866 CLG589865:CLN589866 CVC589865:CVJ589866 DEY589865:DFF589866 DOU589865:DPB589866 DYQ589865:DYX589866 EIM589865:EIT589866 ESI589865:ESP589866 FCE589865:FCL589866 FMA589865:FMH589866 FVW589865:FWD589866 GFS589865:GFZ589866 GPO589865:GPV589866 GZK589865:GZR589866 HJG589865:HJN589866 HTC589865:HTJ589866 ICY589865:IDF589866 IMU589865:INB589866 IWQ589865:IWX589866 JGM589865:JGT589866 JQI589865:JQP589866 KAE589865:KAL589866 KKA589865:KKH589866 KTW589865:KUD589866 LDS589865:LDZ589866 LNO589865:LNV589866 LXK589865:LXR589866 MHG589865:MHN589866 MRC589865:MRJ589866 NAY589865:NBF589866 NKU589865:NLB589866 NUQ589865:NUX589866 OEM589865:OET589866 OOI589865:OOP589866 OYE589865:OYL589866 PIA589865:PIH589866 PRW589865:PSD589866 QBS589865:QBZ589866 QLO589865:QLV589866 QVK589865:QVR589866 RFG589865:RFN589866 RPC589865:RPJ589866 RYY589865:RZF589866 SIU589865:SJB589866 SSQ589865:SSX589866 TCM589865:TCT589866 TMI589865:TMP589866 TWE589865:TWL589866 UGA589865:UGH589866 UPW589865:UQD589866 UZS589865:UZZ589866 VJO589865:VJV589866 VTK589865:VTR589866 WDG589865:WDN589866 WNC589865:WNJ589866 WWY589865:WXF589866 AQ655401:AX655402 KM655401:KT655402 UI655401:UP655402 AEE655401:AEL655402 AOA655401:AOH655402 AXW655401:AYD655402 BHS655401:BHZ655402 BRO655401:BRV655402 CBK655401:CBR655402 CLG655401:CLN655402 CVC655401:CVJ655402 DEY655401:DFF655402 DOU655401:DPB655402 DYQ655401:DYX655402 EIM655401:EIT655402 ESI655401:ESP655402 FCE655401:FCL655402 FMA655401:FMH655402 FVW655401:FWD655402 GFS655401:GFZ655402 GPO655401:GPV655402 GZK655401:GZR655402 HJG655401:HJN655402 HTC655401:HTJ655402 ICY655401:IDF655402 IMU655401:INB655402 IWQ655401:IWX655402 JGM655401:JGT655402 JQI655401:JQP655402 KAE655401:KAL655402 KKA655401:KKH655402 KTW655401:KUD655402 LDS655401:LDZ655402 LNO655401:LNV655402 LXK655401:LXR655402 MHG655401:MHN655402 MRC655401:MRJ655402 NAY655401:NBF655402 NKU655401:NLB655402 NUQ655401:NUX655402 OEM655401:OET655402 OOI655401:OOP655402 OYE655401:OYL655402 PIA655401:PIH655402 PRW655401:PSD655402 QBS655401:QBZ655402 QLO655401:QLV655402 QVK655401:QVR655402 RFG655401:RFN655402 RPC655401:RPJ655402 RYY655401:RZF655402 SIU655401:SJB655402 SSQ655401:SSX655402 TCM655401:TCT655402 TMI655401:TMP655402 TWE655401:TWL655402 UGA655401:UGH655402 UPW655401:UQD655402 UZS655401:UZZ655402 VJO655401:VJV655402 VTK655401:VTR655402 WDG655401:WDN655402 WNC655401:WNJ655402 WWY655401:WXF655402 AQ720937:AX720938 KM720937:KT720938 UI720937:UP720938 AEE720937:AEL720938 AOA720937:AOH720938 AXW720937:AYD720938 BHS720937:BHZ720938 BRO720937:BRV720938 CBK720937:CBR720938 CLG720937:CLN720938 CVC720937:CVJ720938 DEY720937:DFF720938 DOU720937:DPB720938 DYQ720937:DYX720938 EIM720937:EIT720938 ESI720937:ESP720938 FCE720937:FCL720938 FMA720937:FMH720938 FVW720937:FWD720938 GFS720937:GFZ720938 GPO720937:GPV720938 GZK720937:GZR720938 HJG720937:HJN720938 HTC720937:HTJ720938 ICY720937:IDF720938 IMU720937:INB720938 IWQ720937:IWX720938 JGM720937:JGT720938 JQI720937:JQP720938 KAE720937:KAL720938 KKA720937:KKH720938 KTW720937:KUD720938 LDS720937:LDZ720938 LNO720937:LNV720938 LXK720937:LXR720938 MHG720937:MHN720938 MRC720937:MRJ720938 NAY720937:NBF720938 NKU720937:NLB720938 NUQ720937:NUX720938 OEM720937:OET720938 OOI720937:OOP720938 OYE720937:OYL720938 PIA720937:PIH720938 PRW720937:PSD720938 QBS720937:QBZ720938 QLO720937:QLV720938 QVK720937:QVR720938 RFG720937:RFN720938 RPC720937:RPJ720938 RYY720937:RZF720938 SIU720937:SJB720938 SSQ720937:SSX720938 TCM720937:TCT720938 TMI720937:TMP720938 TWE720937:TWL720938 UGA720937:UGH720938 UPW720937:UQD720938 UZS720937:UZZ720938 VJO720937:VJV720938 VTK720937:VTR720938 WDG720937:WDN720938 WNC720937:WNJ720938 WWY720937:WXF720938 AQ786473:AX786474 KM786473:KT786474 UI786473:UP786474 AEE786473:AEL786474 AOA786473:AOH786474 AXW786473:AYD786474 BHS786473:BHZ786474 BRO786473:BRV786474 CBK786473:CBR786474 CLG786473:CLN786474 CVC786473:CVJ786474 DEY786473:DFF786474 DOU786473:DPB786474 DYQ786473:DYX786474 EIM786473:EIT786474 ESI786473:ESP786474 FCE786473:FCL786474 FMA786473:FMH786474 FVW786473:FWD786474 GFS786473:GFZ786474 GPO786473:GPV786474 GZK786473:GZR786474 HJG786473:HJN786474 HTC786473:HTJ786474 ICY786473:IDF786474 IMU786473:INB786474 IWQ786473:IWX786474 JGM786473:JGT786474 JQI786473:JQP786474 KAE786473:KAL786474 KKA786473:KKH786474 KTW786473:KUD786474 LDS786473:LDZ786474 LNO786473:LNV786474 LXK786473:LXR786474 MHG786473:MHN786474 MRC786473:MRJ786474 NAY786473:NBF786474 NKU786473:NLB786474 NUQ786473:NUX786474 OEM786473:OET786474 OOI786473:OOP786474 OYE786473:OYL786474 PIA786473:PIH786474 PRW786473:PSD786474 QBS786473:QBZ786474 QLO786473:QLV786474 QVK786473:QVR786474 RFG786473:RFN786474 RPC786473:RPJ786474 RYY786473:RZF786474 SIU786473:SJB786474 SSQ786473:SSX786474 TCM786473:TCT786474 TMI786473:TMP786474 TWE786473:TWL786474 UGA786473:UGH786474 UPW786473:UQD786474 UZS786473:UZZ786474 VJO786473:VJV786474 VTK786473:VTR786474 WDG786473:WDN786474 WNC786473:WNJ786474 WWY786473:WXF786474 AQ852009:AX852010 KM852009:KT852010 UI852009:UP852010 AEE852009:AEL852010 AOA852009:AOH852010 AXW852009:AYD852010 BHS852009:BHZ852010 BRO852009:BRV852010 CBK852009:CBR852010 CLG852009:CLN852010 CVC852009:CVJ852010 DEY852009:DFF852010 DOU852009:DPB852010 DYQ852009:DYX852010 EIM852009:EIT852010 ESI852009:ESP852010 FCE852009:FCL852010 FMA852009:FMH852010 FVW852009:FWD852010 GFS852009:GFZ852010 GPO852009:GPV852010 GZK852009:GZR852010 HJG852009:HJN852010 HTC852009:HTJ852010 ICY852009:IDF852010 IMU852009:INB852010 IWQ852009:IWX852010 JGM852009:JGT852010 JQI852009:JQP852010 KAE852009:KAL852010 KKA852009:KKH852010 KTW852009:KUD852010 LDS852009:LDZ852010 LNO852009:LNV852010 LXK852009:LXR852010 MHG852009:MHN852010 MRC852009:MRJ852010 NAY852009:NBF852010 NKU852009:NLB852010 NUQ852009:NUX852010 OEM852009:OET852010 OOI852009:OOP852010 OYE852009:OYL852010 PIA852009:PIH852010 PRW852009:PSD852010 QBS852009:QBZ852010 QLO852009:QLV852010 QVK852009:QVR852010 RFG852009:RFN852010 RPC852009:RPJ852010 RYY852009:RZF852010 SIU852009:SJB852010 SSQ852009:SSX852010 TCM852009:TCT852010 TMI852009:TMP852010 TWE852009:TWL852010 UGA852009:UGH852010 UPW852009:UQD852010 UZS852009:UZZ852010 VJO852009:VJV852010 VTK852009:VTR852010 WDG852009:WDN852010 WNC852009:WNJ852010 WWY852009:WXF852010 AQ917545:AX917546 KM917545:KT917546 UI917545:UP917546 AEE917545:AEL917546 AOA917545:AOH917546 AXW917545:AYD917546 BHS917545:BHZ917546 BRO917545:BRV917546 CBK917545:CBR917546 CLG917545:CLN917546 CVC917545:CVJ917546 DEY917545:DFF917546 DOU917545:DPB917546 DYQ917545:DYX917546 EIM917545:EIT917546 ESI917545:ESP917546 FCE917545:FCL917546 FMA917545:FMH917546 FVW917545:FWD917546 GFS917545:GFZ917546 GPO917545:GPV917546 GZK917545:GZR917546 HJG917545:HJN917546 HTC917545:HTJ917546 ICY917545:IDF917546 IMU917545:INB917546 IWQ917545:IWX917546 JGM917545:JGT917546 JQI917545:JQP917546 KAE917545:KAL917546 KKA917545:KKH917546 KTW917545:KUD917546 LDS917545:LDZ917546 LNO917545:LNV917546 LXK917545:LXR917546 MHG917545:MHN917546 MRC917545:MRJ917546 NAY917545:NBF917546 NKU917545:NLB917546 NUQ917545:NUX917546 OEM917545:OET917546 OOI917545:OOP917546 OYE917545:OYL917546 PIA917545:PIH917546 PRW917545:PSD917546 QBS917545:QBZ917546 QLO917545:QLV917546 QVK917545:QVR917546 RFG917545:RFN917546 RPC917545:RPJ917546 RYY917545:RZF917546 SIU917545:SJB917546 SSQ917545:SSX917546 TCM917545:TCT917546 TMI917545:TMP917546 TWE917545:TWL917546 UGA917545:UGH917546 UPW917545:UQD917546 UZS917545:UZZ917546 VJO917545:VJV917546 VTK917545:VTR917546 WDG917545:WDN917546 WNC917545:WNJ917546 WWY917545:WXF917546 AQ983081:AX983082 KM983081:KT983082 UI983081:UP983082 AEE983081:AEL983082 AOA983081:AOH983082 AXW983081:AYD983082 BHS983081:BHZ983082 BRO983081:BRV983082 CBK983081:CBR983082 CLG983081:CLN983082 CVC983081:CVJ983082 DEY983081:DFF983082 DOU983081:DPB983082 DYQ983081:DYX983082 EIM983081:EIT983082 ESI983081:ESP983082 FCE983081:FCL983082 FMA983081:FMH983082 FVW983081:FWD983082 GFS983081:GFZ983082 GPO983081:GPV983082 GZK983081:GZR983082 HJG983081:HJN983082 HTC983081:HTJ983082 ICY983081:IDF983082 IMU983081:INB983082 IWQ983081:IWX983082 JGM983081:JGT983082 JQI983081:JQP983082 KAE983081:KAL983082 KKA983081:KKH983082 KTW983081:KUD983082 LDS983081:LDZ983082 LNO983081:LNV983082 LXK983081:LXR983082 MHG983081:MHN983082 MRC983081:MRJ983082 NAY983081:NBF983082 NKU983081:NLB983082 NUQ983081:NUX983082 OEM983081:OET983082 OOI983081:OOP983082 OYE983081:OYL983082 PIA983081:PIH983082 PRW983081:PSD983082 QBS983081:QBZ983082 QLO983081:QLV983082 QVK983081:QVR983082 RFG983081:RFN983082 RPC983081:RPJ983082 RYY983081:RZF983082 SIU983081:SJB983082 SSQ983081:SSX983082 TCM983081:TCT983082 TMI983081:TMP983082 TWE983081:TWL983082 UGA983081:UGH983082 UPW983081:UQD983082 UZS983081:UZZ983082 VJO983081:VJV983082 VTK983081:VTR983082 WDG983081:WDN983082 WNC983081:WNJ983082 WWY983081:WXF983082 X41:Z41 JT41:JV41 TP41:TR41 ADL41:ADN41 ANH41:ANJ41 AXD41:AXF41 BGZ41:BHB41 BQV41:BQX41 CAR41:CAT41 CKN41:CKP41 CUJ41:CUL41 DEF41:DEH41 DOB41:DOD41 DXX41:DXZ41 EHT41:EHV41 ERP41:ERR41 FBL41:FBN41 FLH41:FLJ41 FVD41:FVF41 GEZ41:GFB41 GOV41:GOX41 GYR41:GYT41 HIN41:HIP41 HSJ41:HSL41 ICF41:ICH41 IMB41:IMD41 IVX41:IVZ41 JFT41:JFV41 JPP41:JPR41 JZL41:JZN41 KJH41:KJJ41 KTD41:KTF41 LCZ41:LDB41 LMV41:LMX41 LWR41:LWT41 MGN41:MGP41 MQJ41:MQL41 NAF41:NAH41 NKB41:NKD41 NTX41:NTZ41 ODT41:ODV41 ONP41:ONR41 OXL41:OXN41 PHH41:PHJ41 PRD41:PRF41 QAZ41:QBB41 QKV41:QKX41 QUR41:QUT41 REN41:REP41 ROJ41:ROL41 RYF41:RYH41 SIB41:SID41 SRX41:SRZ41 TBT41:TBV41 TLP41:TLR41 TVL41:TVN41 UFH41:UFJ41 UPD41:UPF41 UYZ41:UZB41 VIV41:VIX41 VSR41:VST41 WCN41:WCP41 WMJ41:WML41 WWF41:WWH41 X65577:Z65577 JT65577:JV65577 TP65577:TR65577 ADL65577:ADN65577 ANH65577:ANJ65577 AXD65577:AXF65577 BGZ65577:BHB65577 BQV65577:BQX65577 CAR65577:CAT65577 CKN65577:CKP65577 CUJ65577:CUL65577 DEF65577:DEH65577 DOB65577:DOD65577 DXX65577:DXZ65577 EHT65577:EHV65577 ERP65577:ERR65577 FBL65577:FBN65577 FLH65577:FLJ65577 FVD65577:FVF65577 GEZ65577:GFB65577 GOV65577:GOX65577 GYR65577:GYT65577 HIN65577:HIP65577 HSJ65577:HSL65577 ICF65577:ICH65577 IMB65577:IMD65577 IVX65577:IVZ65577 JFT65577:JFV65577 JPP65577:JPR65577 JZL65577:JZN65577 KJH65577:KJJ65577 KTD65577:KTF65577 LCZ65577:LDB65577 LMV65577:LMX65577 LWR65577:LWT65577 MGN65577:MGP65577 MQJ65577:MQL65577 NAF65577:NAH65577 NKB65577:NKD65577 NTX65577:NTZ65577 ODT65577:ODV65577 ONP65577:ONR65577 OXL65577:OXN65577 PHH65577:PHJ65577 PRD65577:PRF65577 QAZ65577:QBB65577 QKV65577:QKX65577 QUR65577:QUT65577 REN65577:REP65577 ROJ65577:ROL65577 RYF65577:RYH65577 SIB65577:SID65577 SRX65577:SRZ65577 TBT65577:TBV65577 TLP65577:TLR65577 TVL65577:TVN65577 UFH65577:UFJ65577 UPD65577:UPF65577 UYZ65577:UZB65577 VIV65577:VIX65577 VSR65577:VST65577 WCN65577:WCP65577 WMJ65577:WML65577 WWF65577:WWH65577 X131113:Z131113 JT131113:JV131113 TP131113:TR131113 ADL131113:ADN131113 ANH131113:ANJ131113 AXD131113:AXF131113 BGZ131113:BHB131113 BQV131113:BQX131113 CAR131113:CAT131113 CKN131113:CKP131113 CUJ131113:CUL131113 DEF131113:DEH131113 DOB131113:DOD131113 DXX131113:DXZ131113 EHT131113:EHV131113 ERP131113:ERR131113 FBL131113:FBN131113 FLH131113:FLJ131113 FVD131113:FVF131113 GEZ131113:GFB131113 GOV131113:GOX131113 GYR131113:GYT131113 HIN131113:HIP131113 HSJ131113:HSL131113 ICF131113:ICH131113 IMB131113:IMD131113 IVX131113:IVZ131113 JFT131113:JFV131113 JPP131113:JPR131113 JZL131113:JZN131113 KJH131113:KJJ131113 KTD131113:KTF131113 LCZ131113:LDB131113 LMV131113:LMX131113 LWR131113:LWT131113 MGN131113:MGP131113 MQJ131113:MQL131113 NAF131113:NAH131113 NKB131113:NKD131113 NTX131113:NTZ131113 ODT131113:ODV131113 ONP131113:ONR131113 OXL131113:OXN131113 PHH131113:PHJ131113 PRD131113:PRF131113 QAZ131113:QBB131113 QKV131113:QKX131113 QUR131113:QUT131113 REN131113:REP131113 ROJ131113:ROL131113 RYF131113:RYH131113 SIB131113:SID131113 SRX131113:SRZ131113 TBT131113:TBV131113 TLP131113:TLR131113 TVL131113:TVN131113 UFH131113:UFJ131113 UPD131113:UPF131113 UYZ131113:UZB131113 VIV131113:VIX131113 VSR131113:VST131113 WCN131113:WCP131113 WMJ131113:WML131113 WWF131113:WWH131113 X196649:Z196649 JT196649:JV196649 TP196649:TR196649 ADL196649:ADN196649 ANH196649:ANJ196649 AXD196649:AXF196649 BGZ196649:BHB196649 BQV196649:BQX196649 CAR196649:CAT196649 CKN196649:CKP196649 CUJ196649:CUL196649 DEF196649:DEH196649 DOB196649:DOD196649 DXX196649:DXZ196649 EHT196649:EHV196649 ERP196649:ERR196649 FBL196649:FBN196649 FLH196649:FLJ196649 FVD196649:FVF196649 GEZ196649:GFB196649 GOV196649:GOX196649 GYR196649:GYT196649 HIN196649:HIP196649 HSJ196649:HSL196649 ICF196649:ICH196649 IMB196649:IMD196649 IVX196649:IVZ196649 JFT196649:JFV196649 JPP196649:JPR196649 JZL196649:JZN196649 KJH196649:KJJ196649 KTD196649:KTF196649 LCZ196649:LDB196649 LMV196649:LMX196649 LWR196649:LWT196649 MGN196649:MGP196649 MQJ196649:MQL196649 NAF196649:NAH196649 NKB196649:NKD196649 NTX196649:NTZ196649 ODT196649:ODV196649 ONP196649:ONR196649 OXL196649:OXN196649 PHH196649:PHJ196649 PRD196649:PRF196649 QAZ196649:QBB196649 QKV196649:QKX196649 QUR196649:QUT196649 REN196649:REP196649 ROJ196649:ROL196649 RYF196649:RYH196649 SIB196649:SID196649 SRX196649:SRZ196649 TBT196649:TBV196649 TLP196649:TLR196649 TVL196649:TVN196649 UFH196649:UFJ196649 UPD196649:UPF196649 UYZ196649:UZB196649 VIV196649:VIX196649 VSR196649:VST196649 WCN196649:WCP196649 WMJ196649:WML196649 WWF196649:WWH196649 X262185:Z262185 JT262185:JV262185 TP262185:TR262185 ADL262185:ADN262185 ANH262185:ANJ262185 AXD262185:AXF262185 BGZ262185:BHB262185 BQV262185:BQX262185 CAR262185:CAT262185 CKN262185:CKP262185 CUJ262185:CUL262185 DEF262185:DEH262185 DOB262185:DOD262185 DXX262185:DXZ262185 EHT262185:EHV262185 ERP262185:ERR262185 FBL262185:FBN262185 FLH262185:FLJ262185 FVD262185:FVF262185 GEZ262185:GFB262185 GOV262185:GOX262185 GYR262185:GYT262185 HIN262185:HIP262185 HSJ262185:HSL262185 ICF262185:ICH262185 IMB262185:IMD262185 IVX262185:IVZ262185 JFT262185:JFV262185 JPP262185:JPR262185 JZL262185:JZN262185 KJH262185:KJJ262185 KTD262185:KTF262185 LCZ262185:LDB262185 LMV262185:LMX262185 LWR262185:LWT262185 MGN262185:MGP262185 MQJ262185:MQL262185 NAF262185:NAH262185 NKB262185:NKD262185 NTX262185:NTZ262185 ODT262185:ODV262185 ONP262185:ONR262185 OXL262185:OXN262185 PHH262185:PHJ262185 PRD262185:PRF262185 QAZ262185:QBB262185 QKV262185:QKX262185 QUR262185:QUT262185 REN262185:REP262185 ROJ262185:ROL262185 RYF262185:RYH262185 SIB262185:SID262185 SRX262185:SRZ262185 TBT262185:TBV262185 TLP262185:TLR262185 TVL262185:TVN262185 UFH262185:UFJ262185 UPD262185:UPF262185 UYZ262185:UZB262185 VIV262185:VIX262185 VSR262185:VST262185 WCN262185:WCP262185 WMJ262185:WML262185 WWF262185:WWH262185 X327721:Z327721 JT327721:JV327721 TP327721:TR327721 ADL327721:ADN327721 ANH327721:ANJ327721 AXD327721:AXF327721 BGZ327721:BHB327721 BQV327721:BQX327721 CAR327721:CAT327721 CKN327721:CKP327721 CUJ327721:CUL327721 DEF327721:DEH327721 DOB327721:DOD327721 DXX327721:DXZ327721 EHT327721:EHV327721 ERP327721:ERR327721 FBL327721:FBN327721 FLH327721:FLJ327721 FVD327721:FVF327721 GEZ327721:GFB327721 GOV327721:GOX327721 GYR327721:GYT327721 HIN327721:HIP327721 HSJ327721:HSL327721 ICF327721:ICH327721 IMB327721:IMD327721 IVX327721:IVZ327721 JFT327721:JFV327721 JPP327721:JPR327721 JZL327721:JZN327721 KJH327721:KJJ327721 KTD327721:KTF327721 LCZ327721:LDB327721 LMV327721:LMX327721 LWR327721:LWT327721 MGN327721:MGP327721 MQJ327721:MQL327721 NAF327721:NAH327721 NKB327721:NKD327721 NTX327721:NTZ327721 ODT327721:ODV327721 ONP327721:ONR327721 OXL327721:OXN327721 PHH327721:PHJ327721 PRD327721:PRF327721 QAZ327721:QBB327721 QKV327721:QKX327721 QUR327721:QUT327721 REN327721:REP327721 ROJ327721:ROL327721 RYF327721:RYH327721 SIB327721:SID327721 SRX327721:SRZ327721 TBT327721:TBV327721 TLP327721:TLR327721 TVL327721:TVN327721 UFH327721:UFJ327721 UPD327721:UPF327721 UYZ327721:UZB327721 VIV327721:VIX327721 VSR327721:VST327721 WCN327721:WCP327721 WMJ327721:WML327721 WWF327721:WWH327721 X393257:Z393257 JT393257:JV393257 TP393257:TR393257 ADL393257:ADN393257 ANH393257:ANJ393257 AXD393257:AXF393257 BGZ393257:BHB393257 BQV393257:BQX393257 CAR393257:CAT393257 CKN393257:CKP393257 CUJ393257:CUL393257 DEF393257:DEH393257 DOB393257:DOD393257 DXX393257:DXZ393257 EHT393257:EHV393257 ERP393257:ERR393257 FBL393257:FBN393257 FLH393257:FLJ393257 FVD393257:FVF393257 GEZ393257:GFB393257 GOV393257:GOX393257 GYR393257:GYT393257 HIN393257:HIP393257 HSJ393257:HSL393257 ICF393257:ICH393257 IMB393257:IMD393257 IVX393257:IVZ393257 JFT393257:JFV393257 JPP393257:JPR393257 JZL393257:JZN393257 KJH393257:KJJ393257 KTD393257:KTF393257 LCZ393257:LDB393257 LMV393257:LMX393257 LWR393257:LWT393257 MGN393257:MGP393257 MQJ393257:MQL393257 NAF393257:NAH393257 NKB393257:NKD393257 NTX393257:NTZ393257 ODT393257:ODV393257 ONP393257:ONR393257 OXL393257:OXN393257 PHH393257:PHJ393257 PRD393257:PRF393257 QAZ393257:QBB393257 QKV393257:QKX393257 QUR393257:QUT393257 REN393257:REP393257 ROJ393257:ROL393257 RYF393257:RYH393257 SIB393257:SID393257 SRX393257:SRZ393257 TBT393257:TBV393257 TLP393257:TLR393257 TVL393257:TVN393257 UFH393257:UFJ393257 UPD393257:UPF393257 UYZ393257:UZB393257 VIV393257:VIX393257 VSR393257:VST393257 WCN393257:WCP393257 WMJ393257:WML393257 WWF393257:WWH393257 X458793:Z458793 JT458793:JV458793 TP458793:TR458793 ADL458793:ADN458793 ANH458793:ANJ458793 AXD458793:AXF458793 BGZ458793:BHB458793 BQV458793:BQX458793 CAR458793:CAT458793 CKN458793:CKP458793 CUJ458793:CUL458793 DEF458793:DEH458793 DOB458793:DOD458793 DXX458793:DXZ458793 EHT458793:EHV458793 ERP458793:ERR458793 FBL458793:FBN458793 FLH458793:FLJ458793 FVD458793:FVF458793 GEZ458793:GFB458793 GOV458793:GOX458793 GYR458793:GYT458793 HIN458793:HIP458793 HSJ458793:HSL458793 ICF458793:ICH458793 IMB458793:IMD458793 IVX458793:IVZ458793 JFT458793:JFV458793 JPP458793:JPR458793 JZL458793:JZN458793 KJH458793:KJJ458793 KTD458793:KTF458793 LCZ458793:LDB458793 LMV458793:LMX458793 LWR458793:LWT458793 MGN458793:MGP458793 MQJ458793:MQL458793 NAF458793:NAH458793 NKB458793:NKD458793 NTX458793:NTZ458793 ODT458793:ODV458793 ONP458793:ONR458793 OXL458793:OXN458793 PHH458793:PHJ458793 PRD458793:PRF458793 QAZ458793:QBB458793 QKV458793:QKX458793 QUR458793:QUT458793 REN458793:REP458793 ROJ458793:ROL458793 RYF458793:RYH458793 SIB458793:SID458793 SRX458793:SRZ458793 TBT458793:TBV458793 TLP458793:TLR458793 TVL458793:TVN458793 UFH458793:UFJ458793 UPD458793:UPF458793 UYZ458793:UZB458793 VIV458793:VIX458793 VSR458793:VST458793 WCN458793:WCP458793 WMJ458793:WML458793 WWF458793:WWH458793 X524329:Z524329 JT524329:JV524329 TP524329:TR524329 ADL524329:ADN524329 ANH524329:ANJ524329 AXD524329:AXF524329 BGZ524329:BHB524329 BQV524329:BQX524329 CAR524329:CAT524329 CKN524329:CKP524329 CUJ524329:CUL524329 DEF524329:DEH524329 DOB524329:DOD524329 DXX524329:DXZ524329 EHT524329:EHV524329 ERP524329:ERR524329 FBL524329:FBN524329 FLH524329:FLJ524329 FVD524329:FVF524329 GEZ524329:GFB524329 GOV524329:GOX524329 GYR524329:GYT524329 HIN524329:HIP524329 HSJ524329:HSL524329 ICF524329:ICH524329 IMB524329:IMD524329 IVX524329:IVZ524329 JFT524329:JFV524329 JPP524329:JPR524329 JZL524329:JZN524329 KJH524329:KJJ524329 KTD524329:KTF524329 LCZ524329:LDB524329 LMV524329:LMX524329 LWR524329:LWT524329 MGN524329:MGP524329 MQJ524329:MQL524329 NAF524329:NAH524329 NKB524329:NKD524329 NTX524329:NTZ524329 ODT524329:ODV524329 ONP524329:ONR524329 OXL524329:OXN524329 PHH524329:PHJ524329 PRD524329:PRF524329 QAZ524329:QBB524329 QKV524329:QKX524329 QUR524329:QUT524329 REN524329:REP524329 ROJ524329:ROL524329 RYF524329:RYH524329 SIB524329:SID524329 SRX524329:SRZ524329 TBT524329:TBV524329 TLP524329:TLR524329 TVL524329:TVN524329 UFH524329:UFJ524329 UPD524329:UPF524329 UYZ524329:UZB524329 VIV524329:VIX524329 VSR524329:VST524329 WCN524329:WCP524329 WMJ524329:WML524329 WWF524329:WWH524329 X589865:Z589865 JT589865:JV589865 TP589865:TR589865 ADL589865:ADN589865 ANH589865:ANJ589865 AXD589865:AXF589865 BGZ589865:BHB589865 BQV589865:BQX589865 CAR589865:CAT589865 CKN589865:CKP589865 CUJ589865:CUL589865 DEF589865:DEH589865 DOB589865:DOD589865 DXX589865:DXZ589865 EHT589865:EHV589865 ERP589865:ERR589865 FBL589865:FBN589865 FLH589865:FLJ589865 FVD589865:FVF589865 GEZ589865:GFB589865 GOV589865:GOX589865 GYR589865:GYT589865 HIN589865:HIP589865 HSJ589865:HSL589865 ICF589865:ICH589865 IMB589865:IMD589865 IVX589865:IVZ589865 JFT589865:JFV589865 JPP589865:JPR589865 JZL589865:JZN589865 KJH589865:KJJ589865 KTD589865:KTF589865 LCZ589865:LDB589865 LMV589865:LMX589865 LWR589865:LWT589865 MGN589865:MGP589865 MQJ589865:MQL589865 NAF589865:NAH589865 NKB589865:NKD589865 NTX589865:NTZ589865 ODT589865:ODV589865 ONP589865:ONR589865 OXL589865:OXN589865 PHH589865:PHJ589865 PRD589865:PRF589865 QAZ589865:QBB589865 QKV589865:QKX589865 QUR589865:QUT589865 REN589865:REP589865 ROJ589865:ROL589865 RYF589865:RYH589865 SIB589865:SID589865 SRX589865:SRZ589865 TBT589865:TBV589865 TLP589865:TLR589865 TVL589865:TVN589865 UFH589865:UFJ589865 UPD589865:UPF589865 UYZ589865:UZB589865 VIV589865:VIX589865 VSR589865:VST589865 WCN589865:WCP589865 WMJ589865:WML589865 WWF589865:WWH589865 X655401:Z655401 JT655401:JV655401 TP655401:TR655401 ADL655401:ADN655401 ANH655401:ANJ655401 AXD655401:AXF655401 BGZ655401:BHB655401 BQV655401:BQX655401 CAR655401:CAT655401 CKN655401:CKP655401 CUJ655401:CUL655401 DEF655401:DEH655401 DOB655401:DOD655401 DXX655401:DXZ655401 EHT655401:EHV655401 ERP655401:ERR655401 FBL655401:FBN655401 FLH655401:FLJ655401 FVD655401:FVF655401 GEZ655401:GFB655401 GOV655401:GOX655401 GYR655401:GYT655401 HIN655401:HIP655401 HSJ655401:HSL655401 ICF655401:ICH655401 IMB655401:IMD655401 IVX655401:IVZ655401 JFT655401:JFV655401 JPP655401:JPR655401 JZL655401:JZN655401 KJH655401:KJJ655401 KTD655401:KTF655401 LCZ655401:LDB655401 LMV655401:LMX655401 LWR655401:LWT655401 MGN655401:MGP655401 MQJ655401:MQL655401 NAF655401:NAH655401 NKB655401:NKD655401 NTX655401:NTZ655401 ODT655401:ODV655401 ONP655401:ONR655401 OXL655401:OXN655401 PHH655401:PHJ655401 PRD655401:PRF655401 QAZ655401:QBB655401 QKV655401:QKX655401 QUR655401:QUT655401 REN655401:REP655401 ROJ655401:ROL655401 RYF655401:RYH655401 SIB655401:SID655401 SRX655401:SRZ655401 TBT655401:TBV655401 TLP655401:TLR655401 TVL655401:TVN655401 UFH655401:UFJ655401 UPD655401:UPF655401 UYZ655401:UZB655401 VIV655401:VIX655401 VSR655401:VST655401 WCN655401:WCP655401 WMJ655401:WML655401 WWF655401:WWH655401 X720937:Z720937 JT720937:JV720937 TP720937:TR720937 ADL720937:ADN720937 ANH720937:ANJ720937 AXD720937:AXF720937 BGZ720937:BHB720937 BQV720937:BQX720937 CAR720937:CAT720937 CKN720937:CKP720937 CUJ720937:CUL720937 DEF720937:DEH720937 DOB720937:DOD720937 DXX720937:DXZ720937 EHT720937:EHV720937 ERP720937:ERR720937 FBL720937:FBN720937 FLH720937:FLJ720937 FVD720937:FVF720937 GEZ720937:GFB720937 GOV720937:GOX720937 GYR720937:GYT720937 HIN720937:HIP720937 HSJ720937:HSL720937 ICF720937:ICH720937 IMB720937:IMD720937 IVX720937:IVZ720937 JFT720937:JFV720937 JPP720937:JPR720937 JZL720937:JZN720937 KJH720937:KJJ720937 KTD720937:KTF720937 LCZ720937:LDB720937 LMV720937:LMX720937 LWR720937:LWT720937 MGN720937:MGP720937 MQJ720937:MQL720937 NAF720937:NAH720937 NKB720937:NKD720937 NTX720937:NTZ720937 ODT720937:ODV720937 ONP720937:ONR720937 OXL720937:OXN720937 PHH720937:PHJ720937 PRD720937:PRF720937 QAZ720937:QBB720937 QKV720937:QKX720937 QUR720937:QUT720937 REN720937:REP720937 ROJ720937:ROL720937 RYF720937:RYH720937 SIB720937:SID720937 SRX720937:SRZ720937 TBT720937:TBV720937 TLP720937:TLR720937 TVL720937:TVN720937 UFH720937:UFJ720937 UPD720937:UPF720937 UYZ720937:UZB720937 VIV720937:VIX720937 VSR720937:VST720937 WCN720937:WCP720937 WMJ720937:WML720937 WWF720937:WWH720937 X786473:Z786473 JT786473:JV786473 TP786473:TR786473 ADL786473:ADN786473 ANH786473:ANJ786473 AXD786473:AXF786473 BGZ786473:BHB786473 BQV786473:BQX786473 CAR786473:CAT786473 CKN786473:CKP786473 CUJ786473:CUL786473 DEF786473:DEH786473 DOB786473:DOD786473 DXX786473:DXZ786473 EHT786473:EHV786473 ERP786473:ERR786473 FBL786473:FBN786473 FLH786473:FLJ786473 FVD786473:FVF786473 GEZ786473:GFB786473 GOV786473:GOX786473 GYR786473:GYT786473 HIN786473:HIP786473 HSJ786473:HSL786473 ICF786473:ICH786473 IMB786473:IMD786473 IVX786473:IVZ786473 JFT786473:JFV786473 JPP786473:JPR786473 JZL786473:JZN786473 KJH786473:KJJ786473 KTD786473:KTF786473 LCZ786473:LDB786473 LMV786473:LMX786473 LWR786473:LWT786473 MGN786473:MGP786473 MQJ786473:MQL786473 NAF786473:NAH786473 NKB786473:NKD786473 NTX786473:NTZ786473 ODT786473:ODV786473 ONP786473:ONR786473 OXL786473:OXN786473 PHH786473:PHJ786473 PRD786473:PRF786473 QAZ786473:QBB786473 QKV786473:QKX786473 QUR786473:QUT786473 REN786473:REP786473 ROJ786473:ROL786473 RYF786473:RYH786473 SIB786473:SID786473 SRX786473:SRZ786473 TBT786473:TBV786473 TLP786473:TLR786473 TVL786473:TVN786473 UFH786473:UFJ786473 UPD786473:UPF786473 UYZ786473:UZB786473 VIV786473:VIX786473 VSR786473:VST786473 WCN786473:WCP786473 WMJ786473:WML786473 WWF786473:WWH786473 X852009:Z852009 JT852009:JV852009 TP852009:TR852009 ADL852009:ADN852009 ANH852009:ANJ852009 AXD852009:AXF852009 BGZ852009:BHB852009 BQV852009:BQX852009 CAR852009:CAT852009 CKN852009:CKP852009 CUJ852009:CUL852009 DEF852009:DEH852009 DOB852009:DOD852009 DXX852009:DXZ852009 EHT852009:EHV852009 ERP852009:ERR852009 FBL852009:FBN852009 FLH852009:FLJ852009 FVD852009:FVF852009 GEZ852009:GFB852009 GOV852009:GOX852009 GYR852009:GYT852009 HIN852009:HIP852009 HSJ852009:HSL852009 ICF852009:ICH852009 IMB852009:IMD852009 IVX852009:IVZ852009 JFT852009:JFV852009 JPP852009:JPR852009 JZL852009:JZN852009 KJH852009:KJJ852009 KTD852009:KTF852009 LCZ852009:LDB852009 LMV852009:LMX852009 LWR852009:LWT852009 MGN852009:MGP852009 MQJ852009:MQL852009 NAF852009:NAH852009 NKB852009:NKD852009 NTX852009:NTZ852009 ODT852009:ODV852009 ONP852009:ONR852009 OXL852009:OXN852009 PHH852009:PHJ852009 PRD852009:PRF852009 QAZ852009:QBB852009 QKV852009:QKX852009 QUR852009:QUT852009 REN852009:REP852009 ROJ852009:ROL852009 RYF852009:RYH852009 SIB852009:SID852009 SRX852009:SRZ852009 TBT852009:TBV852009 TLP852009:TLR852009 TVL852009:TVN852009 UFH852009:UFJ852009 UPD852009:UPF852009 UYZ852009:UZB852009 VIV852009:VIX852009 VSR852009:VST852009 WCN852009:WCP852009 WMJ852009:WML852009 WWF852009:WWH852009 X917545:Z917545 JT917545:JV917545 TP917545:TR917545 ADL917545:ADN917545 ANH917545:ANJ917545 AXD917545:AXF917545 BGZ917545:BHB917545 BQV917545:BQX917545 CAR917545:CAT917545 CKN917545:CKP917545 CUJ917545:CUL917545 DEF917545:DEH917545 DOB917545:DOD917545 DXX917545:DXZ917545 EHT917545:EHV917545 ERP917545:ERR917545 FBL917545:FBN917545 FLH917545:FLJ917545 FVD917545:FVF917545 GEZ917545:GFB917545 GOV917545:GOX917545 GYR917545:GYT917545 HIN917545:HIP917545 HSJ917545:HSL917545 ICF917545:ICH917545 IMB917545:IMD917545 IVX917545:IVZ917545 JFT917545:JFV917545 JPP917545:JPR917545 JZL917545:JZN917545 KJH917545:KJJ917545 KTD917545:KTF917545 LCZ917545:LDB917545 LMV917545:LMX917545 LWR917545:LWT917545 MGN917545:MGP917545 MQJ917545:MQL917545 NAF917545:NAH917545 NKB917545:NKD917545 NTX917545:NTZ917545 ODT917545:ODV917545 ONP917545:ONR917545 OXL917545:OXN917545 PHH917545:PHJ917545 PRD917545:PRF917545 QAZ917545:QBB917545 QKV917545:QKX917545 QUR917545:QUT917545 REN917545:REP917545 ROJ917545:ROL917545 RYF917545:RYH917545 SIB917545:SID917545 SRX917545:SRZ917545 TBT917545:TBV917545 TLP917545:TLR917545 TVL917545:TVN917545 UFH917545:UFJ917545 UPD917545:UPF917545 UYZ917545:UZB917545 VIV917545:VIX917545 VSR917545:VST917545 WCN917545:WCP917545 WMJ917545:WML917545 WWF917545:WWH917545 X983081:Z983081 JT983081:JV983081 TP983081:TR983081 ADL983081:ADN983081 ANH983081:ANJ983081 AXD983081:AXF983081 BGZ983081:BHB983081 BQV983081:BQX983081 CAR983081:CAT983081 CKN983081:CKP983081 CUJ983081:CUL983081 DEF983081:DEH983081 DOB983081:DOD983081 DXX983081:DXZ983081 EHT983081:EHV983081 ERP983081:ERR983081 FBL983081:FBN983081 FLH983081:FLJ983081 FVD983081:FVF983081 GEZ983081:GFB983081 GOV983081:GOX983081 GYR983081:GYT983081 HIN983081:HIP983081 HSJ983081:HSL983081 ICF983081:ICH983081 IMB983081:IMD983081 IVX983081:IVZ983081 JFT983081:JFV983081 JPP983081:JPR983081 JZL983081:JZN983081 KJH983081:KJJ983081 KTD983081:KTF983081 LCZ983081:LDB983081 LMV983081:LMX983081 LWR983081:LWT983081 MGN983081:MGP983081 MQJ983081:MQL983081 NAF983081:NAH983081 NKB983081:NKD983081 NTX983081:NTZ983081 ODT983081:ODV983081 ONP983081:ONR983081 OXL983081:OXN983081 PHH983081:PHJ983081 PRD983081:PRF983081 QAZ983081:QBB983081 QKV983081:QKX983081 QUR983081:QUT983081 REN983081:REP983081 ROJ983081:ROL983081 RYF983081:RYH983081 SIB983081:SID983081 SRX983081:SRZ983081 TBT983081:TBV983081 TLP983081:TLR983081 TVL983081:TVN983081 UFH983081:UFJ983081 UPD983081:UPF983081 UYZ983081:UZB983081 VIV983081:VIX983081 VSR983081:VST983081 WCN983081:WCP983081 WMJ983081:WML983081 WWF983081:WWH983081" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Corregi la plantilla, poliza especial, y una excepcion al crear
</commit_message>
<xml_diff>
--- a/assets/plantillaIngresos.xlsx
+++ b/assets/plantillaIngresos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\OneDrive\Escritorio\python\programaEscuela\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\OneDrive\Escritorio\python\programaEscuela - copia\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCE6CA-A097-40B8-B57B-1F86C2CA85FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350037AF-FFE9-4911-9B2C-EFFA350F6A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>500+</t>
-  </si>
-  <si>
-    <t>JOSÉ EDUARDO MARTÍNEZ CRUZ</t>
   </si>
 </sst>
 </file>
@@ -518,6 +515,170 @@
     <xf numFmtId="44" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
@@ -576,170 +737,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2170,8 +2167,8 @@
   </sheetPr>
   <dimension ref="A1:CF43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="69" zoomScaleNormal="69" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" zoomScaleNormal="69" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:AR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2905,45 +2902,45 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
-      <c r="AE1" s="61"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="61"/>
-      <c r="AH1" s="61"/>
-      <c r="AI1" s="61"/>
-      <c r="AJ1" s="61"/>
-      <c r="AK1" s="61"/>
-      <c r="AL1" s="61"/>
-      <c r="AM1" s="61"/>
-      <c r="AN1" s="61"/>
-      <c r="AO1" s="62" t="s">
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
+      <c r="AK1" s="105"/>
+      <c r="AL1" s="105"/>
+      <c r="AM1" s="105"/>
+      <c r="AN1" s="105"/>
+      <c r="AO1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="64"/>
-      <c r="AZ1" s="64"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="107"/>
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="107"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="108"/>
+      <c r="AZ1" s="108"/>
     </row>
     <row r="2" spans="1:61" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -3000,60 +2997,60 @@
       <c r="AZ2" s="56"/>
     </row>
     <row r="3" spans="1:61" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65"/>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="65"/>
-      <c r="AL3" s="65"/>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65"/>
-      <c r="AX3" s="65"/>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109"/>
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109"/>
+      <c r="AH3" s="109"/>
+      <c r="AI3" s="109"/>
+      <c r="AJ3" s="109"/>
+      <c r="AK3" s="109"/>
+      <c r="AL3" s="109"/>
+      <c r="AM3" s="109"/>
+      <c r="AN3" s="109"/>
+      <c r="AO3" s="109"/>
+      <c r="AP3" s="109"/>
+      <c r="AQ3" s="109"/>
+      <c r="AR3" s="109"/>
+      <c r="AS3" s="109"/>
+      <c r="AT3" s="109"/>
+      <c r="AU3" s="109"/>
+      <c r="AV3" s="109"/>
+      <c r="AW3" s="109"/>
+      <c r="AX3" s="109"/>
+      <c r="AY3" s="109"/>
+      <c r="AZ3" s="109"/>
     </row>
     <row r="4" spans="1:61" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -3097,16 +3094,16 @@
       <c r="AM4" s="6"/>
       <c r="AN4" s="6"/>
       <c r="AO4" s="7"/>
-      <c r="AP4" s="62"/>
-      <c r="AQ4" s="63"/>
-      <c r="AR4" s="63"/>
-      <c r="AS4" s="63"/>
-      <c r="AT4" s="63"/>
-      <c r="AU4" s="63"/>
-      <c r="AV4" s="63"/>
-      <c r="AW4" s="63"/>
-      <c r="AX4" s="63"/>
-      <c r="AY4" s="63"/>
+      <c r="AP4" s="106"/>
+      <c r="AQ4" s="107"/>
+      <c r="AR4" s="107"/>
+      <c r="AS4" s="107"/>
+      <c r="AT4" s="107"/>
+      <c r="AU4" s="107"/>
+      <c r="AV4" s="107"/>
+      <c r="AW4" s="107"/>
+      <c r="AX4" s="107"/>
+      <c r="AY4" s="107"/>
       <c r="AZ4" s="8"/>
     </row>
     <row r="5" spans="1:61" s="13" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3129,43 +3126,43 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66"/>
+      <c r="T5" s="110"/>
+      <c r="U5" s="110"/>
+      <c r="V5" s="110"/>
+      <c r="W5" s="110"/>
+      <c r="X5" s="110"/>
+      <c r="Y5" s="110"/>
+      <c r="Z5" s="110"/>
+      <c r="AA5" s="110"/>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="66"/>
-      <c r="AE5" s="66"/>
-      <c r="AF5" s="66"/>
-      <c r="AG5" s="66"/>
-      <c r="AH5" s="66"/>
-      <c r="AI5" s="66"/>
-      <c r="AJ5" s="66"/>
+      <c r="AC5" s="110"/>
+      <c r="AD5" s="110"/>
+      <c r="AE5" s="110"/>
+      <c r="AF5" s="110"/>
+      <c r="AG5" s="110"/>
+      <c r="AH5" s="110"/>
+      <c r="AI5" s="110"/>
+      <c r="AJ5" s="110"/>
       <c r="AK5" s="12"/>
-      <c r="AL5" s="67" t="s">
+      <c r="AL5" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="AM5" s="67"/>
-      <c r="AN5" s="67"/>
-      <c r="AO5" s="67"/>
-      <c r="AP5" s="67"/>
-      <c r="AQ5" s="67"/>
-      <c r="AR5" s="67"/>
+      <c r="AM5" s="111"/>
+      <c r="AN5" s="111"/>
+      <c r="AO5" s="111"/>
+      <c r="AP5" s="111"/>
+      <c r="AQ5" s="111"/>
+      <c r="AR5" s="111"/>
       <c r="AS5" s="12"/>
-      <c r="AT5" s="67" t="s">
+      <c r="AT5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="AU5" s="67"/>
-      <c r="AV5" s="67"/>
-      <c r="AW5" s="67"/>
-      <c r="AX5" s="67"/>
-      <c r="AY5" s="67"/>
-      <c r="AZ5" s="67"/>
+      <c r="AU5" s="111"/>
+      <c r="AV5" s="111"/>
+      <c r="AW5" s="111"/>
+      <c r="AX5" s="111"/>
+      <c r="AY5" s="111"/>
+      <c r="AZ5" s="111"/>
     </row>
     <row r="6" spans="1:61" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -3187,39 +3184,39 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="68"/>
+      <c r="T6" s="112"/>
+      <c r="U6" s="112"/>
+      <c r="V6" s="112"/>
+      <c r="W6" s="112"/>
+      <c r="X6" s="112"/>
+      <c r="Y6" s="112"/>
+      <c r="Z6" s="112"/>
+      <c r="AA6" s="112"/>
       <c r="AB6" s="14"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="68"/>
-      <c r="AF6" s="68"/>
-      <c r="AG6" s="68"/>
-      <c r="AH6" s="68"/>
-      <c r="AI6" s="68"/>
-      <c r="AJ6" s="68"/>
+      <c r="AC6" s="112"/>
+      <c r="AD6" s="112"/>
+      <c r="AE6" s="112"/>
+      <c r="AF6" s="112"/>
+      <c r="AG6" s="112"/>
+      <c r="AH6" s="112"/>
+      <c r="AI6" s="112"/>
+      <c r="AJ6" s="112"/>
       <c r="AK6" s="14"/>
-      <c r="AL6" s="59"/>
-      <c r="AM6" s="69"/>
-      <c r="AN6" s="71"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="72"/>
-      <c r="AQ6" s="59"/>
-      <c r="AR6" s="69"/>
+      <c r="AL6" s="103"/>
+      <c r="AM6" s="113"/>
+      <c r="AN6" s="115"/>
+      <c r="AO6" s="113"/>
+      <c r="AP6" s="116"/>
+      <c r="AQ6" s="103"/>
+      <c r="AR6" s="113"/>
       <c r="AS6" s="12"/>
-      <c r="AT6" s="59"/>
-      <c r="AU6" s="59"/>
-      <c r="AV6" s="59"/>
-      <c r="AW6" s="59"/>
-      <c r="AX6" s="59"/>
-      <c r="AY6" s="59"/>
-      <c r="AZ6" s="59"/>
+      <c r="AT6" s="103"/>
+      <c r="AU6" s="103"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="AX6" s="103"/>
+      <c r="AY6" s="103"/>
+      <c r="AZ6" s="103"/>
     </row>
     <row r="7" spans="1:61" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3241,39 +3238,39 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
-      <c r="V7" s="68"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="112"/>
+      <c r="V7" s="112"/>
+      <c r="W7" s="112"/>
+      <c r="X7" s="112"/>
+      <c r="Y7" s="112"/>
+      <c r="Z7" s="112"/>
+      <c r="AA7" s="112"/>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="68"/>
-      <c r="AD7" s="68"/>
-      <c r="AE7" s="68"/>
-      <c r="AF7" s="68"/>
-      <c r="AG7" s="68"/>
-      <c r="AH7" s="68"/>
-      <c r="AI7" s="68"/>
-      <c r="AJ7" s="68"/>
+      <c r="AC7" s="112"/>
+      <c r="AD7" s="112"/>
+      <c r="AE7" s="112"/>
+      <c r="AF7" s="112"/>
+      <c r="AG7" s="112"/>
+      <c r="AH7" s="112"/>
+      <c r="AI7" s="112"/>
+      <c r="AJ7" s="112"/>
       <c r="AK7" s="14"/>
-      <c r="AL7" s="70"/>
-      <c r="AM7" s="70"/>
-      <c r="AN7" s="73"/>
-      <c r="AO7" s="70"/>
-      <c r="AP7" s="74"/>
-      <c r="AQ7" s="70"/>
-      <c r="AR7" s="70"/>
+      <c r="AL7" s="114"/>
+      <c r="AM7" s="114"/>
+      <c r="AN7" s="117"/>
+      <c r="AO7" s="114"/>
+      <c r="AP7" s="118"/>
+      <c r="AQ7" s="114"/>
+      <c r="AR7" s="114"/>
       <c r="AS7" s="12"/>
-      <c r="AT7" s="60"/>
-      <c r="AU7" s="60"/>
-      <c r="AV7" s="60"/>
-      <c r="AW7" s="60"/>
-      <c r="AX7" s="60"/>
-      <c r="AY7" s="60"/>
-      <c r="AZ7" s="60"/>
+      <c r="AT7" s="104"/>
+      <c r="AU7" s="104"/>
+      <c r="AV7" s="104"/>
+      <c r="AW7" s="104"/>
+      <c r="AX7" s="104"/>
+      <c r="AY7" s="104"/>
+      <c r="AZ7" s="104"/>
     </row>
     <row r="8" spans="1:61" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -3334,116 +3331,116 @@
       <c r="AZ8" s="52"/>
     </row>
     <row r="9" spans="1:61" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
-      <c r="X9" s="78"/>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78"/>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78"/>
-      <c r="AH9" s="78"/>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="78"/>
-      <c r="AL9" s="78"/>
-      <c r="AM9" s="78"/>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78"/>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="78"/>
-      <c r="AR9" s="79"/>
-      <c r="AS9" s="78" t="s">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="86"/>
+      <c r="AA9" s="86"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="86"/>
+      <c r="AD9" s="86"/>
+      <c r="AE9" s="86"/>
+      <c r="AF9" s="86"/>
+      <c r="AG9" s="86"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="86"/>
+      <c r="AJ9" s="86"/>
+      <c r="AK9" s="86"/>
+      <c r="AL9" s="86"/>
+      <c r="AM9" s="86"/>
+      <c r="AN9" s="86"/>
+      <c r="AO9" s="86"/>
+      <c r="AP9" s="86"/>
+      <c r="AQ9" s="86"/>
+      <c r="AR9" s="87"/>
+      <c r="AS9" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78"/>
-      <c r="AV9" s="78"/>
-      <c r="AW9" s="78"/>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78"/>
-      <c r="AZ9" s="78"/>
+      <c r="AT9" s="86"/>
+      <c r="AU9" s="86"/>
+      <c r="AV9" s="86"/>
+      <c r="AW9" s="86"/>
+      <c r="AX9" s="86"/>
+      <c r="AY9" s="86"/>
+      <c r="AZ9" s="86"/>
     </row>
     <row r="10" spans="1:61" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="81"/>
-      <c r="AD10" s="81"/>
-      <c r="AE10" s="81"/>
-      <c r="AF10" s="81"/>
-      <c r="AG10" s="81"/>
-      <c r="AH10" s="81"/>
-      <c r="AI10" s="81"/>
-      <c r="AJ10" s="81"/>
-      <c r="AK10" s="81"/>
-      <c r="AL10" s="81"/>
-      <c r="AM10" s="81"/>
-      <c r="AN10" s="81"/>
-      <c r="AO10" s="81"/>
-      <c r="AP10" s="81"/>
-      <c r="AQ10" s="81"/>
-      <c r="AR10" s="82"/>
-      <c r="AS10" s="83"/>
-      <c r="AT10" s="84"/>
-      <c r="AU10" s="84"/>
-      <c r="AV10" s="84"/>
-      <c r="AW10" s="84"/>
-      <c r="AX10" s="84"/>
-      <c r="AY10" s="84"/>
-      <c r="AZ10" s="84"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+      <c r="AB10" s="89"/>
+      <c r="AC10" s="89"/>
+      <c r="AD10" s="89"/>
+      <c r="AE10" s="89"/>
+      <c r="AF10" s="89"/>
+      <c r="AG10" s="89"/>
+      <c r="AH10" s="89"/>
+      <c r="AI10" s="89"/>
+      <c r="AJ10" s="89"/>
+      <c r="AK10" s="89"/>
+      <c r="AL10" s="89"/>
+      <c r="AM10" s="89"/>
+      <c r="AN10" s="89"/>
+      <c r="AO10" s="89"/>
+      <c r="AP10" s="89"/>
+      <c r="AQ10" s="89"/>
+      <c r="AR10" s="90"/>
+      <c r="AS10" s="91"/>
+      <c r="AT10" s="92"/>
+      <c r="AU10" s="92"/>
+      <c r="AV10" s="92"/>
+      <c r="AW10" s="92"/>
+      <c r="AX10" s="92"/>
+      <c r="AY10" s="92"/>
+      <c r="AZ10" s="92"/>
     </row>
     <row r="11" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -3500,118 +3497,118 @@
       <c r="AZ11" s="52"/>
     </row>
     <row r="12" spans="1:61" s="20" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="89" t="s">
+      <c r="B12" s="93"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="90"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="90"/>
-      <c r="AA12" s="90"/>
-      <c r="AB12" s="90"/>
-      <c r="AC12" s="90"/>
-      <c r="AD12" s="90"/>
-      <c r="AE12" s="90"/>
-      <c r="AF12" s="90"/>
-      <c r="AG12" s="90"/>
-      <c r="AH12" s="90"/>
-      <c r="AI12" s="90"/>
-      <c r="AJ12" s="90"/>
-      <c r="AK12" s="91"/>
-      <c r="AL12" s="91"/>
-      <c r="AM12" s="91"/>
-      <c r="AN12" s="91"/>
-      <c r="AO12" s="91"/>
-      <c r="AP12" s="91"/>
-      <c r="AQ12" s="91"/>
-      <c r="AR12" s="91"/>
-      <c r="AS12" s="89" t="s">
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="98"/>
+      <c r="AC12" s="98"/>
+      <c r="AD12" s="98"/>
+      <c r="AE12" s="98"/>
+      <c r="AF12" s="98"/>
+      <c r="AG12" s="98"/>
+      <c r="AH12" s="98"/>
+      <c r="AI12" s="98"/>
+      <c r="AJ12" s="98"/>
+      <c r="AK12" s="99"/>
+      <c r="AL12" s="99"/>
+      <c r="AM12" s="99"/>
+      <c r="AN12" s="99"/>
+      <c r="AO12" s="99"/>
+      <c r="AP12" s="99"/>
+      <c r="AQ12" s="99"/>
+      <c r="AR12" s="99"/>
+      <c r="AS12" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="AT12" s="91"/>
-      <c r="AU12" s="91"/>
-      <c r="AV12" s="91"/>
-      <c r="AW12" s="91"/>
-      <c r="AX12" s="91"/>
-      <c r="AY12" s="91"/>
-      <c r="AZ12" s="91"/>
+      <c r="AT12" s="99"/>
+      <c r="AU12" s="99"/>
+      <c r="AV12" s="99"/>
+      <c r="AW12" s="99"/>
+      <c r="AX12" s="99"/>
+      <c r="AY12" s="99"/>
+      <c r="AZ12" s="99"/>
     </row>
     <row r="13" spans="1:61" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
-      <c r="X13" s="78"/>
-      <c r="Y13" s="78"/>
-      <c r="Z13" s="78"/>
-      <c r="AA13" s="78"/>
-      <c r="AB13" s="78"/>
-      <c r="AC13" s="78"/>
-      <c r="AD13" s="78"/>
-      <c r="AE13" s="78"/>
-      <c r="AF13" s="78"/>
-      <c r="AG13" s="78"/>
-      <c r="AH13" s="78"/>
-      <c r="AI13" s="78"/>
-      <c r="AJ13" s="78"/>
-      <c r="AK13" s="93"/>
-      <c r="AL13" s="93"/>
-      <c r="AM13" s="93"/>
-      <c r="AN13" s="93"/>
-      <c r="AO13" s="93"/>
-      <c r="AP13" s="93"/>
-      <c r="AQ13" s="93"/>
-      <c r="AR13" s="93"/>
-      <c r="AS13" s="94"/>
-      <c r="AT13" s="93"/>
-      <c r="AU13" s="93"/>
-      <c r="AV13" s="93"/>
-      <c r="AW13" s="93"/>
-      <c r="AX13" s="93"/>
-      <c r="AY13" s="93"/>
-      <c r="AZ13" s="93"/>
+      <c r="A13" s="95"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="86"/>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="86"/>
+      <c r="Z13" s="86"/>
+      <c r="AA13" s="86"/>
+      <c r="AB13" s="86"/>
+      <c r="AC13" s="86"/>
+      <c r="AD13" s="86"/>
+      <c r="AE13" s="86"/>
+      <c r="AF13" s="86"/>
+      <c r="AG13" s="86"/>
+      <c r="AH13" s="86"/>
+      <c r="AI13" s="86"/>
+      <c r="AJ13" s="86"/>
+      <c r="AK13" s="101"/>
+      <c r="AL13" s="101"/>
+      <c r="AM13" s="101"/>
+      <c r="AN13" s="101"/>
+      <c r="AO13" s="101"/>
+      <c r="AP13" s="101"/>
+      <c r="AQ13" s="101"/>
+      <c r="AR13" s="101"/>
+      <c r="AS13" s="102"/>
+      <c r="AT13" s="101"/>
+      <c r="AU13" s="101"/>
+      <c r="AV13" s="101"/>
+      <c r="AW13" s="101"/>
+      <c r="AX13" s="101"/>
+      <c r="AY13" s="101"/>
+      <c r="AZ13" s="101"/>
     </row>
     <row r="14" spans="1:61" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
@@ -3670,9 +3667,9 @@
     </row>
     <row r="15" spans="1:61" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="25"/>
       <c r="F15" s="26"/>
       <c r="G15" s="27" t="str">
@@ -3717,12 +3714,12 @@
       <c r="AQ15" s="30"/>
       <c r="AR15" s="31"/>
       <c r="AS15" s="32"/>
-      <c r="AT15" s="76"/>
-      <c r="AU15" s="77"/>
-      <c r="AV15" s="77"/>
-      <c r="AW15" s="77"/>
-      <c r="AX15" s="77"/>
-      <c r="AY15" s="77"/>
+      <c r="AT15" s="78"/>
+      <c r="AU15" s="79"/>
+      <c r="AV15" s="79"/>
+      <c r="AW15" s="79"/>
+      <c r="AX15" s="79"/>
+      <c r="AY15" s="79"/>
       <c r="AZ15" s="33"/>
       <c r="BA15" s="34" t="str">
         <f>IF(ISBLANK(B15),"",VLOOKUP(B15,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3753,9 +3750,9 @@
     </row>
     <row r="16" spans="1:61" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
       <c r="G16" s="27" t="str">
@@ -3800,12 +3797,12 @@
       <c r="AQ16" s="27"/>
       <c r="AR16" s="58"/>
       <c r="AS16" s="39"/>
-      <c r="AT16" s="76"/>
-      <c r="AU16" s="77"/>
-      <c r="AV16" s="77"/>
-      <c r="AW16" s="77"/>
-      <c r="AX16" s="77"/>
-      <c r="AY16" s="77"/>
+      <c r="AT16" s="78"/>
+      <c r="AU16" s="79"/>
+      <c r="AV16" s="79"/>
+      <c r="AW16" s="79"/>
+      <c r="AX16" s="79"/>
+      <c r="AY16" s="79"/>
       <c r="AZ16" s="33"/>
       <c r="BA16" s="34" t="str">
         <f>IF(ISBLANK(B16),"",VLOOKUP(B16,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3836,9 +3833,9 @@
     </row>
     <row r="17" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
       <c r="G17" s="27" t="str">
@@ -3883,12 +3880,12 @@
       <c r="AQ17" s="27"/>
       <c r="AR17" s="58"/>
       <c r="AS17" s="32"/>
-      <c r="AT17" s="76"/>
-      <c r="AU17" s="77"/>
-      <c r="AV17" s="77"/>
-      <c r="AW17" s="77"/>
-      <c r="AX17" s="77"/>
-      <c r="AY17" s="77"/>
+      <c r="AT17" s="78"/>
+      <c r="AU17" s="79"/>
+      <c r="AV17" s="79"/>
+      <c r="AW17" s="79"/>
+      <c r="AX17" s="79"/>
+      <c r="AY17" s="79"/>
       <c r="AZ17" s="33"/>
       <c r="BA17" s="34" t="str">
         <f>IF(ISBLANK(B17),"",VLOOKUP(B17,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -3919,9 +3916,9 @@
     </row>
     <row r="18" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
       <c r="G18" s="27" t="str">
@@ -3966,12 +3963,12 @@
       <c r="AQ18" s="27"/>
       <c r="AR18" s="58"/>
       <c r="AS18" s="39"/>
-      <c r="AT18" s="76"/>
-      <c r="AU18" s="77"/>
-      <c r="AV18" s="77"/>
-      <c r="AW18" s="77"/>
-      <c r="AX18" s="77"/>
-      <c r="AY18" s="77"/>
+      <c r="AT18" s="78"/>
+      <c r="AU18" s="79"/>
+      <c r="AV18" s="79"/>
+      <c r="AW18" s="79"/>
+      <c r="AX18" s="79"/>
+      <c r="AY18" s="79"/>
       <c r="AZ18" s="33"/>
       <c r="BA18" s="34" t="str">
         <f>IF(ISBLANK(B18),"",VLOOKUP(B18,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4005,9 +4002,9 @@
     </row>
     <row r="19" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
       <c r="G19" s="27" t="str">
@@ -4052,12 +4049,12 @@
       <c r="AQ19" s="27"/>
       <c r="AR19" s="58"/>
       <c r="AS19" s="32"/>
-      <c r="AT19" s="76"/>
-      <c r="AU19" s="77"/>
-      <c r="AV19" s="77"/>
-      <c r="AW19" s="77"/>
-      <c r="AX19" s="77"/>
-      <c r="AY19" s="77"/>
+      <c r="AT19" s="78"/>
+      <c r="AU19" s="79"/>
+      <c r="AV19" s="79"/>
+      <c r="AW19" s="79"/>
+      <c r="AX19" s="79"/>
+      <c r="AY19" s="79"/>
       <c r="AZ19" s="33"/>
       <c r="BA19" s="34" t="str">
         <f>IF(ISBLANK(B19),"",VLOOKUP(B19,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4088,9 +4085,9 @@
     </row>
     <row r="20" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
       <c r="G20" s="27" t="str">
@@ -4135,12 +4132,12 @@
       <c r="AQ20" s="27"/>
       <c r="AR20" s="58"/>
       <c r="AS20" s="39"/>
-      <c r="AT20" s="76"/>
-      <c r="AU20" s="77"/>
-      <c r="AV20" s="77"/>
-      <c r="AW20" s="77"/>
-      <c r="AX20" s="77"/>
-      <c r="AY20" s="77"/>
+      <c r="AT20" s="78"/>
+      <c r="AU20" s="79"/>
+      <c r="AV20" s="79"/>
+      <c r="AW20" s="79"/>
+      <c r="AX20" s="79"/>
+      <c r="AY20" s="79"/>
       <c r="AZ20" s="33"/>
       <c r="BA20" s="34" t="str">
         <f>IF(ISBLANK(B20),"",VLOOKUP(B20,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4162,9 +4159,9 @@
     </row>
     <row r="21" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
       <c r="G21" s="27" t="str">
@@ -4209,12 +4206,12 @@
       <c r="AQ21" s="27"/>
       <c r="AR21" s="58"/>
       <c r="AS21" s="32"/>
-      <c r="AT21" s="76"/>
-      <c r="AU21" s="77"/>
-      <c r="AV21" s="77"/>
-      <c r="AW21" s="77"/>
-      <c r="AX21" s="77"/>
-      <c r="AY21" s="77"/>
+      <c r="AT21" s="78"/>
+      <c r="AU21" s="79"/>
+      <c r="AV21" s="79"/>
+      <c r="AW21" s="79"/>
+      <c r="AX21" s="79"/>
+      <c r="AY21" s="79"/>
       <c r="AZ21" s="33"/>
       <c r="BA21" s="34" t="str">
         <f>IF(ISBLANK(B21),"",VLOOKUP(B21,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4233,9 +4230,9 @@
     </row>
     <row r="22" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
       <c r="E22" s="25"/>
       <c r="F22" s="26"/>
       <c r="G22" s="27" t="str">
@@ -4282,12 +4279,12 @@
       <c r="AQ22" s="27"/>
       <c r="AR22" s="58"/>
       <c r="AS22" s="39"/>
-      <c r="AT22" s="76"/>
-      <c r="AU22" s="77"/>
-      <c r="AV22" s="77"/>
-      <c r="AW22" s="77"/>
-      <c r="AX22" s="77"/>
-      <c r="AY22" s="77"/>
+      <c r="AT22" s="78"/>
+      <c r="AU22" s="79"/>
+      <c r="AV22" s="79"/>
+      <c r="AW22" s="79"/>
+      <c r="AX22" s="79"/>
+      <c r="AY22" s="79"/>
       <c r="AZ22" s="33"/>
       <c r="BA22" s="34" t="str">
         <f>IF(ISBLANK(B22),"",VLOOKUP(B22,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4304,9 +4301,9 @@
     </row>
     <row r="23" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="27" t="str">
@@ -4353,12 +4350,12 @@
       <c r="AQ23" s="27"/>
       <c r="AR23" s="40"/>
       <c r="AS23" s="32"/>
-      <c r="AT23" s="76"/>
-      <c r="AU23" s="77"/>
-      <c r="AV23" s="77"/>
-      <c r="AW23" s="77"/>
-      <c r="AX23" s="77"/>
-      <c r="AY23" s="77"/>
+      <c r="AT23" s="78"/>
+      <c r="AU23" s="79"/>
+      <c r="AV23" s="79"/>
+      <c r="AW23" s="79"/>
+      <c r="AX23" s="79"/>
+      <c r="AY23" s="79"/>
       <c r="AZ23" s="33"/>
       <c r="BA23" s="34" t="str">
         <f>IF(ISBLANK(B23),"",VLOOKUP(B23,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4376,9 +4373,9 @@
     </row>
     <row r="24" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
       <c r="G24" s="27" t="str">
@@ -4425,12 +4422,12 @@
       <c r="AQ24" s="30"/>
       <c r="AR24" s="40"/>
       <c r="AS24" s="39"/>
-      <c r="AT24" s="76"/>
-      <c r="AU24" s="77"/>
-      <c r="AV24" s="77"/>
-      <c r="AW24" s="77"/>
-      <c r="AX24" s="77"/>
-      <c r="AY24" s="77"/>
+      <c r="AT24" s="78"/>
+      <c r="AU24" s="79"/>
+      <c r="AV24" s="79"/>
+      <c r="AW24" s="79"/>
+      <c r="AX24" s="79"/>
+      <c r="AY24" s="79"/>
       <c r="AZ24" s="33"/>
       <c r="BA24" s="34" t="str">
         <f>IF(ISBLANK(B24),"",VLOOKUP(B24,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4447,9 +4444,9 @@
     </row>
     <row r="25" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
       <c r="G25" s="27" t="str">
@@ -4496,12 +4493,12 @@
       <c r="AQ25" s="30"/>
       <c r="AR25" s="40"/>
       <c r="AS25" s="39"/>
-      <c r="AT25" s="76"/>
-      <c r="AU25" s="77"/>
-      <c r="AV25" s="77"/>
-      <c r="AW25" s="77"/>
-      <c r="AX25" s="77"/>
-      <c r="AY25" s="77"/>
+      <c r="AT25" s="78"/>
+      <c r="AU25" s="79"/>
+      <c r="AV25" s="79"/>
+      <c r="AW25" s="79"/>
+      <c r="AX25" s="79"/>
+      <c r="AY25" s="79"/>
       <c r="AZ25" s="33"/>
       <c r="BA25" s="34" t="str">
         <f>IF(ISBLANK(B25),"",VLOOKUP(B25,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4518,9 +4515,9 @@
     </row>
     <row r="26" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
       <c r="G26" s="27" t="str">
@@ -4567,12 +4564,12 @@
       <c r="AQ26" s="30"/>
       <c r="AR26" s="40"/>
       <c r="AS26" s="39"/>
-      <c r="AT26" s="76"/>
-      <c r="AU26" s="77"/>
-      <c r="AV26" s="77"/>
-      <c r="AW26" s="77"/>
-      <c r="AX26" s="77"/>
-      <c r="AY26" s="77"/>
+      <c r="AT26" s="78"/>
+      <c r="AU26" s="79"/>
+      <c r="AV26" s="79"/>
+      <c r="AW26" s="79"/>
+      <c r="AX26" s="79"/>
+      <c r="AY26" s="79"/>
       <c r="AZ26" s="33"/>
       <c r="BA26" s="34" t="str">
         <f>IF(ISBLANK(B26),"",VLOOKUP(B26,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4589,9 +4586,9 @@
     </row>
     <row r="27" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
       <c r="E27" s="25"/>
       <c r="F27" s="26"/>
       <c r="G27" s="27" t="str">
@@ -4636,12 +4633,12 @@
       <c r="AQ27" s="27"/>
       <c r="AR27" s="58"/>
       <c r="AS27" s="39"/>
-      <c r="AT27" s="76"/>
-      <c r="AU27" s="77"/>
-      <c r="AV27" s="77"/>
-      <c r="AW27" s="77"/>
-      <c r="AX27" s="77"/>
-      <c r="AY27" s="77"/>
+      <c r="AT27" s="78"/>
+      <c r="AU27" s="79"/>
+      <c r="AV27" s="79"/>
+      <c r="AW27" s="79"/>
+      <c r="AX27" s="79"/>
+      <c r="AY27" s="79"/>
       <c r="AZ27" s="33"/>
       <c r="BA27" s="34" t="str">
         <f>IF(ISBLANK(B27),"",VLOOKUP(B27,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4658,9 +4655,9 @@
     </row>
     <row r="28" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
       <c r="E28" s="25"/>
       <c r="F28" s="26"/>
       <c r="G28" s="27" t="str">
@@ -4707,12 +4704,12 @@
       <c r="AQ28" s="30"/>
       <c r="AR28" s="40"/>
       <c r="AS28" s="39"/>
-      <c r="AT28" s="76"/>
-      <c r="AU28" s="77"/>
-      <c r="AV28" s="77"/>
-      <c r="AW28" s="77"/>
-      <c r="AX28" s="77"/>
-      <c r="AY28" s="77"/>
+      <c r="AT28" s="78"/>
+      <c r="AU28" s="79"/>
+      <c r="AV28" s="79"/>
+      <c r="AW28" s="79"/>
+      <c r="AX28" s="79"/>
+      <c r="AY28" s="79"/>
       <c r="AZ28" s="33"/>
       <c r="BA28" s="34" t="str">
         <f>IF(ISBLANK(B28),"",VLOOKUP(B28,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4729,9 +4726,9 @@
     </row>
     <row r="29" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
       <c r="E29" s="25"/>
       <c r="F29" s="26"/>
       <c r="G29" s="27" t="str">
@@ -4778,12 +4775,12 @@
       <c r="AQ29" s="30"/>
       <c r="AR29" s="40"/>
       <c r="AS29" s="39"/>
-      <c r="AT29" s="76"/>
-      <c r="AU29" s="77"/>
-      <c r="AV29" s="77"/>
-      <c r="AW29" s="77"/>
-      <c r="AX29" s="77"/>
-      <c r="AY29" s="77"/>
+      <c r="AT29" s="78"/>
+      <c r="AU29" s="79"/>
+      <c r="AV29" s="79"/>
+      <c r="AW29" s="79"/>
+      <c r="AX29" s="79"/>
+      <c r="AY29" s="79"/>
       <c r="AZ29" s="33"/>
       <c r="BA29" s="34" t="str">
         <f>IF(ISBLANK(B29),"",VLOOKUP(B29,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4800,9 +4797,9 @@
     </row>
     <row r="30" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="str">
@@ -4849,12 +4846,12 @@
       <c r="AQ30" s="30"/>
       <c r="AR30" s="40"/>
       <c r="AS30" s="39"/>
-      <c r="AT30" s="76"/>
-      <c r="AU30" s="77"/>
-      <c r="AV30" s="77"/>
-      <c r="AW30" s="77"/>
-      <c r="AX30" s="77"/>
-      <c r="AY30" s="77"/>
+      <c r="AT30" s="78"/>
+      <c r="AU30" s="79"/>
+      <c r="AV30" s="79"/>
+      <c r="AW30" s="79"/>
+      <c r="AX30" s="79"/>
+      <c r="AY30" s="79"/>
       <c r="AZ30" s="33"/>
       <c r="BA30" s="34" t="str">
         <f>IF(ISBLANK(B30),"",VLOOKUP(B30,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4871,9 +4868,9 @@
     </row>
     <row r="31" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="str">
@@ -4920,12 +4917,12 @@
       <c r="AQ31" s="30"/>
       <c r="AR31" s="40"/>
       <c r="AS31" s="39"/>
-      <c r="AT31" s="76"/>
-      <c r="AU31" s="77"/>
-      <c r="AV31" s="77"/>
-      <c r="AW31" s="77"/>
-      <c r="AX31" s="77"/>
-      <c r="AY31" s="77"/>
+      <c r="AT31" s="78"/>
+      <c r="AU31" s="79"/>
+      <c r="AV31" s="79"/>
+      <c r="AW31" s="79"/>
+      <c r="AX31" s="79"/>
+      <c r="AY31" s="79"/>
       <c r="AZ31" s="33"/>
       <c r="BA31" s="34" t="str">
         <f>IF(ISBLANK(B31),"",VLOOKUP(B31,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -4945,9 +4942,9 @@
     </row>
     <row r="32" spans="1:84" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="21"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
       <c r="G32" s="27" t="str">
@@ -4994,12 +4991,12 @@
       <c r="AQ32" s="30"/>
       <c r="AR32" s="40"/>
       <c r="AS32" s="39"/>
-      <c r="AT32" s="76"/>
-      <c r="AU32" s="77"/>
-      <c r="AV32" s="77"/>
-      <c r="AW32" s="77"/>
-      <c r="AX32" s="77"/>
-      <c r="AY32" s="77"/>
+      <c r="AT32" s="78"/>
+      <c r="AU32" s="79"/>
+      <c r="AV32" s="79"/>
+      <c r="AW32" s="79"/>
+      <c r="AX32" s="79"/>
+      <c r="AY32" s="79"/>
       <c r="AZ32" s="33"/>
       <c r="BA32" s="34" t="str">
         <f>IF(ISBLANK(B32),"",VLOOKUP(B32,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5016,9 +5013,9 @@
     </row>
     <row r="33" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="27" t="str">
@@ -5065,12 +5062,12 @@
       <c r="AQ33" s="30"/>
       <c r="AR33" s="40"/>
       <c r="AS33" s="39"/>
-      <c r="AT33" s="76"/>
-      <c r="AU33" s="77"/>
-      <c r="AV33" s="77"/>
-      <c r="AW33" s="77"/>
-      <c r="AX33" s="77"/>
-      <c r="AY33" s="77"/>
+      <c r="AT33" s="78"/>
+      <c r="AU33" s="79"/>
+      <c r="AV33" s="79"/>
+      <c r="AW33" s="79"/>
+      <c r="AX33" s="79"/>
+      <c r="AY33" s="79"/>
       <c r="AZ33" s="33"/>
       <c r="BA33" s="34" t="str">
         <f>IF(ISBLANK(B33),"",VLOOKUP(B33,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5087,9 +5084,9 @@
     </row>
     <row r="34" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
       <c r="G34" s="27" t="str">
@@ -5136,12 +5133,12 @@
       <c r="AQ34" s="30"/>
       <c r="AR34" s="40"/>
       <c r="AS34" s="39"/>
-      <c r="AT34" s="76"/>
-      <c r="AU34" s="77"/>
-      <c r="AV34" s="77"/>
-      <c r="AW34" s="77"/>
-      <c r="AX34" s="77"/>
-      <c r="AY34" s="77"/>
+      <c r="AT34" s="78"/>
+      <c r="AU34" s="79"/>
+      <c r="AV34" s="79"/>
+      <c r="AW34" s="79"/>
+      <c r="AX34" s="79"/>
+      <c r="AY34" s="79"/>
       <c r="AZ34" s="33"/>
       <c r="BA34" s="34" t="str">
         <f>IF(ISBLANK(B34),"",VLOOKUP(B34,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5158,9 +5155,9 @@
     </row>
     <row r="35" spans="1:58" s="20" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
       <c r="G35" s="27" t="str">
@@ -5207,12 +5204,12 @@
       <c r="AQ35" s="30"/>
       <c r="AR35" s="40"/>
       <c r="AS35" s="39"/>
-      <c r="AT35" s="76"/>
-      <c r="AU35" s="77"/>
-      <c r="AV35" s="77"/>
-      <c r="AW35" s="77"/>
-      <c r="AX35" s="77"/>
-      <c r="AY35" s="77"/>
+      <c r="AT35" s="78"/>
+      <c r="AU35" s="79"/>
+      <c r="AV35" s="79"/>
+      <c r="AW35" s="79"/>
+      <c r="AX35" s="79"/>
+      <c r="AY35" s="79"/>
       <c r="AZ35" s="33"/>
       <c r="BA35" s="34" t="str">
         <f>IF(ISBLANK(B35),"",VLOOKUP(B35,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5229,58 +5226,58 @@
     </row>
     <row r="36" spans="1:58" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="96"/>
-      <c r="J36" s="96"/>
-      <c r="K36" s="96"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="96"/>
-      <c r="N36" s="96"/>
-      <c r="O36" s="96"/>
-      <c r="P36" s="96"/>
-      <c r="Q36" s="96"/>
-      <c r="R36" s="96"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="96"/>
-      <c r="U36" s="96"/>
-      <c r="V36" s="96"/>
-      <c r="W36" s="96"/>
-      <c r="X36" s="96"/>
-      <c r="Y36" s="96"/>
-      <c r="Z36" s="96"/>
-      <c r="AA36" s="96"/>
-      <c r="AB36" s="96"/>
-      <c r="AC36" s="96"/>
-      <c r="AD36" s="96"/>
-      <c r="AE36" s="96"/>
-      <c r="AF36" s="96"/>
-      <c r="AG36" s="96"/>
-      <c r="AH36" s="96"/>
-      <c r="AI36" s="96"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="81"/>
+      <c r="N36" s="81"/>
+      <c r="O36" s="81"/>
+      <c r="P36" s="81"/>
+      <c r="Q36" s="81"/>
+      <c r="R36" s="81"/>
+      <c r="S36" s="81"/>
+      <c r="T36" s="81"/>
+      <c r="U36" s="81"/>
+      <c r="V36" s="81"/>
+      <c r="W36" s="81"/>
+      <c r="X36" s="81"/>
+      <c r="Y36" s="81"/>
+      <c r="Z36" s="81"/>
+      <c r="AA36" s="81"/>
+      <c r="AB36" s="81"/>
+      <c r="AC36" s="81"/>
+      <c r="AD36" s="81"/>
+      <c r="AE36" s="81"/>
+      <c r="AF36" s="81"/>
+      <c r="AG36" s="81"/>
+      <c r="AH36" s="81"/>
+      <c r="AI36" s="81"/>
       <c r="AJ36" s="26"/>
       <c r="AK36" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AL36" s="97"/>
-      <c r="AM36" s="98"/>
-      <c r="AN36" s="98"/>
-      <c r="AO36" s="98"/>
-      <c r="AP36" s="98"/>
-      <c r="AQ36" s="98"/>
+      <c r="AL36" s="82"/>
+      <c r="AM36" s="83"/>
+      <c r="AN36" s="83"/>
+      <c r="AO36" s="83"/>
+      <c r="AP36" s="83"/>
+      <c r="AQ36" s="83"/>
       <c r="AR36" s="25"/>
       <c r="AS36" s="39"/>
-      <c r="AT36" s="99"/>
-      <c r="AU36" s="100"/>
-      <c r="AV36" s="100"/>
-      <c r="AW36" s="100"/>
-      <c r="AX36" s="100"/>
-      <c r="AY36" s="100"/>
+      <c r="AT36" s="84"/>
+      <c r="AU36" s="85"/>
+      <c r="AV36" s="85"/>
+      <c r="AW36" s="85"/>
+      <c r="AX36" s="85"/>
+      <c r="AY36" s="85"/>
       <c r="AZ36" s="33"/>
       <c r="BA36" s="34" t="str">
         <f>IF(ISBLANK(B36),"",VLOOKUP(B36,'[1]CLAVES INGRESOS'!$A$1:$C$65536,3,0))</f>
@@ -5399,17 +5396,17 @@
         <v>10</v>
       </c>
       <c r="AR38" s="1"/>
-      <c r="AS38" s="107">
+      <c r="AS38" s="65">
         <f>SUM(AT15:AY35)</f>
         <v>0</v>
       </c>
-      <c r="AT38" s="108"/>
-      <c r="AU38" s="108"/>
-      <c r="AV38" s="108"/>
-      <c r="AW38" s="108"/>
-      <c r="AX38" s="108"/>
-      <c r="AY38" s="108"/>
-      <c r="AZ38" s="108"/>
+      <c r="AT38" s="66"/>
+      <c r="AU38" s="66"/>
+      <c r="AV38" s="66"/>
+      <c r="AW38" s="66"/>
+      <c r="AX38" s="66"/>
+      <c r="AY38" s="66"/>
+      <c r="AZ38" s="66"/>
       <c r="BA38" s="24"/>
     </row>
     <row r="39" spans="1:58" s="20" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5468,58 +5465,58 @@
       <c r="BA39" s="24"/>
     </row>
     <row r="40" spans="1:58" s="20" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="109"/>
-      <c r="B40" s="109"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="109"/>
-      <c r="F40" s="109"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
-      <c r="I40" s="109"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="111"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="111"/>
-      <c r="R40" s="111"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="111"/>
-      <c r="W40" s="111"/>
-      <c r="X40" s="111"/>
-      <c r="Y40" s="111"/>
-      <c r="Z40" s="111"/>
-      <c r="AA40" s="111"/>
-      <c r="AB40" s="111"/>
-      <c r="AC40" s="111"/>
-      <c r="AD40" s="111"/>
-      <c r="AE40" s="111"/>
-      <c r="AF40" s="111"/>
-      <c r="AG40" s="111"/>
-      <c r="AH40" s="111"/>
-      <c r="AI40" s="111"/>
-      <c r="AJ40" s="111"/>
-      <c r="AK40" s="111"/>
-      <c r="AL40" s="111"/>
-      <c r="AM40" s="111"/>
-      <c r="AN40" s="111"/>
-      <c r="AO40" s="111"/>
-      <c r="AP40" s="111"/>
-      <c r="AQ40" s="111"/>
-      <c r="AR40" s="111"/>
-      <c r="AS40" s="111"/>
-      <c r="AT40" s="111"/>
-      <c r="AU40" s="111"/>
-      <c r="AV40" s="111"/>
-      <c r="AW40" s="111"/>
-      <c r="AX40" s="111"/>
-      <c r="AY40" s="111"/>
-      <c r="AZ40" s="111"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="69"/>
+      <c r="V40" s="69"/>
+      <c r="W40" s="69"/>
+      <c r="X40" s="69"/>
+      <c r="Y40" s="69"/>
+      <c r="Z40" s="69"/>
+      <c r="AA40" s="69"/>
+      <c r="AB40" s="69"/>
+      <c r="AC40" s="69"/>
+      <c r="AD40" s="69"/>
+      <c r="AE40" s="69"/>
+      <c r="AF40" s="69"/>
+      <c r="AG40" s="69"/>
+      <c r="AH40" s="69"/>
+      <c r="AI40" s="69"/>
+      <c r="AJ40" s="69"/>
+      <c r="AK40" s="69"/>
+      <c r="AL40" s="69"/>
+      <c r="AM40" s="69"/>
+      <c r="AN40" s="69"/>
+      <c r="AO40" s="69"/>
+      <c r="AP40" s="69"/>
+      <c r="AQ40" s="69"/>
+      <c r="AR40" s="69"/>
+      <c r="AS40" s="69"/>
+      <c r="AT40" s="69"/>
+      <c r="AU40" s="69"/>
+      <c r="AV40" s="69"/>
+      <c r="AW40" s="69"/>
+      <c r="AX40" s="69"/>
+      <c r="AY40" s="69"/>
+      <c r="AZ40" s="69"/>
       <c r="BA40" s="24"/>
     </row>
     <row r="41" spans="1:58" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.3">
@@ -5549,22 +5546,22 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="112"/>
-      <c r="AB41" s="112"/>
-      <c r="AC41" s="112"/>
-      <c r="AD41" s="112"/>
-      <c r="AE41" s="112"/>
-      <c r="AF41" s="112"/>
-      <c r="AG41" s="112"/>
-      <c r="AH41" s="112"/>
-      <c r="AI41" s="112"/>
-      <c r="AJ41" s="112"/>
-      <c r="AK41" s="112"/>
-      <c r="AL41" s="112"/>
-      <c r="AM41" s="112"/>
-      <c r="AN41" s="112"/>
-      <c r="AO41" s="112"/>
-      <c r="AP41" s="112"/>
+      <c r="AA41" s="70"/>
+      <c r="AB41" s="70"/>
+      <c r="AC41" s="70"/>
+      <c r="AD41" s="70"/>
+      <c r="AE41" s="70"/>
+      <c r="AF41" s="70"/>
+      <c r="AG41" s="70"/>
+      <c r="AH41" s="70"/>
+      <c r="AI41" s="70"/>
+      <c r="AJ41" s="70"/>
+      <c r="AK41" s="70"/>
+      <c r="AL41" s="70"/>
+      <c r="AM41" s="70"/>
+      <c r="AN41" s="70"/>
+      <c r="AO41" s="70"/>
+      <c r="AP41" s="70"/>
       <c r="AQ41" s="1"/>
       <c r="AR41" s="48"/>
       <c r="AS41" s="1"/>
@@ -5579,196 +5576,133 @@
       <c r="BB41" s="51"/>
     </row>
     <row r="42" spans="1:58" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="113"/>
-      <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="113"/>
-      <c r="G42" s="113"/>
-      <c r="H42" s="113"/>
-      <c r="I42" s="113"/>
-      <c r="J42" s="113"/>
-      <c r="K42" s="113"/>
-      <c r="L42" s="113"/>
-      <c r="M42" s="113"/>
-      <c r="N42" s="113"/>
-      <c r="O42" s="113"/>
-      <c r="P42" s="113"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="115" t="s">
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+      <c r="P42" s="71"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="S42" s="113"/>
-      <c r="T42" s="113"/>
-      <c r="U42" s="113"/>
-      <c r="V42" s="113"/>
-      <c r="W42" s="113"/>
-      <c r="X42" s="113"/>
-      <c r="Y42" s="113"/>
-      <c r="Z42" s="113"/>
-      <c r="AA42" s="113"/>
-      <c r="AB42" s="113"/>
-      <c r="AC42" s="113"/>
-      <c r="AD42" s="113"/>
-      <c r="AE42" s="113"/>
-      <c r="AF42" s="113"/>
-      <c r="AG42" s="113"/>
-      <c r="AH42" s="113"/>
-      <c r="AI42" s="113"/>
-      <c r="AJ42" s="113"/>
-      <c r="AK42" s="113"/>
-      <c r="AL42" s="114"/>
-      <c r="AM42" s="116" t="s">
+      <c r="S42" s="71"/>
+      <c r="T42" s="71"/>
+      <c r="U42" s="71"/>
+      <c r="V42" s="71"/>
+      <c r="W42" s="71"/>
+      <c r="X42" s="71"/>
+      <c r="Y42" s="71"/>
+      <c r="Z42" s="71"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="71"/>
+      <c r="AC42" s="71"/>
+      <c r="AD42" s="71"/>
+      <c r="AE42" s="71"/>
+      <c r="AF42" s="71"/>
+      <c r="AG42" s="71"/>
+      <c r="AH42" s="71"/>
+      <c r="AI42" s="71"/>
+      <c r="AJ42" s="71"/>
+      <c r="AK42" s="71"/>
+      <c r="AL42" s="72"/>
+      <c r="AM42" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="AN42" s="117"/>
-      <c r="AO42" s="117"/>
-      <c r="AP42" s="117"/>
-      <c r="AQ42" s="117"/>
-      <c r="AR42" s="117"/>
-      <c r="AS42" s="117"/>
-      <c r="AT42" s="117"/>
-      <c r="AU42" s="117"/>
-      <c r="AV42" s="117"/>
-      <c r="AW42" s="117"/>
-      <c r="AX42" s="117"/>
-      <c r="AY42" s="117"/>
-      <c r="AZ42" s="117"/>
-      <c r="BA42" s="117"/>
-      <c r="BB42" s="117"/>
-      <c r="BC42" s="118"/>
+      <c r="AN42" s="75"/>
+      <c r="AO42" s="75"/>
+      <c r="AP42" s="75"/>
+      <c r="AQ42" s="75"/>
+      <c r="AR42" s="75"/>
+      <c r="AS42" s="75"/>
+      <c r="AT42" s="75"/>
+      <c r="AU42" s="75"/>
+      <c r="AV42" s="75"/>
+      <c r="AW42" s="75"/>
+      <c r="AX42" s="75"/>
+      <c r="AY42" s="75"/>
+      <c r="AZ42" s="75"/>
+      <c r="BA42" s="75"/>
+      <c r="BB42" s="75"/>
+      <c r="BC42" s="76"/>
     </row>
     <row r="43" spans="1:58" s="20" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="101" t="s">
+      <c r="A43" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="102"/>
-      <c r="C43" s="102"/>
-      <c r="D43" s="102"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="102"/>
-      <c r="G43" s="102"/>
-      <c r="H43" s="102"/>
-      <c r="I43" s="102"/>
-      <c r="J43" s="102"/>
-      <c r="K43" s="102"/>
-      <c r="L43" s="102"/>
-      <c r="M43" s="102"/>
-      <c r="N43" s="102"/>
-      <c r="O43" s="102"/>
-      <c r="P43" s="102"/>
-      <c r="Q43" s="103"/>
-      <c r="R43" s="104" t="s">
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="60"/>
+      <c r="Q43" s="61"/>
+      <c r="R43" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="S43" s="102"/>
-      <c r="T43" s="102"/>
-      <c r="U43" s="102"/>
-      <c r="V43" s="102"/>
-      <c r="W43" s="102"/>
-      <c r="X43" s="102"/>
-      <c r="Y43" s="102"/>
-      <c r="Z43" s="102"/>
-      <c r="AA43" s="102"/>
-      <c r="AB43" s="102"/>
-      <c r="AC43" s="102"/>
-      <c r="AD43" s="102"/>
-      <c r="AE43" s="102"/>
-      <c r="AF43" s="102"/>
-      <c r="AG43" s="102"/>
-      <c r="AH43" s="102"/>
-      <c r="AI43" s="105"/>
-      <c r="AJ43" s="105"/>
-      <c r="AK43" s="105"/>
-      <c r="AL43" s="106"/>
-      <c r="AM43" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN43" s="102"/>
-      <c r="AO43" s="102"/>
-      <c r="AP43" s="102"/>
-      <c r="AQ43" s="102"/>
-      <c r="AR43" s="102"/>
-      <c r="AS43" s="102"/>
-      <c r="AT43" s="102"/>
-      <c r="AU43" s="102"/>
-      <c r="AV43" s="102"/>
-      <c r="AW43" s="102"/>
-      <c r="AX43" s="102"/>
-      <c r="AY43" s="102"/>
-      <c r="AZ43" s="102"/>
-      <c r="BA43" s="102"/>
-      <c r="BB43" s="102"/>
-      <c r="BC43" s="103"/>
+      <c r="S43" s="60"/>
+      <c r="T43" s="60"/>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="60"/>
+      <c r="Y43" s="60"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="60"/>
+      <c r="AB43" s="60"/>
+      <c r="AC43" s="60"/>
+      <c r="AD43" s="60"/>
+      <c r="AE43" s="60"/>
+      <c r="AF43" s="60"/>
+      <c r="AG43" s="60"/>
+      <c r="AH43" s="60"/>
+      <c r="AI43" s="63"/>
+      <c r="AJ43" s="63"/>
+      <c r="AK43" s="63"/>
+      <c r="AL43" s="64"/>
+      <c r="AM43" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN43" s="60"/>
+      <c r="AO43" s="60"/>
+      <c r="AP43" s="60"/>
+      <c r="AQ43" s="60"/>
+      <c r="AR43" s="60"/>
+      <c r="AS43" s="60"/>
+      <c r="AT43" s="60"/>
+      <c r="AU43" s="60"/>
+      <c r="AV43" s="60"/>
+      <c r="AW43" s="60"/>
+      <c r="AX43" s="60"/>
+      <c r="AY43" s="60"/>
+      <c r="AZ43" s="60"/>
+      <c r="BA43" s="60"/>
+      <c r="BB43" s="60"/>
+      <c r="BC43" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A43:Q43"/>
-    <mergeCell ref="R43:AL43"/>
-    <mergeCell ref="AM43:BC43"/>
-    <mergeCell ref="AS38:AZ38"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="J40:AZ40"/>
-    <mergeCell ref="AA41:AP41"/>
-    <mergeCell ref="A42:Q42"/>
-    <mergeCell ref="R42:AL42"/>
-    <mergeCell ref="AM42:BC42"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="AT34:AY34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="AT35:AY35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="G36:AI36"/>
-    <mergeCell ref="AL36:AQ36"/>
-    <mergeCell ref="AT36:AY36"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="AT31:AY31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="AT32:AY32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="AT33:AY33"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="AT28:AY28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="AT29:AY29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="AT30:AY30"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="AT25:AY25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="AT26:AY26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="AT27:AY27"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="AT18:AY18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="AT19:AY19"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="AT24:AY24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="AT20:AY20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="AT21:AY21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="AT22:AY22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="AT23:AY23"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="AT17:AY17"/>
-    <mergeCell ref="A9:AR9"/>
-    <mergeCell ref="AS9:AZ9"/>
-    <mergeCell ref="A10:AR10"/>
-    <mergeCell ref="AS10:AZ10"/>
-    <mergeCell ref="A12:E13"/>
-    <mergeCell ref="F12:AR13"/>
-    <mergeCell ref="AS12:AZ13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="AT15:AY15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="AT16:AY16"/>
     <mergeCell ref="AT6:AZ7"/>
     <mergeCell ref="P1:AN1"/>
     <mergeCell ref="AO1:AX1"/>
@@ -5784,6 +5718,69 @@
     <mergeCell ref="AL6:AM7"/>
     <mergeCell ref="AN6:AP7"/>
     <mergeCell ref="AQ6:AR7"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="AT17:AY17"/>
+    <mergeCell ref="A9:AR9"/>
+    <mergeCell ref="AS9:AZ9"/>
+    <mergeCell ref="A10:AR10"/>
+    <mergeCell ref="AS10:AZ10"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:AR13"/>
+    <mergeCell ref="AS12:AZ13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="AT15:AY15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="AT16:AY16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="AT18:AY18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="AT19:AY19"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="AT24:AY24"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="AT20:AY20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="AT21:AY21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="AT22:AY22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="AT23:AY23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="AT25:AY25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="AT26:AY26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="AT27:AY27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="AT28:AY28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="AT29:AY29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="AT30:AY30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="AT31:AY31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="AT32:AY32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="AT33:AY33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="AT34:AY34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="AT35:AY35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G36:AI36"/>
+    <mergeCell ref="AL36:AQ36"/>
+    <mergeCell ref="AT36:AY36"/>
+    <mergeCell ref="A43:Q43"/>
+    <mergeCell ref="R43:AL43"/>
+    <mergeCell ref="AM43:BC43"/>
+    <mergeCell ref="AS38:AZ38"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="J40:AZ40"/>
+    <mergeCell ref="AA41:AP41"/>
+    <mergeCell ref="A42:Q42"/>
+    <mergeCell ref="R42:AL42"/>
+    <mergeCell ref="AM42:BC42"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ41:AX42 KM41:KT42 UI41:UP42 AEE41:AEL42 AOA41:AOH42 AXW41:AYD42 BHS41:BHZ42 BRO41:BRV42 CBK41:CBR42 CLG41:CLN42 CVC41:CVJ42 DEY41:DFF42 DOU41:DPB42 DYQ41:DYX42 EIM41:EIT42 ESI41:ESP42 FCE41:FCL42 FMA41:FMH42 FVW41:FWD42 GFS41:GFZ42 GPO41:GPV42 GZK41:GZR42 HJG41:HJN42 HTC41:HTJ42 ICY41:IDF42 IMU41:INB42 IWQ41:IWX42 JGM41:JGT42 JQI41:JQP42 KAE41:KAL42 KKA41:KKH42 KTW41:KUD42 LDS41:LDZ42 LNO41:LNV42 LXK41:LXR42 MHG41:MHN42 MRC41:MRJ42 NAY41:NBF42 NKU41:NLB42 NUQ41:NUX42 OEM41:OET42 OOI41:OOP42 OYE41:OYL42 PIA41:PIH42 PRW41:PSD42 QBS41:QBZ42 QLO41:QLV42 QVK41:QVR42 RFG41:RFN42 RPC41:RPJ42 RYY41:RZF42 SIU41:SJB42 SSQ41:SSX42 TCM41:TCT42 TMI41:TMP42 TWE41:TWL42 UGA41:UGH42 UPW41:UQD42 UZS41:UZZ42 VJO41:VJV42 VTK41:VTR42 WDG41:WDN42 WNC41:WNJ42 WWY41:WXF42 AQ65577:AX65578 KM65577:KT65578 UI65577:UP65578 AEE65577:AEL65578 AOA65577:AOH65578 AXW65577:AYD65578 BHS65577:BHZ65578 BRO65577:BRV65578 CBK65577:CBR65578 CLG65577:CLN65578 CVC65577:CVJ65578 DEY65577:DFF65578 DOU65577:DPB65578 DYQ65577:DYX65578 EIM65577:EIT65578 ESI65577:ESP65578 FCE65577:FCL65578 FMA65577:FMH65578 FVW65577:FWD65578 GFS65577:GFZ65578 GPO65577:GPV65578 GZK65577:GZR65578 HJG65577:HJN65578 HTC65577:HTJ65578 ICY65577:IDF65578 IMU65577:INB65578 IWQ65577:IWX65578 JGM65577:JGT65578 JQI65577:JQP65578 KAE65577:KAL65578 KKA65577:KKH65578 KTW65577:KUD65578 LDS65577:LDZ65578 LNO65577:LNV65578 LXK65577:LXR65578 MHG65577:MHN65578 MRC65577:MRJ65578 NAY65577:NBF65578 NKU65577:NLB65578 NUQ65577:NUX65578 OEM65577:OET65578 OOI65577:OOP65578 OYE65577:OYL65578 PIA65577:PIH65578 PRW65577:PSD65578 QBS65577:QBZ65578 QLO65577:QLV65578 QVK65577:QVR65578 RFG65577:RFN65578 RPC65577:RPJ65578 RYY65577:RZF65578 SIU65577:SJB65578 SSQ65577:SSX65578 TCM65577:TCT65578 TMI65577:TMP65578 TWE65577:TWL65578 UGA65577:UGH65578 UPW65577:UQD65578 UZS65577:UZZ65578 VJO65577:VJV65578 VTK65577:VTR65578 WDG65577:WDN65578 WNC65577:WNJ65578 WWY65577:WXF65578 AQ131113:AX131114 KM131113:KT131114 UI131113:UP131114 AEE131113:AEL131114 AOA131113:AOH131114 AXW131113:AYD131114 BHS131113:BHZ131114 BRO131113:BRV131114 CBK131113:CBR131114 CLG131113:CLN131114 CVC131113:CVJ131114 DEY131113:DFF131114 DOU131113:DPB131114 DYQ131113:DYX131114 EIM131113:EIT131114 ESI131113:ESP131114 FCE131113:FCL131114 FMA131113:FMH131114 FVW131113:FWD131114 GFS131113:GFZ131114 GPO131113:GPV131114 GZK131113:GZR131114 HJG131113:HJN131114 HTC131113:HTJ131114 ICY131113:IDF131114 IMU131113:INB131114 IWQ131113:IWX131114 JGM131113:JGT131114 JQI131113:JQP131114 KAE131113:KAL131114 KKA131113:KKH131114 KTW131113:KUD131114 LDS131113:LDZ131114 LNO131113:LNV131114 LXK131113:LXR131114 MHG131113:MHN131114 MRC131113:MRJ131114 NAY131113:NBF131114 NKU131113:NLB131114 NUQ131113:NUX131114 OEM131113:OET131114 OOI131113:OOP131114 OYE131113:OYL131114 PIA131113:PIH131114 PRW131113:PSD131114 QBS131113:QBZ131114 QLO131113:QLV131114 QVK131113:QVR131114 RFG131113:RFN131114 RPC131113:RPJ131114 RYY131113:RZF131114 SIU131113:SJB131114 SSQ131113:SSX131114 TCM131113:TCT131114 TMI131113:TMP131114 TWE131113:TWL131114 UGA131113:UGH131114 UPW131113:UQD131114 UZS131113:UZZ131114 VJO131113:VJV131114 VTK131113:VTR131114 WDG131113:WDN131114 WNC131113:WNJ131114 WWY131113:WXF131114 AQ196649:AX196650 KM196649:KT196650 UI196649:UP196650 AEE196649:AEL196650 AOA196649:AOH196650 AXW196649:AYD196650 BHS196649:BHZ196650 BRO196649:BRV196650 CBK196649:CBR196650 CLG196649:CLN196650 CVC196649:CVJ196650 DEY196649:DFF196650 DOU196649:DPB196650 DYQ196649:DYX196650 EIM196649:EIT196650 ESI196649:ESP196650 FCE196649:FCL196650 FMA196649:FMH196650 FVW196649:FWD196650 GFS196649:GFZ196650 GPO196649:GPV196650 GZK196649:GZR196650 HJG196649:HJN196650 HTC196649:HTJ196650 ICY196649:IDF196650 IMU196649:INB196650 IWQ196649:IWX196650 JGM196649:JGT196650 JQI196649:JQP196650 KAE196649:KAL196650 KKA196649:KKH196650 KTW196649:KUD196650 LDS196649:LDZ196650 LNO196649:LNV196650 LXK196649:LXR196650 MHG196649:MHN196650 MRC196649:MRJ196650 NAY196649:NBF196650 NKU196649:NLB196650 NUQ196649:NUX196650 OEM196649:OET196650 OOI196649:OOP196650 OYE196649:OYL196650 PIA196649:PIH196650 PRW196649:PSD196650 QBS196649:QBZ196650 QLO196649:QLV196650 QVK196649:QVR196650 RFG196649:RFN196650 RPC196649:RPJ196650 RYY196649:RZF196650 SIU196649:SJB196650 SSQ196649:SSX196650 TCM196649:TCT196650 TMI196649:TMP196650 TWE196649:TWL196650 UGA196649:UGH196650 UPW196649:UQD196650 UZS196649:UZZ196650 VJO196649:VJV196650 VTK196649:VTR196650 WDG196649:WDN196650 WNC196649:WNJ196650 WWY196649:WXF196650 AQ262185:AX262186 KM262185:KT262186 UI262185:UP262186 AEE262185:AEL262186 AOA262185:AOH262186 AXW262185:AYD262186 BHS262185:BHZ262186 BRO262185:BRV262186 CBK262185:CBR262186 CLG262185:CLN262186 CVC262185:CVJ262186 DEY262185:DFF262186 DOU262185:DPB262186 DYQ262185:DYX262186 EIM262185:EIT262186 ESI262185:ESP262186 FCE262185:FCL262186 FMA262185:FMH262186 FVW262185:FWD262186 GFS262185:GFZ262186 GPO262185:GPV262186 GZK262185:GZR262186 HJG262185:HJN262186 HTC262185:HTJ262186 ICY262185:IDF262186 IMU262185:INB262186 IWQ262185:IWX262186 JGM262185:JGT262186 JQI262185:JQP262186 KAE262185:KAL262186 KKA262185:KKH262186 KTW262185:KUD262186 LDS262185:LDZ262186 LNO262185:LNV262186 LXK262185:LXR262186 MHG262185:MHN262186 MRC262185:MRJ262186 NAY262185:NBF262186 NKU262185:NLB262186 NUQ262185:NUX262186 OEM262185:OET262186 OOI262185:OOP262186 OYE262185:OYL262186 PIA262185:PIH262186 PRW262185:PSD262186 QBS262185:QBZ262186 QLO262185:QLV262186 QVK262185:QVR262186 RFG262185:RFN262186 RPC262185:RPJ262186 RYY262185:RZF262186 SIU262185:SJB262186 SSQ262185:SSX262186 TCM262185:TCT262186 TMI262185:TMP262186 TWE262185:TWL262186 UGA262185:UGH262186 UPW262185:UQD262186 UZS262185:UZZ262186 VJO262185:VJV262186 VTK262185:VTR262186 WDG262185:WDN262186 WNC262185:WNJ262186 WWY262185:WXF262186 AQ327721:AX327722 KM327721:KT327722 UI327721:UP327722 AEE327721:AEL327722 AOA327721:AOH327722 AXW327721:AYD327722 BHS327721:BHZ327722 BRO327721:BRV327722 CBK327721:CBR327722 CLG327721:CLN327722 CVC327721:CVJ327722 DEY327721:DFF327722 DOU327721:DPB327722 DYQ327721:DYX327722 EIM327721:EIT327722 ESI327721:ESP327722 FCE327721:FCL327722 FMA327721:FMH327722 FVW327721:FWD327722 GFS327721:GFZ327722 GPO327721:GPV327722 GZK327721:GZR327722 HJG327721:HJN327722 HTC327721:HTJ327722 ICY327721:IDF327722 IMU327721:INB327722 IWQ327721:IWX327722 JGM327721:JGT327722 JQI327721:JQP327722 KAE327721:KAL327722 KKA327721:KKH327722 KTW327721:KUD327722 LDS327721:LDZ327722 LNO327721:LNV327722 LXK327721:LXR327722 MHG327721:MHN327722 MRC327721:MRJ327722 NAY327721:NBF327722 NKU327721:NLB327722 NUQ327721:NUX327722 OEM327721:OET327722 OOI327721:OOP327722 OYE327721:OYL327722 PIA327721:PIH327722 PRW327721:PSD327722 QBS327721:QBZ327722 QLO327721:QLV327722 QVK327721:QVR327722 RFG327721:RFN327722 RPC327721:RPJ327722 RYY327721:RZF327722 SIU327721:SJB327722 SSQ327721:SSX327722 TCM327721:TCT327722 TMI327721:TMP327722 TWE327721:TWL327722 UGA327721:UGH327722 UPW327721:UQD327722 UZS327721:UZZ327722 VJO327721:VJV327722 VTK327721:VTR327722 WDG327721:WDN327722 WNC327721:WNJ327722 WWY327721:WXF327722 AQ393257:AX393258 KM393257:KT393258 UI393257:UP393258 AEE393257:AEL393258 AOA393257:AOH393258 AXW393257:AYD393258 BHS393257:BHZ393258 BRO393257:BRV393258 CBK393257:CBR393258 CLG393257:CLN393258 CVC393257:CVJ393258 DEY393257:DFF393258 DOU393257:DPB393258 DYQ393257:DYX393258 EIM393257:EIT393258 ESI393257:ESP393258 FCE393257:FCL393258 FMA393257:FMH393258 FVW393257:FWD393258 GFS393257:GFZ393258 GPO393257:GPV393258 GZK393257:GZR393258 HJG393257:HJN393258 HTC393257:HTJ393258 ICY393257:IDF393258 IMU393257:INB393258 IWQ393257:IWX393258 JGM393257:JGT393258 JQI393257:JQP393258 KAE393257:KAL393258 KKA393257:KKH393258 KTW393257:KUD393258 LDS393257:LDZ393258 LNO393257:LNV393258 LXK393257:LXR393258 MHG393257:MHN393258 MRC393257:MRJ393258 NAY393257:NBF393258 NKU393257:NLB393258 NUQ393257:NUX393258 OEM393257:OET393258 OOI393257:OOP393258 OYE393257:OYL393258 PIA393257:PIH393258 PRW393257:PSD393258 QBS393257:QBZ393258 QLO393257:QLV393258 QVK393257:QVR393258 RFG393257:RFN393258 RPC393257:RPJ393258 RYY393257:RZF393258 SIU393257:SJB393258 SSQ393257:SSX393258 TCM393257:TCT393258 TMI393257:TMP393258 TWE393257:TWL393258 UGA393257:UGH393258 UPW393257:UQD393258 UZS393257:UZZ393258 VJO393257:VJV393258 VTK393257:VTR393258 WDG393257:WDN393258 WNC393257:WNJ393258 WWY393257:WXF393258 AQ458793:AX458794 KM458793:KT458794 UI458793:UP458794 AEE458793:AEL458794 AOA458793:AOH458794 AXW458793:AYD458794 BHS458793:BHZ458794 BRO458793:BRV458794 CBK458793:CBR458794 CLG458793:CLN458794 CVC458793:CVJ458794 DEY458793:DFF458794 DOU458793:DPB458794 DYQ458793:DYX458794 EIM458793:EIT458794 ESI458793:ESP458794 FCE458793:FCL458794 FMA458793:FMH458794 FVW458793:FWD458794 GFS458793:GFZ458794 GPO458793:GPV458794 GZK458793:GZR458794 HJG458793:HJN458794 HTC458793:HTJ458794 ICY458793:IDF458794 IMU458793:INB458794 IWQ458793:IWX458794 JGM458793:JGT458794 JQI458793:JQP458794 KAE458793:KAL458794 KKA458793:KKH458794 KTW458793:KUD458794 LDS458793:LDZ458794 LNO458793:LNV458794 LXK458793:LXR458794 MHG458793:MHN458794 MRC458793:MRJ458794 NAY458793:NBF458794 NKU458793:NLB458794 NUQ458793:NUX458794 OEM458793:OET458794 OOI458793:OOP458794 OYE458793:OYL458794 PIA458793:PIH458794 PRW458793:PSD458794 QBS458793:QBZ458794 QLO458793:QLV458794 QVK458793:QVR458794 RFG458793:RFN458794 RPC458793:RPJ458794 RYY458793:RZF458794 SIU458793:SJB458794 SSQ458793:SSX458794 TCM458793:TCT458794 TMI458793:TMP458794 TWE458793:TWL458794 UGA458793:UGH458794 UPW458793:UQD458794 UZS458793:UZZ458794 VJO458793:VJV458794 VTK458793:VTR458794 WDG458793:WDN458794 WNC458793:WNJ458794 WWY458793:WXF458794 AQ524329:AX524330 KM524329:KT524330 UI524329:UP524330 AEE524329:AEL524330 AOA524329:AOH524330 AXW524329:AYD524330 BHS524329:BHZ524330 BRO524329:BRV524330 CBK524329:CBR524330 CLG524329:CLN524330 CVC524329:CVJ524330 DEY524329:DFF524330 DOU524329:DPB524330 DYQ524329:DYX524330 EIM524329:EIT524330 ESI524329:ESP524330 FCE524329:FCL524330 FMA524329:FMH524330 FVW524329:FWD524330 GFS524329:GFZ524330 GPO524329:GPV524330 GZK524329:GZR524330 HJG524329:HJN524330 HTC524329:HTJ524330 ICY524329:IDF524330 IMU524329:INB524330 IWQ524329:IWX524330 JGM524329:JGT524330 JQI524329:JQP524330 KAE524329:KAL524330 KKA524329:KKH524330 KTW524329:KUD524330 LDS524329:LDZ524330 LNO524329:LNV524330 LXK524329:LXR524330 MHG524329:MHN524330 MRC524329:MRJ524330 NAY524329:NBF524330 NKU524329:NLB524330 NUQ524329:NUX524330 OEM524329:OET524330 OOI524329:OOP524330 OYE524329:OYL524330 PIA524329:PIH524330 PRW524329:PSD524330 QBS524329:QBZ524330 QLO524329:QLV524330 QVK524329:QVR524330 RFG524329:RFN524330 RPC524329:RPJ524330 RYY524329:RZF524330 SIU524329:SJB524330 SSQ524329:SSX524330 TCM524329:TCT524330 TMI524329:TMP524330 TWE524329:TWL524330 UGA524329:UGH524330 UPW524329:UQD524330 UZS524329:UZZ524330 VJO524329:VJV524330 VTK524329:VTR524330 WDG524329:WDN524330 WNC524329:WNJ524330 WWY524329:WXF524330 AQ589865:AX589866 KM589865:KT589866 UI589865:UP589866 AEE589865:AEL589866 AOA589865:AOH589866 AXW589865:AYD589866 BHS589865:BHZ589866 BRO589865:BRV589866 CBK589865:CBR589866 CLG589865:CLN589866 CVC589865:CVJ589866 DEY589865:DFF589866 DOU589865:DPB589866 DYQ589865:DYX589866 EIM589865:EIT589866 ESI589865:ESP589866 FCE589865:FCL589866 FMA589865:FMH589866 FVW589865:FWD589866 GFS589865:GFZ589866 GPO589865:GPV589866 GZK589865:GZR589866 HJG589865:HJN589866 HTC589865:HTJ589866 ICY589865:IDF589866 IMU589865:INB589866 IWQ589865:IWX589866 JGM589865:JGT589866 JQI589865:JQP589866 KAE589865:KAL589866 KKA589865:KKH589866 KTW589865:KUD589866 LDS589865:LDZ589866 LNO589865:LNV589866 LXK589865:LXR589866 MHG589865:MHN589866 MRC589865:MRJ589866 NAY589865:NBF589866 NKU589865:NLB589866 NUQ589865:NUX589866 OEM589865:OET589866 OOI589865:OOP589866 OYE589865:OYL589866 PIA589865:PIH589866 PRW589865:PSD589866 QBS589865:QBZ589866 QLO589865:QLV589866 QVK589865:QVR589866 RFG589865:RFN589866 RPC589865:RPJ589866 RYY589865:RZF589866 SIU589865:SJB589866 SSQ589865:SSX589866 TCM589865:TCT589866 TMI589865:TMP589866 TWE589865:TWL589866 UGA589865:UGH589866 UPW589865:UQD589866 UZS589865:UZZ589866 VJO589865:VJV589866 VTK589865:VTR589866 WDG589865:WDN589866 WNC589865:WNJ589866 WWY589865:WXF589866 AQ655401:AX655402 KM655401:KT655402 UI655401:UP655402 AEE655401:AEL655402 AOA655401:AOH655402 AXW655401:AYD655402 BHS655401:BHZ655402 BRO655401:BRV655402 CBK655401:CBR655402 CLG655401:CLN655402 CVC655401:CVJ655402 DEY655401:DFF655402 DOU655401:DPB655402 DYQ655401:DYX655402 EIM655401:EIT655402 ESI655401:ESP655402 FCE655401:FCL655402 FMA655401:FMH655402 FVW655401:FWD655402 GFS655401:GFZ655402 GPO655401:GPV655402 GZK655401:GZR655402 HJG655401:HJN655402 HTC655401:HTJ655402 ICY655401:IDF655402 IMU655401:INB655402 IWQ655401:IWX655402 JGM655401:JGT655402 JQI655401:JQP655402 KAE655401:KAL655402 KKA655401:KKH655402 KTW655401:KUD655402 LDS655401:LDZ655402 LNO655401:LNV655402 LXK655401:LXR655402 MHG655401:MHN655402 MRC655401:MRJ655402 NAY655401:NBF655402 NKU655401:NLB655402 NUQ655401:NUX655402 OEM655401:OET655402 OOI655401:OOP655402 OYE655401:OYL655402 PIA655401:PIH655402 PRW655401:PSD655402 QBS655401:QBZ655402 QLO655401:QLV655402 QVK655401:QVR655402 RFG655401:RFN655402 RPC655401:RPJ655402 RYY655401:RZF655402 SIU655401:SJB655402 SSQ655401:SSX655402 TCM655401:TCT655402 TMI655401:TMP655402 TWE655401:TWL655402 UGA655401:UGH655402 UPW655401:UQD655402 UZS655401:UZZ655402 VJO655401:VJV655402 VTK655401:VTR655402 WDG655401:WDN655402 WNC655401:WNJ655402 WWY655401:WXF655402 AQ720937:AX720938 KM720937:KT720938 UI720937:UP720938 AEE720937:AEL720938 AOA720937:AOH720938 AXW720937:AYD720938 BHS720937:BHZ720938 BRO720937:BRV720938 CBK720937:CBR720938 CLG720937:CLN720938 CVC720937:CVJ720938 DEY720937:DFF720938 DOU720937:DPB720938 DYQ720937:DYX720938 EIM720937:EIT720938 ESI720937:ESP720938 FCE720937:FCL720938 FMA720937:FMH720938 FVW720937:FWD720938 GFS720937:GFZ720938 GPO720937:GPV720938 GZK720937:GZR720938 HJG720937:HJN720938 HTC720937:HTJ720938 ICY720937:IDF720938 IMU720937:INB720938 IWQ720937:IWX720938 JGM720937:JGT720938 JQI720937:JQP720938 KAE720937:KAL720938 KKA720937:KKH720938 KTW720937:KUD720938 LDS720937:LDZ720938 LNO720937:LNV720938 LXK720937:LXR720938 MHG720937:MHN720938 MRC720937:MRJ720938 NAY720937:NBF720938 NKU720937:NLB720938 NUQ720937:NUX720938 OEM720937:OET720938 OOI720937:OOP720938 OYE720937:OYL720938 PIA720937:PIH720938 PRW720937:PSD720938 QBS720937:QBZ720938 QLO720937:QLV720938 QVK720937:QVR720938 RFG720937:RFN720938 RPC720937:RPJ720938 RYY720937:RZF720938 SIU720937:SJB720938 SSQ720937:SSX720938 TCM720937:TCT720938 TMI720937:TMP720938 TWE720937:TWL720938 UGA720937:UGH720938 UPW720937:UQD720938 UZS720937:UZZ720938 VJO720937:VJV720938 VTK720937:VTR720938 WDG720937:WDN720938 WNC720937:WNJ720938 WWY720937:WXF720938 AQ786473:AX786474 KM786473:KT786474 UI786473:UP786474 AEE786473:AEL786474 AOA786473:AOH786474 AXW786473:AYD786474 BHS786473:BHZ786474 BRO786473:BRV786474 CBK786473:CBR786474 CLG786473:CLN786474 CVC786473:CVJ786474 DEY786473:DFF786474 DOU786473:DPB786474 DYQ786473:DYX786474 EIM786473:EIT786474 ESI786473:ESP786474 FCE786473:FCL786474 FMA786473:FMH786474 FVW786473:FWD786474 GFS786473:GFZ786474 GPO786473:GPV786474 GZK786473:GZR786474 HJG786473:HJN786474 HTC786473:HTJ786474 ICY786473:IDF786474 IMU786473:INB786474 IWQ786473:IWX786474 JGM786473:JGT786474 JQI786473:JQP786474 KAE786473:KAL786474 KKA786473:KKH786474 KTW786473:KUD786474 LDS786473:LDZ786474 LNO786473:LNV786474 LXK786473:LXR786474 MHG786473:MHN786474 MRC786473:MRJ786474 NAY786473:NBF786474 NKU786473:NLB786474 NUQ786473:NUX786474 OEM786473:OET786474 OOI786473:OOP786474 OYE786473:OYL786474 PIA786473:PIH786474 PRW786473:PSD786474 QBS786473:QBZ786474 QLO786473:QLV786474 QVK786473:QVR786474 RFG786473:RFN786474 RPC786473:RPJ786474 RYY786473:RZF786474 SIU786473:SJB786474 SSQ786473:SSX786474 TCM786473:TCT786474 TMI786473:TMP786474 TWE786473:TWL786474 UGA786473:UGH786474 UPW786473:UQD786474 UZS786473:UZZ786474 VJO786473:VJV786474 VTK786473:VTR786474 WDG786473:WDN786474 WNC786473:WNJ786474 WWY786473:WXF786474 AQ852009:AX852010 KM852009:KT852010 UI852009:UP852010 AEE852009:AEL852010 AOA852009:AOH852010 AXW852009:AYD852010 BHS852009:BHZ852010 BRO852009:BRV852010 CBK852009:CBR852010 CLG852009:CLN852010 CVC852009:CVJ852010 DEY852009:DFF852010 DOU852009:DPB852010 DYQ852009:DYX852010 EIM852009:EIT852010 ESI852009:ESP852010 FCE852009:FCL852010 FMA852009:FMH852010 FVW852009:FWD852010 GFS852009:GFZ852010 GPO852009:GPV852010 GZK852009:GZR852010 HJG852009:HJN852010 HTC852009:HTJ852010 ICY852009:IDF852010 IMU852009:INB852010 IWQ852009:IWX852010 JGM852009:JGT852010 JQI852009:JQP852010 KAE852009:KAL852010 KKA852009:KKH852010 KTW852009:KUD852010 LDS852009:LDZ852010 LNO852009:LNV852010 LXK852009:LXR852010 MHG852009:MHN852010 MRC852009:MRJ852010 NAY852009:NBF852010 NKU852009:NLB852010 NUQ852009:NUX852010 OEM852009:OET852010 OOI852009:OOP852010 OYE852009:OYL852010 PIA852009:PIH852010 PRW852009:PSD852010 QBS852009:QBZ852010 QLO852009:QLV852010 QVK852009:QVR852010 RFG852009:RFN852010 RPC852009:RPJ852010 RYY852009:RZF852010 SIU852009:SJB852010 SSQ852009:SSX852010 TCM852009:TCT852010 TMI852009:TMP852010 TWE852009:TWL852010 UGA852009:UGH852010 UPW852009:UQD852010 UZS852009:UZZ852010 VJO852009:VJV852010 VTK852009:VTR852010 WDG852009:WDN852010 WNC852009:WNJ852010 WWY852009:WXF852010 AQ917545:AX917546 KM917545:KT917546 UI917545:UP917546 AEE917545:AEL917546 AOA917545:AOH917546 AXW917545:AYD917546 BHS917545:BHZ917546 BRO917545:BRV917546 CBK917545:CBR917546 CLG917545:CLN917546 CVC917545:CVJ917546 DEY917545:DFF917546 DOU917545:DPB917546 DYQ917545:DYX917546 EIM917545:EIT917546 ESI917545:ESP917546 FCE917545:FCL917546 FMA917545:FMH917546 FVW917545:FWD917546 GFS917545:GFZ917546 GPO917545:GPV917546 GZK917545:GZR917546 HJG917545:HJN917546 HTC917545:HTJ917546 ICY917545:IDF917546 IMU917545:INB917546 IWQ917545:IWX917546 JGM917545:JGT917546 JQI917545:JQP917546 KAE917545:KAL917546 KKA917545:KKH917546 KTW917545:KUD917546 LDS917545:LDZ917546 LNO917545:LNV917546 LXK917545:LXR917546 MHG917545:MHN917546 MRC917545:MRJ917546 NAY917545:NBF917546 NKU917545:NLB917546 NUQ917545:NUX917546 OEM917545:OET917546 OOI917545:OOP917546 OYE917545:OYL917546 PIA917545:PIH917546 PRW917545:PSD917546 QBS917545:QBZ917546 QLO917545:QLV917546 QVK917545:QVR917546 RFG917545:RFN917546 RPC917545:RPJ917546 RYY917545:RZF917546 SIU917545:SJB917546 SSQ917545:SSX917546 TCM917545:TCT917546 TMI917545:TMP917546 TWE917545:TWL917546 UGA917545:UGH917546 UPW917545:UQD917546 UZS917545:UZZ917546 VJO917545:VJV917546 VTK917545:VTR917546 WDG917545:WDN917546 WNC917545:WNJ917546 WWY917545:WXF917546 AQ983081:AX983082 KM983081:KT983082 UI983081:UP983082 AEE983081:AEL983082 AOA983081:AOH983082 AXW983081:AYD983082 BHS983081:BHZ983082 BRO983081:BRV983082 CBK983081:CBR983082 CLG983081:CLN983082 CVC983081:CVJ983082 DEY983081:DFF983082 DOU983081:DPB983082 DYQ983081:DYX983082 EIM983081:EIT983082 ESI983081:ESP983082 FCE983081:FCL983082 FMA983081:FMH983082 FVW983081:FWD983082 GFS983081:GFZ983082 GPO983081:GPV983082 GZK983081:GZR983082 HJG983081:HJN983082 HTC983081:HTJ983082 ICY983081:IDF983082 IMU983081:INB983082 IWQ983081:IWX983082 JGM983081:JGT983082 JQI983081:JQP983082 KAE983081:KAL983082 KKA983081:KKH983082 KTW983081:KUD983082 LDS983081:LDZ983082 LNO983081:LNV983082 LXK983081:LXR983082 MHG983081:MHN983082 MRC983081:MRJ983082 NAY983081:NBF983082 NKU983081:NLB983082 NUQ983081:NUX983082 OEM983081:OET983082 OOI983081:OOP983082 OYE983081:OYL983082 PIA983081:PIH983082 PRW983081:PSD983082 QBS983081:QBZ983082 QLO983081:QLV983082 QVK983081:QVR983082 RFG983081:RFN983082 RPC983081:RPJ983082 RYY983081:RZF983082 SIU983081:SJB983082 SSQ983081:SSX983082 TCM983081:TCT983082 TMI983081:TMP983082 TWE983081:TWL983082 UGA983081:UGH983082 UPW983081:UQD983082 UZS983081:UZZ983082 VJO983081:VJV983082 VTK983081:VTR983082 WDG983081:WDN983082 WNC983081:WNJ983082 WWY983081:WXF983082 X41:Z41 JT41:JV41 TP41:TR41 ADL41:ADN41 ANH41:ANJ41 AXD41:AXF41 BGZ41:BHB41 BQV41:BQX41 CAR41:CAT41 CKN41:CKP41 CUJ41:CUL41 DEF41:DEH41 DOB41:DOD41 DXX41:DXZ41 EHT41:EHV41 ERP41:ERR41 FBL41:FBN41 FLH41:FLJ41 FVD41:FVF41 GEZ41:GFB41 GOV41:GOX41 GYR41:GYT41 HIN41:HIP41 HSJ41:HSL41 ICF41:ICH41 IMB41:IMD41 IVX41:IVZ41 JFT41:JFV41 JPP41:JPR41 JZL41:JZN41 KJH41:KJJ41 KTD41:KTF41 LCZ41:LDB41 LMV41:LMX41 LWR41:LWT41 MGN41:MGP41 MQJ41:MQL41 NAF41:NAH41 NKB41:NKD41 NTX41:NTZ41 ODT41:ODV41 ONP41:ONR41 OXL41:OXN41 PHH41:PHJ41 PRD41:PRF41 QAZ41:QBB41 QKV41:QKX41 QUR41:QUT41 REN41:REP41 ROJ41:ROL41 RYF41:RYH41 SIB41:SID41 SRX41:SRZ41 TBT41:TBV41 TLP41:TLR41 TVL41:TVN41 UFH41:UFJ41 UPD41:UPF41 UYZ41:UZB41 VIV41:VIX41 VSR41:VST41 WCN41:WCP41 WMJ41:WML41 WWF41:WWH41 X65577:Z65577 JT65577:JV65577 TP65577:TR65577 ADL65577:ADN65577 ANH65577:ANJ65577 AXD65577:AXF65577 BGZ65577:BHB65577 BQV65577:BQX65577 CAR65577:CAT65577 CKN65577:CKP65577 CUJ65577:CUL65577 DEF65577:DEH65577 DOB65577:DOD65577 DXX65577:DXZ65577 EHT65577:EHV65577 ERP65577:ERR65577 FBL65577:FBN65577 FLH65577:FLJ65577 FVD65577:FVF65577 GEZ65577:GFB65577 GOV65577:GOX65577 GYR65577:GYT65577 HIN65577:HIP65577 HSJ65577:HSL65577 ICF65577:ICH65577 IMB65577:IMD65577 IVX65577:IVZ65577 JFT65577:JFV65577 JPP65577:JPR65577 JZL65577:JZN65577 KJH65577:KJJ65577 KTD65577:KTF65577 LCZ65577:LDB65577 LMV65577:LMX65577 LWR65577:LWT65577 MGN65577:MGP65577 MQJ65577:MQL65577 NAF65577:NAH65577 NKB65577:NKD65577 NTX65577:NTZ65577 ODT65577:ODV65577 ONP65577:ONR65577 OXL65577:OXN65577 PHH65577:PHJ65577 PRD65577:PRF65577 QAZ65577:QBB65577 QKV65577:QKX65577 QUR65577:QUT65577 REN65577:REP65577 ROJ65577:ROL65577 RYF65577:RYH65577 SIB65577:SID65577 SRX65577:SRZ65577 TBT65577:TBV65577 TLP65577:TLR65577 TVL65577:TVN65577 UFH65577:UFJ65577 UPD65577:UPF65577 UYZ65577:UZB65577 VIV65577:VIX65577 VSR65577:VST65577 WCN65577:WCP65577 WMJ65577:WML65577 WWF65577:WWH65577 X131113:Z131113 JT131113:JV131113 TP131113:TR131113 ADL131113:ADN131113 ANH131113:ANJ131113 AXD131113:AXF131113 BGZ131113:BHB131113 BQV131113:BQX131113 CAR131113:CAT131113 CKN131113:CKP131113 CUJ131113:CUL131113 DEF131113:DEH131113 DOB131113:DOD131113 DXX131113:DXZ131113 EHT131113:EHV131113 ERP131113:ERR131113 FBL131113:FBN131113 FLH131113:FLJ131113 FVD131113:FVF131113 GEZ131113:GFB131113 GOV131113:GOX131113 GYR131113:GYT131113 HIN131113:HIP131113 HSJ131113:HSL131113 ICF131113:ICH131113 IMB131113:IMD131113 IVX131113:IVZ131113 JFT131113:JFV131113 JPP131113:JPR131113 JZL131113:JZN131113 KJH131113:KJJ131113 KTD131113:KTF131113 LCZ131113:LDB131113 LMV131113:LMX131113 LWR131113:LWT131113 MGN131113:MGP131113 MQJ131113:MQL131113 NAF131113:NAH131113 NKB131113:NKD131113 NTX131113:NTZ131113 ODT131113:ODV131113 ONP131113:ONR131113 OXL131113:OXN131113 PHH131113:PHJ131113 PRD131113:PRF131113 QAZ131113:QBB131113 QKV131113:QKX131113 QUR131113:QUT131113 REN131113:REP131113 ROJ131113:ROL131113 RYF131113:RYH131113 SIB131113:SID131113 SRX131113:SRZ131113 TBT131113:TBV131113 TLP131113:TLR131113 TVL131113:TVN131113 UFH131113:UFJ131113 UPD131113:UPF131113 UYZ131113:UZB131113 VIV131113:VIX131113 VSR131113:VST131113 WCN131113:WCP131113 WMJ131113:WML131113 WWF131113:WWH131113 X196649:Z196649 JT196649:JV196649 TP196649:TR196649 ADL196649:ADN196649 ANH196649:ANJ196649 AXD196649:AXF196649 BGZ196649:BHB196649 BQV196649:BQX196649 CAR196649:CAT196649 CKN196649:CKP196649 CUJ196649:CUL196649 DEF196649:DEH196649 DOB196649:DOD196649 DXX196649:DXZ196649 EHT196649:EHV196649 ERP196649:ERR196649 FBL196649:FBN196649 FLH196649:FLJ196649 FVD196649:FVF196649 GEZ196649:GFB196649 GOV196649:GOX196649 GYR196649:GYT196649 HIN196649:HIP196649 HSJ196649:HSL196649 ICF196649:ICH196649 IMB196649:IMD196649 IVX196649:IVZ196649 JFT196649:JFV196649 JPP196649:JPR196649 JZL196649:JZN196649 KJH196649:KJJ196649 KTD196649:KTF196649 LCZ196649:LDB196649 LMV196649:LMX196649 LWR196649:LWT196649 MGN196649:MGP196649 MQJ196649:MQL196649 NAF196649:NAH196649 NKB196649:NKD196649 NTX196649:NTZ196649 ODT196649:ODV196649 ONP196649:ONR196649 OXL196649:OXN196649 PHH196649:PHJ196649 PRD196649:PRF196649 QAZ196649:QBB196649 QKV196649:QKX196649 QUR196649:QUT196649 REN196649:REP196649 ROJ196649:ROL196649 RYF196649:RYH196649 SIB196649:SID196649 SRX196649:SRZ196649 TBT196649:TBV196649 TLP196649:TLR196649 TVL196649:TVN196649 UFH196649:UFJ196649 UPD196649:UPF196649 UYZ196649:UZB196649 VIV196649:VIX196649 VSR196649:VST196649 WCN196649:WCP196649 WMJ196649:WML196649 WWF196649:WWH196649 X262185:Z262185 JT262185:JV262185 TP262185:TR262185 ADL262185:ADN262185 ANH262185:ANJ262185 AXD262185:AXF262185 BGZ262185:BHB262185 BQV262185:BQX262185 CAR262185:CAT262185 CKN262185:CKP262185 CUJ262185:CUL262185 DEF262185:DEH262185 DOB262185:DOD262185 DXX262185:DXZ262185 EHT262185:EHV262185 ERP262185:ERR262185 FBL262185:FBN262185 FLH262185:FLJ262185 FVD262185:FVF262185 GEZ262185:GFB262185 GOV262185:GOX262185 GYR262185:GYT262185 HIN262185:HIP262185 HSJ262185:HSL262185 ICF262185:ICH262185 IMB262185:IMD262185 IVX262185:IVZ262185 JFT262185:JFV262185 JPP262185:JPR262185 JZL262185:JZN262185 KJH262185:KJJ262185 KTD262185:KTF262185 LCZ262185:LDB262185 LMV262185:LMX262185 LWR262185:LWT262185 MGN262185:MGP262185 MQJ262185:MQL262185 NAF262185:NAH262185 NKB262185:NKD262185 NTX262185:NTZ262185 ODT262185:ODV262185 ONP262185:ONR262185 OXL262185:OXN262185 PHH262185:PHJ262185 PRD262185:PRF262185 QAZ262185:QBB262185 QKV262185:QKX262185 QUR262185:QUT262185 REN262185:REP262185 ROJ262185:ROL262185 RYF262185:RYH262185 SIB262185:SID262185 SRX262185:SRZ262185 TBT262185:TBV262185 TLP262185:TLR262185 TVL262185:TVN262185 UFH262185:UFJ262185 UPD262185:UPF262185 UYZ262185:UZB262185 VIV262185:VIX262185 VSR262185:VST262185 WCN262185:WCP262185 WMJ262185:WML262185 WWF262185:WWH262185 X327721:Z327721 JT327721:JV327721 TP327721:TR327721 ADL327721:ADN327721 ANH327721:ANJ327721 AXD327721:AXF327721 BGZ327721:BHB327721 BQV327721:BQX327721 CAR327721:CAT327721 CKN327721:CKP327721 CUJ327721:CUL327721 DEF327721:DEH327721 DOB327721:DOD327721 DXX327721:DXZ327721 EHT327721:EHV327721 ERP327721:ERR327721 FBL327721:FBN327721 FLH327721:FLJ327721 FVD327721:FVF327721 GEZ327721:GFB327721 GOV327721:GOX327721 GYR327721:GYT327721 HIN327721:HIP327721 HSJ327721:HSL327721 ICF327721:ICH327721 IMB327721:IMD327721 IVX327721:IVZ327721 JFT327721:JFV327721 JPP327721:JPR327721 JZL327721:JZN327721 KJH327721:KJJ327721 KTD327721:KTF327721 LCZ327721:LDB327721 LMV327721:LMX327721 LWR327721:LWT327721 MGN327721:MGP327721 MQJ327721:MQL327721 NAF327721:NAH327721 NKB327721:NKD327721 NTX327721:NTZ327721 ODT327721:ODV327721 ONP327721:ONR327721 OXL327721:OXN327721 PHH327721:PHJ327721 PRD327721:PRF327721 QAZ327721:QBB327721 QKV327721:QKX327721 QUR327721:QUT327721 REN327721:REP327721 ROJ327721:ROL327721 RYF327721:RYH327721 SIB327721:SID327721 SRX327721:SRZ327721 TBT327721:TBV327721 TLP327721:TLR327721 TVL327721:TVN327721 UFH327721:UFJ327721 UPD327721:UPF327721 UYZ327721:UZB327721 VIV327721:VIX327721 VSR327721:VST327721 WCN327721:WCP327721 WMJ327721:WML327721 WWF327721:WWH327721 X393257:Z393257 JT393257:JV393257 TP393257:TR393257 ADL393257:ADN393257 ANH393257:ANJ393257 AXD393257:AXF393257 BGZ393257:BHB393257 BQV393257:BQX393257 CAR393257:CAT393257 CKN393257:CKP393257 CUJ393257:CUL393257 DEF393257:DEH393257 DOB393257:DOD393257 DXX393257:DXZ393257 EHT393257:EHV393257 ERP393257:ERR393257 FBL393257:FBN393257 FLH393257:FLJ393257 FVD393257:FVF393257 GEZ393257:GFB393257 GOV393257:GOX393257 GYR393257:GYT393257 HIN393257:HIP393257 HSJ393257:HSL393257 ICF393257:ICH393257 IMB393257:IMD393257 IVX393257:IVZ393257 JFT393257:JFV393257 JPP393257:JPR393257 JZL393257:JZN393257 KJH393257:KJJ393257 KTD393257:KTF393257 LCZ393257:LDB393257 LMV393257:LMX393257 LWR393257:LWT393257 MGN393257:MGP393257 MQJ393257:MQL393257 NAF393257:NAH393257 NKB393257:NKD393257 NTX393257:NTZ393257 ODT393257:ODV393257 ONP393257:ONR393257 OXL393257:OXN393257 PHH393257:PHJ393257 PRD393257:PRF393257 QAZ393257:QBB393257 QKV393257:QKX393257 QUR393257:QUT393257 REN393257:REP393257 ROJ393257:ROL393257 RYF393257:RYH393257 SIB393257:SID393257 SRX393257:SRZ393257 TBT393257:TBV393257 TLP393257:TLR393257 TVL393257:TVN393257 UFH393257:UFJ393257 UPD393257:UPF393257 UYZ393257:UZB393257 VIV393257:VIX393257 VSR393257:VST393257 WCN393257:WCP393257 WMJ393257:WML393257 WWF393257:WWH393257 X458793:Z458793 JT458793:JV458793 TP458793:TR458793 ADL458793:ADN458793 ANH458793:ANJ458793 AXD458793:AXF458793 BGZ458793:BHB458793 BQV458793:BQX458793 CAR458793:CAT458793 CKN458793:CKP458793 CUJ458793:CUL458793 DEF458793:DEH458793 DOB458793:DOD458793 DXX458793:DXZ458793 EHT458793:EHV458793 ERP458793:ERR458793 FBL458793:FBN458793 FLH458793:FLJ458793 FVD458793:FVF458793 GEZ458793:GFB458793 GOV458793:GOX458793 GYR458793:GYT458793 HIN458793:HIP458793 HSJ458793:HSL458793 ICF458793:ICH458793 IMB458793:IMD458793 IVX458793:IVZ458793 JFT458793:JFV458793 JPP458793:JPR458793 JZL458793:JZN458793 KJH458793:KJJ458793 KTD458793:KTF458793 LCZ458793:LDB458793 LMV458793:LMX458793 LWR458793:LWT458793 MGN458793:MGP458793 MQJ458793:MQL458793 NAF458793:NAH458793 NKB458793:NKD458793 NTX458793:NTZ458793 ODT458793:ODV458793 ONP458793:ONR458793 OXL458793:OXN458793 PHH458793:PHJ458793 PRD458793:PRF458793 QAZ458793:QBB458793 QKV458793:QKX458793 QUR458793:QUT458793 REN458793:REP458793 ROJ458793:ROL458793 RYF458793:RYH458793 SIB458793:SID458793 SRX458793:SRZ458793 TBT458793:TBV458793 TLP458793:TLR458793 TVL458793:TVN458793 UFH458793:UFJ458793 UPD458793:UPF458793 UYZ458793:UZB458793 VIV458793:VIX458793 VSR458793:VST458793 WCN458793:WCP458793 WMJ458793:WML458793 WWF458793:WWH458793 X524329:Z524329 JT524329:JV524329 TP524329:TR524329 ADL524329:ADN524329 ANH524329:ANJ524329 AXD524329:AXF524329 BGZ524329:BHB524329 BQV524329:BQX524329 CAR524329:CAT524329 CKN524329:CKP524329 CUJ524329:CUL524329 DEF524329:DEH524329 DOB524329:DOD524329 DXX524329:DXZ524329 EHT524329:EHV524329 ERP524329:ERR524329 FBL524329:FBN524329 FLH524329:FLJ524329 FVD524329:FVF524329 GEZ524329:GFB524329 GOV524329:GOX524329 GYR524329:GYT524329 HIN524329:HIP524329 HSJ524329:HSL524329 ICF524329:ICH524329 IMB524329:IMD524329 IVX524329:IVZ524329 JFT524329:JFV524329 JPP524329:JPR524329 JZL524329:JZN524329 KJH524329:KJJ524329 KTD524329:KTF524329 LCZ524329:LDB524329 LMV524329:LMX524329 LWR524329:LWT524329 MGN524329:MGP524329 MQJ524329:MQL524329 NAF524329:NAH524329 NKB524329:NKD524329 NTX524329:NTZ524329 ODT524329:ODV524329 ONP524329:ONR524329 OXL524329:OXN524329 PHH524329:PHJ524329 PRD524329:PRF524329 QAZ524329:QBB524329 QKV524329:QKX524329 QUR524329:QUT524329 REN524329:REP524329 ROJ524329:ROL524329 RYF524329:RYH524329 SIB524329:SID524329 SRX524329:SRZ524329 TBT524329:TBV524329 TLP524329:TLR524329 TVL524329:TVN524329 UFH524329:UFJ524329 UPD524329:UPF524329 UYZ524329:UZB524329 VIV524329:VIX524329 VSR524329:VST524329 WCN524329:WCP524329 WMJ524329:WML524329 WWF524329:WWH524329 X589865:Z589865 JT589865:JV589865 TP589865:TR589865 ADL589865:ADN589865 ANH589865:ANJ589865 AXD589865:AXF589865 BGZ589865:BHB589865 BQV589865:BQX589865 CAR589865:CAT589865 CKN589865:CKP589865 CUJ589865:CUL589865 DEF589865:DEH589865 DOB589865:DOD589865 DXX589865:DXZ589865 EHT589865:EHV589865 ERP589865:ERR589865 FBL589865:FBN589865 FLH589865:FLJ589865 FVD589865:FVF589865 GEZ589865:GFB589865 GOV589865:GOX589865 GYR589865:GYT589865 HIN589865:HIP589865 HSJ589865:HSL589865 ICF589865:ICH589865 IMB589865:IMD589865 IVX589865:IVZ589865 JFT589865:JFV589865 JPP589865:JPR589865 JZL589865:JZN589865 KJH589865:KJJ589865 KTD589865:KTF589865 LCZ589865:LDB589865 LMV589865:LMX589865 LWR589865:LWT589865 MGN589865:MGP589865 MQJ589865:MQL589865 NAF589865:NAH589865 NKB589865:NKD589865 NTX589865:NTZ589865 ODT589865:ODV589865 ONP589865:ONR589865 OXL589865:OXN589865 PHH589865:PHJ589865 PRD589865:PRF589865 QAZ589865:QBB589865 QKV589865:QKX589865 QUR589865:QUT589865 REN589865:REP589865 ROJ589865:ROL589865 RYF589865:RYH589865 SIB589865:SID589865 SRX589865:SRZ589865 TBT589865:TBV589865 TLP589865:TLR589865 TVL589865:TVN589865 UFH589865:UFJ589865 UPD589865:UPF589865 UYZ589865:UZB589865 VIV589865:VIX589865 VSR589865:VST589865 WCN589865:WCP589865 WMJ589865:WML589865 WWF589865:WWH589865 X655401:Z655401 JT655401:JV655401 TP655401:TR655401 ADL655401:ADN655401 ANH655401:ANJ655401 AXD655401:AXF655401 BGZ655401:BHB655401 BQV655401:BQX655401 CAR655401:CAT655401 CKN655401:CKP655401 CUJ655401:CUL655401 DEF655401:DEH655401 DOB655401:DOD655401 DXX655401:DXZ655401 EHT655401:EHV655401 ERP655401:ERR655401 FBL655401:FBN655401 FLH655401:FLJ655401 FVD655401:FVF655401 GEZ655401:GFB655401 GOV655401:GOX655401 GYR655401:GYT655401 HIN655401:HIP655401 HSJ655401:HSL655401 ICF655401:ICH655401 IMB655401:IMD655401 IVX655401:IVZ655401 JFT655401:JFV655401 JPP655401:JPR655401 JZL655401:JZN655401 KJH655401:KJJ655401 KTD655401:KTF655401 LCZ655401:LDB655401 LMV655401:LMX655401 LWR655401:LWT655401 MGN655401:MGP655401 MQJ655401:MQL655401 NAF655401:NAH655401 NKB655401:NKD655401 NTX655401:NTZ655401 ODT655401:ODV655401 ONP655401:ONR655401 OXL655401:OXN655401 PHH655401:PHJ655401 PRD655401:PRF655401 QAZ655401:QBB655401 QKV655401:QKX655401 QUR655401:QUT655401 REN655401:REP655401 ROJ655401:ROL655401 RYF655401:RYH655401 SIB655401:SID655401 SRX655401:SRZ655401 TBT655401:TBV655401 TLP655401:TLR655401 TVL655401:TVN655401 UFH655401:UFJ655401 UPD655401:UPF655401 UYZ655401:UZB655401 VIV655401:VIX655401 VSR655401:VST655401 WCN655401:WCP655401 WMJ655401:WML655401 WWF655401:WWH655401 X720937:Z720937 JT720937:JV720937 TP720937:TR720937 ADL720937:ADN720937 ANH720937:ANJ720937 AXD720937:AXF720937 BGZ720937:BHB720937 BQV720937:BQX720937 CAR720937:CAT720937 CKN720937:CKP720937 CUJ720937:CUL720937 DEF720937:DEH720937 DOB720937:DOD720937 DXX720937:DXZ720937 EHT720937:EHV720937 ERP720937:ERR720937 FBL720937:FBN720937 FLH720937:FLJ720937 FVD720937:FVF720937 GEZ720937:GFB720937 GOV720937:GOX720937 GYR720937:GYT720937 HIN720937:HIP720937 HSJ720937:HSL720937 ICF720937:ICH720937 IMB720937:IMD720937 IVX720937:IVZ720937 JFT720937:JFV720937 JPP720937:JPR720937 JZL720937:JZN720937 KJH720937:KJJ720937 KTD720937:KTF720937 LCZ720937:LDB720937 LMV720937:LMX720937 LWR720937:LWT720937 MGN720937:MGP720937 MQJ720937:MQL720937 NAF720937:NAH720937 NKB720937:NKD720937 NTX720937:NTZ720937 ODT720937:ODV720937 ONP720937:ONR720937 OXL720937:OXN720937 PHH720937:PHJ720937 PRD720937:PRF720937 QAZ720937:QBB720937 QKV720937:QKX720937 QUR720937:QUT720937 REN720937:REP720937 ROJ720937:ROL720937 RYF720937:RYH720937 SIB720937:SID720937 SRX720937:SRZ720937 TBT720937:TBV720937 TLP720937:TLR720937 TVL720937:TVN720937 UFH720937:UFJ720937 UPD720937:UPF720937 UYZ720937:UZB720937 VIV720937:VIX720937 VSR720937:VST720937 WCN720937:WCP720937 WMJ720937:WML720937 WWF720937:WWH720937 X786473:Z786473 JT786473:JV786473 TP786473:TR786473 ADL786473:ADN786473 ANH786473:ANJ786473 AXD786473:AXF786473 BGZ786473:BHB786473 BQV786473:BQX786473 CAR786473:CAT786473 CKN786473:CKP786473 CUJ786473:CUL786473 DEF786473:DEH786473 DOB786473:DOD786473 DXX786473:DXZ786473 EHT786473:EHV786473 ERP786473:ERR786473 FBL786473:FBN786473 FLH786473:FLJ786473 FVD786473:FVF786473 GEZ786473:GFB786473 GOV786473:GOX786473 GYR786473:GYT786473 HIN786473:HIP786473 HSJ786473:HSL786473 ICF786473:ICH786473 IMB786473:IMD786473 IVX786473:IVZ786473 JFT786473:JFV786473 JPP786473:JPR786473 JZL786473:JZN786473 KJH786473:KJJ786473 KTD786473:KTF786473 LCZ786473:LDB786473 LMV786473:LMX786473 LWR786473:LWT786473 MGN786473:MGP786473 MQJ786473:MQL786473 NAF786473:NAH786473 NKB786473:NKD786473 NTX786473:NTZ786473 ODT786473:ODV786473 ONP786473:ONR786473 OXL786473:OXN786473 PHH786473:PHJ786473 PRD786473:PRF786473 QAZ786473:QBB786473 QKV786473:QKX786473 QUR786473:QUT786473 REN786473:REP786473 ROJ786473:ROL786473 RYF786473:RYH786473 SIB786473:SID786473 SRX786473:SRZ786473 TBT786473:TBV786473 TLP786473:TLR786473 TVL786473:TVN786473 UFH786473:UFJ786473 UPD786473:UPF786473 UYZ786473:UZB786473 VIV786473:VIX786473 VSR786473:VST786473 WCN786473:WCP786473 WMJ786473:WML786473 WWF786473:WWH786473 X852009:Z852009 JT852009:JV852009 TP852009:TR852009 ADL852009:ADN852009 ANH852009:ANJ852009 AXD852009:AXF852009 BGZ852009:BHB852009 BQV852009:BQX852009 CAR852009:CAT852009 CKN852009:CKP852009 CUJ852009:CUL852009 DEF852009:DEH852009 DOB852009:DOD852009 DXX852009:DXZ852009 EHT852009:EHV852009 ERP852009:ERR852009 FBL852009:FBN852009 FLH852009:FLJ852009 FVD852009:FVF852009 GEZ852009:GFB852009 GOV852009:GOX852009 GYR852009:GYT852009 HIN852009:HIP852009 HSJ852009:HSL852009 ICF852009:ICH852009 IMB852009:IMD852009 IVX852009:IVZ852009 JFT852009:JFV852009 JPP852009:JPR852009 JZL852009:JZN852009 KJH852009:KJJ852009 KTD852009:KTF852009 LCZ852009:LDB852009 LMV852009:LMX852009 LWR852009:LWT852009 MGN852009:MGP852009 MQJ852009:MQL852009 NAF852009:NAH852009 NKB852009:NKD852009 NTX852009:NTZ852009 ODT852009:ODV852009 ONP852009:ONR852009 OXL852009:OXN852009 PHH852009:PHJ852009 PRD852009:PRF852009 QAZ852009:QBB852009 QKV852009:QKX852009 QUR852009:QUT852009 REN852009:REP852009 ROJ852009:ROL852009 RYF852009:RYH852009 SIB852009:SID852009 SRX852009:SRZ852009 TBT852009:TBV852009 TLP852009:TLR852009 TVL852009:TVN852009 UFH852009:UFJ852009 UPD852009:UPF852009 UYZ852009:UZB852009 VIV852009:VIX852009 VSR852009:VST852009 WCN852009:WCP852009 WMJ852009:WML852009 WWF852009:WWH852009 X917545:Z917545 JT917545:JV917545 TP917545:TR917545 ADL917545:ADN917545 ANH917545:ANJ917545 AXD917545:AXF917545 BGZ917545:BHB917545 BQV917545:BQX917545 CAR917545:CAT917545 CKN917545:CKP917545 CUJ917545:CUL917545 DEF917545:DEH917545 DOB917545:DOD917545 DXX917545:DXZ917545 EHT917545:EHV917545 ERP917545:ERR917545 FBL917545:FBN917545 FLH917545:FLJ917545 FVD917545:FVF917545 GEZ917545:GFB917545 GOV917545:GOX917545 GYR917545:GYT917545 HIN917545:HIP917545 HSJ917545:HSL917545 ICF917545:ICH917545 IMB917545:IMD917545 IVX917545:IVZ917545 JFT917545:JFV917545 JPP917545:JPR917545 JZL917545:JZN917545 KJH917545:KJJ917545 KTD917545:KTF917545 LCZ917545:LDB917545 LMV917545:LMX917545 LWR917545:LWT917545 MGN917545:MGP917545 MQJ917545:MQL917545 NAF917545:NAH917545 NKB917545:NKD917545 NTX917545:NTZ917545 ODT917545:ODV917545 ONP917545:ONR917545 OXL917545:OXN917545 PHH917545:PHJ917545 PRD917545:PRF917545 QAZ917545:QBB917545 QKV917545:QKX917545 QUR917545:QUT917545 REN917545:REP917545 ROJ917545:ROL917545 RYF917545:RYH917545 SIB917545:SID917545 SRX917545:SRZ917545 TBT917545:TBV917545 TLP917545:TLR917545 TVL917545:TVN917545 UFH917545:UFJ917545 UPD917545:UPF917545 UYZ917545:UZB917545 VIV917545:VIX917545 VSR917545:VST917545 WCN917545:WCP917545 WMJ917545:WML917545 WWF917545:WWH917545 X983081:Z983081 JT983081:JV983081 TP983081:TR983081 ADL983081:ADN983081 ANH983081:ANJ983081 AXD983081:AXF983081 BGZ983081:BHB983081 BQV983081:BQX983081 CAR983081:CAT983081 CKN983081:CKP983081 CUJ983081:CUL983081 DEF983081:DEH983081 DOB983081:DOD983081 DXX983081:DXZ983081 EHT983081:EHV983081 ERP983081:ERR983081 FBL983081:FBN983081 FLH983081:FLJ983081 FVD983081:FVF983081 GEZ983081:GFB983081 GOV983081:GOX983081 GYR983081:GYT983081 HIN983081:HIP983081 HSJ983081:HSL983081 ICF983081:ICH983081 IMB983081:IMD983081 IVX983081:IVZ983081 JFT983081:JFV983081 JPP983081:JPR983081 JZL983081:JZN983081 KJH983081:KJJ983081 KTD983081:KTF983081 LCZ983081:LDB983081 LMV983081:LMX983081 LWR983081:LWT983081 MGN983081:MGP983081 MQJ983081:MQL983081 NAF983081:NAH983081 NKB983081:NKD983081 NTX983081:NTZ983081 ODT983081:ODV983081 ONP983081:ONR983081 OXL983081:OXN983081 PHH983081:PHJ983081 PRD983081:PRF983081 QAZ983081:QBB983081 QKV983081:QKX983081 QUR983081:QUT983081 REN983081:REP983081 ROJ983081:ROL983081 RYF983081:RYH983081 SIB983081:SID983081 SRX983081:SRZ983081 TBT983081:TBV983081 TLP983081:TLR983081 TVL983081:TVN983081 UFH983081:UFJ983081 UPD983081:UPF983081 UYZ983081:UZB983081 VIV983081:VIX983081 VSR983081:VST983081 WCN983081:WCP983081 WMJ983081:WML983081 WWF983081:WWH983081" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>